<commit_message>
added state purchases add-ons
</commit_message>
<xml_diff>
--- a/documentation/COVID-19 Changes/September/LSFIM_KY_v6_round2.xlsx
+++ b/documentation/COVID-19 Changes/September/LSFIM_KY_v6_round2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyilla\Documents\Git\Fiscal-Impact-Measure\documentation\COVID-19 Changes\September\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD61C30A-B8CA-4288-855F-24D480D9047E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D7F294-2488-4E5A-982B-B24980046BE9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="351">
   <si>
     <t>Corporate Taxes</t>
   </si>
@@ -1973,6 +1973,9 @@
   <si>
     <t>Unemployment $300 (round 2)</t>
   </si>
+  <si>
+    <t>add_state_purchases</t>
+  </si>
 </sst>
 </file>
 
@@ -1990,7 +1993,7 @@
     <numFmt numFmtId="171" formatCode="0.000%"/>
     <numFmt numFmtId="172" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2221,12 +2224,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="18">
@@ -3241,6 +3238,32 @@
       <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="17" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="17" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3307,21 +3330,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3343,44 +3351,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="17" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="17" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3872,11 +3869,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412AAB1A-8B83-4A8D-A21D-8EE870D0279B}">
   <dimension ref="A1:AP105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="O60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomRight" activeCell="L68" sqref="L68:R68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3896,10 +3893,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="300" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="286"/>
+      <c r="B1" s="300"/>
       <c r="C1" s="280"/>
       <c r="D1" s="280"/>
       <c r="E1" s="35"/>
@@ -3909,75 +3906,75 @@
       <c r="AB1" s="179" t="s">
         <v>249</v>
       </c>
-      <c r="AC1" s="288" t="s">
+      <c r="AC1" s="302" t="s">
         <v>247</v>
       </c>
-      <c r="AD1" s="288"/>
-      <c r="AE1" s="288"/>
+      <c r="AD1" s="302"/>
+      <c r="AE1" s="302"/>
       <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="289" t="s">
+      <c r="AH1" s="303" t="s">
         <v>281</v>
       </c>
-      <c r="AI1" s="289"/>
-      <c r="AJ1" s="289"/>
-      <c r="AK1" s="289"/>
-      <c r="AL1" s="287" t="s">
+      <c r="AI1" s="303"/>
+      <c r="AJ1" s="303"/>
+      <c r="AK1" s="303"/>
+      <c r="AL1" s="301" t="s">
         <v>279</v>
       </c>
-      <c r="AM1" s="287"/>
-      <c r="AN1" s="287"/>
-      <c r="AO1" s="287"/>
+      <c r="AM1" s="301"/>
+      <c r="AN1" s="301"/>
+      <c r="AO1" s="301"/>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.35">
-      <c r="F2" s="285" t="s">
+      <c r="F2" s="299" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="285"/>
-      <c r="H2" s="285"/>
-      <c r="I2" s="285"/>
-      <c r="J2" s="285" t="s">
+      <c r="G2" s="299"/>
+      <c r="H2" s="299"/>
+      <c r="I2" s="299"/>
+      <c r="J2" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="285"/>
-      <c r="L2" s="285"/>
-      <c r="M2" s="285"/>
-      <c r="N2" s="285" t="s">
+      <c r="K2" s="299"/>
+      <c r="L2" s="299"/>
+      <c r="M2" s="299"/>
+      <c r="N2" s="299" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="285"/>
-      <c r="P2" s="285"/>
-      <c r="Q2" s="285"/>
-      <c r="R2" s="285" t="s">
+      <c r="O2" s="299"/>
+      <c r="P2" s="299"/>
+      <c r="Q2" s="299"/>
+      <c r="R2" s="299" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="285"/>
-      <c r="T2" s="285"/>
-      <c r="U2" s="285"/>
-      <c r="V2" s="285" t="s">
+      <c r="S2" s="299"/>
+      <c r="T2" s="299"/>
+      <c r="U2" s="299"/>
+      <c r="V2" s="299" t="s">
         <v>268</v>
       </c>
-      <c r="W2" s="285"/>
-      <c r="X2" s="285"/>
-      <c r="Y2" s="285"/>
+      <c r="W2" s="299"/>
+      <c r="X2" s="299"/>
+      <c r="Y2" s="299"/>
       <c r="Z2" s="229"/>
       <c r="AA2" s="229"/>
       <c r="AB2" s="156"/>
-      <c r="AC2" s="285" t="s">
+      <c r="AC2" s="299" t="s">
         <v>102</v>
       </c>
-      <c r="AD2" s="285"/>
-      <c r="AE2" s="285"/>
+      <c r="AD2" s="299"/>
+      <c r="AE2" s="299"/>
       <c r="AF2" s="156"/>
       <c r="AG2" s="156" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" s="285" t="s">
+      <c r="AH2" s="299" t="s">
         <v>102</v>
       </c>
-      <c r="AI2" s="285"/>
-      <c r="AJ2" s="285"/>
+      <c r="AI2" s="299"/>
+      <c r="AJ2" s="299"/>
       <c r="AK2" s="230"/>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.35">
@@ -4082,10 +4079,10 @@
       </c>
     </row>
     <row r="4" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="284" t="s">
+      <c r="A4" s="298" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="284"/>
+      <c r="B4" s="298"/>
       <c r="C4" s="280"/>
       <c r="D4" s="280"/>
       <c r="F4" s="199"/>
@@ -6021,38 +6018,38 @@
       <c r="AK32" s="3"/>
       <c r="AL32" s="184"/>
     </row>
-    <row r="33" spans="1:40" s="327" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="336" t="s">
+    <row r="33" spans="1:40" s="287" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="296" t="s">
         <v>343</v>
       </c>
-      <c r="F33" s="328"/>
-      <c r="G33" s="328"/>
-      <c r="H33" s="328"/>
-      <c r="I33" s="328"/>
-      <c r="J33" s="328"/>
-      <c r="K33" s="328"/>
-      <c r="L33" s="328"/>
-      <c r="M33" s="329"/>
-      <c r="N33" s="330"/>
-      <c r="O33" s="330">
+      <c r="F33" s="288"/>
+      <c r="G33" s="288"/>
+      <c r="H33" s="288"/>
+      <c r="I33" s="288"/>
+      <c r="J33" s="288"/>
+      <c r="K33" s="288"/>
+      <c r="L33" s="288"/>
+      <c r="M33" s="289"/>
+      <c r="N33" s="290"/>
+      <c r="O33" s="290">
         <f>SUM(L32:P32)/2</f>
         <v>562800</v>
       </c>
-      <c r="P33" s="330"/>
-      <c r="Q33" s="330"/>
-      <c r="R33" s="330"/>
-      <c r="S33" s="330"/>
-      <c r="T33" s="330"/>
-      <c r="U33" s="330"/>
-      <c r="AC33" s="332"/>
-      <c r="AD33" s="332"/>
-      <c r="AE33" s="332"/>
-      <c r="AF33" s="331"/>
-      <c r="AH33" s="331"/>
-      <c r="AI33" s="331"/>
-      <c r="AJ33" s="331"/>
-      <c r="AK33" s="331"/>
-      <c r="AL33" s="333"/>
+      <c r="P33" s="290"/>
+      <c r="Q33" s="290"/>
+      <c r="R33" s="290"/>
+      <c r="S33" s="290"/>
+      <c r="T33" s="290"/>
+      <c r="U33" s="290"/>
+      <c r="AC33" s="292"/>
+      <c r="AD33" s="292"/>
+      <c r="AE33" s="292"/>
+      <c r="AF33" s="291"/>
+      <c r="AH33" s="291"/>
+      <c r="AI33" s="291"/>
+      <c r="AJ33" s="291"/>
+      <c r="AK33" s="291"/>
+      <c r="AL33" s="293"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" s="86" t="s">
@@ -6232,7 +6229,7 @@
         <v>108000</v>
       </c>
       <c r="Q36" s="87">
-        <f t="shared" ref="O36:Q36" si="26">Q37+Q38+Q39</f>
+        <f t="shared" ref="Q36" si="26">Q37+Q38+Q39</f>
         <v>0</v>
       </c>
       <c r="R36" s="87">
@@ -6381,44 +6378,44 @@
       <c r="AK38" s="3"/>
       <c r="AL38" s="184"/>
     </row>
-    <row r="39" spans="1:40" s="327" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="326" t="s">
+    <row r="39" spans="1:40" s="287" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="286" t="s">
         <v>349</v>
       </c>
-      <c r="F39" s="328"/>
-      <c r="G39" s="328"/>
-      <c r="H39" s="328"/>
-      <c r="I39" s="328"/>
-      <c r="J39" s="328"/>
-      <c r="K39" s="328"/>
-      <c r="L39" s="328"/>
-      <c r="M39" s="329"/>
-      <c r="N39" s="330"/>
-      <c r="O39" s="330">
+      <c r="F39" s="288"/>
+      <c r="G39" s="288"/>
+      <c r="H39" s="288"/>
+      <c r="I39" s="288"/>
+      <c r="J39" s="288"/>
+      <c r="K39" s="288"/>
+      <c r="L39" s="288"/>
+      <c r="M39" s="289"/>
+      <c r="N39" s="290"/>
+      <c r="O39" s="290">
         <v>720000</v>
       </c>
-      <c r="P39" s="330"/>
-      <c r="Q39" s="330"/>
-      <c r="R39" s="330"/>
-      <c r="S39" s="330"/>
-      <c r="T39" s="330"/>
-      <c r="U39" s="330"/>
-      <c r="V39" s="331"/>
-      <c r="W39" s="331"/>
-      <c r="X39" s="331"/>
-      <c r="Y39" s="331"/>
-      <c r="Z39" s="331"/>
-      <c r="AA39" s="331"/>
-      <c r="AB39" s="331"/>
-      <c r="AC39" s="332"/>
-      <c r="AD39" s="332"/>
-      <c r="AE39" s="332"/>
-      <c r="AF39" s="331"/>
-      <c r="AH39" s="331"/>
-      <c r="AI39" s="331"/>
-      <c r="AJ39" s="331"/>
-      <c r="AK39" s="331"/>
-      <c r="AL39" s="333"/>
+      <c r="P39" s="290"/>
+      <c r="Q39" s="290"/>
+      <c r="R39" s="290"/>
+      <c r="S39" s="290"/>
+      <c r="T39" s="290"/>
+      <c r="U39" s="290"/>
+      <c r="V39" s="291"/>
+      <c r="W39" s="291"/>
+      <c r="X39" s="291"/>
+      <c r="Y39" s="291"/>
+      <c r="Z39" s="291"/>
+      <c r="AA39" s="291"/>
+      <c r="AB39" s="291"/>
+      <c r="AC39" s="292"/>
+      <c r="AD39" s="292"/>
+      <c r="AE39" s="292"/>
+      <c r="AF39" s="291"/>
+      <c r="AH39" s="291"/>
+      <c r="AI39" s="291"/>
+      <c r="AJ39" s="291"/>
+      <c r="AK39" s="291"/>
+      <c r="AL39" s="293"/>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="117" t="s">
@@ -7146,7 +7143,7 @@
       <c r="AL50" s="243"/>
     </row>
     <row r="51" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="324" t="s">
+      <c r="A51" s="284" t="s">
         <v>338</v>
       </c>
       <c r="C51" t="s">
@@ -7270,8 +7267,8 @@
       <c r="AF52" s="44"/>
       <c r="AL52" s="243"/>
     </row>
-    <row r="53" spans="1:38" s="187" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="325" t="s">
+    <row r="53" spans="1:38" s="187" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="285" t="s">
         <v>284</v>
       </c>
       <c r="B53" s="187" t="s">
@@ -7315,8 +7312,8 @@
       <c r="AF53" s="189"/>
       <c r="AL53" s="244"/>
     </row>
-    <row r="54" spans="1:38" s="187" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="325" t="s">
+    <row r="54" spans="1:38" s="187" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="285" t="s">
         <v>285</v>
       </c>
       <c r="B54" s="187" t="s">
@@ -7360,8 +7357,8 @@
       <c r="AF54" s="189"/>
       <c r="AL54" s="244"/>
     </row>
-    <row r="55" spans="1:38" s="187" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="325" t="s">
+    <row r="55" spans="1:38" s="187" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="285" t="s">
         <v>286</v>
       </c>
       <c r="B55" s="187" t="s">
@@ -7440,44 +7437,44 @@
       <c r="AF56" s="189"/>
       <c r="AL56" s="244"/>
     </row>
-    <row r="57" spans="1:38" s="327" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="326" t="s">
+    <row r="57" spans="1:38" s="287" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="286" t="s">
         <v>339</v>
       </c>
-      <c r="F57" s="329"/>
-      <c r="G57" s="329"/>
-      <c r="H57" s="329"/>
-      <c r="I57" s="328"/>
-      <c r="J57" s="328"/>
-      <c r="K57" s="328"/>
-      <c r="L57" s="328"/>
-      <c r="M57" s="329"/>
-      <c r="N57" s="334"/>
-      <c r="O57" s="334">
+      <c r="F57" s="289"/>
+      <c r="G57" s="289"/>
+      <c r="H57" s="289"/>
+      <c r="I57" s="288"/>
+      <c r="J57" s="288"/>
+      <c r="K57" s="288"/>
+      <c r="L57" s="288"/>
+      <c r="M57" s="289"/>
+      <c r="N57" s="294"/>
+      <c r="O57" s="294">
         <v>400000</v>
       </c>
-      <c r="P57" s="334">
+      <c r="P57" s="294">
         <v>400000</v>
       </c>
-      <c r="Q57" s="334">
+      <c r="Q57" s="294">
         <v>400000</v>
       </c>
-      <c r="R57" s="334"/>
-      <c r="S57" s="334"/>
-      <c r="T57" s="334"/>
-      <c r="U57" s="334"/>
-      <c r="V57" s="334"/>
-      <c r="W57" s="331"/>
-      <c r="X57" s="331"/>
-      <c r="Y57" s="331"/>
-      <c r="Z57" s="331"/>
-      <c r="AA57" s="331"/>
-      <c r="AB57" s="331"/>
-      <c r="AC57" s="331"/>
-      <c r="AD57" s="331"/>
-      <c r="AE57" s="331"/>
-      <c r="AF57" s="331"/>
-      <c r="AL57" s="335"/>
+      <c r="R57" s="294"/>
+      <c r="S57" s="294"/>
+      <c r="T57" s="294"/>
+      <c r="U57" s="294"/>
+      <c r="V57" s="294"/>
+      <c r="W57" s="291"/>
+      <c r="X57" s="291"/>
+      <c r="Y57" s="291"/>
+      <c r="Z57" s="291"/>
+      <c r="AA57" s="291"/>
+      <c r="AB57" s="291"/>
+      <c r="AC57" s="291"/>
+      <c r="AD57" s="291"/>
+      <c r="AE57" s="291"/>
+      <c r="AF57" s="291"/>
+      <c r="AL57" s="295"/>
     </row>
     <row r="58" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="134"/>
@@ -7802,7 +7799,7 @@
         <v>50000</v>
       </c>
       <c r="V63" s="116">
-        <f t="shared" ref="O63:W63" si="43">SUM(V65:V71)</f>
+        <f t="shared" ref="V63:W63" si="43">SUM(V65:V71)</f>
         <v>50000</v>
       </c>
       <c r="W63" s="116">
@@ -8017,9 +8014,18 @@
       <c r="L68" s="204"/>
       <c r="M68" s="199"/>
       <c r="N68" s="116"/>
-      <c r="O68" s="116"/>
-      <c r="P68" s="116"/>
-      <c r="Q68" s="116"/>
+      <c r="O68" s="116">
+        <f>SUM(O69:O71)</f>
+        <v>190660</v>
+      </c>
+      <c r="P68" s="116">
+        <f t="shared" ref="P68:Q68" si="44">SUM(P69:P71)</f>
+        <v>190660</v>
+      </c>
+      <c r="Q68" s="116">
+        <f t="shared" si="44"/>
+        <v>190660</v>
+      </c>
       <c r="R68" s="116"/>
       <c r="S68" s="44"/>
       <c r="T68" s="44"/>
@@ -8037,122 +8043,122 @@
       <c r="AF68" s="44"/>
       <c r="AL68" s="243"/>
     </row>
-    <row r="69" spans="1:38" s="327" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="337" t="s">
+    <row r="69" spans="1:38" s="287" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="297" t="s">
         <v>346</v>
       </c>
-      <c r="F69" s="329"/>
-      <c r="G69" s="329"/>
-      <c r="H69" s="329"/>
-      <c r="I69" s="328"/>
-      <c r="J69" s="328"/>
-      <c r="K69" s="328"/>
-      <c r="L69" s="328"/>
-      <c r="M69" s="329"/>
-      <c r="N69" s="334"/>
-      <c r="O69" s="334">
+      <c r="F69" s="289"/>
+      <c r="G69" s="289"/>
+      <c r="H69" s="289"/>
+      <c r="I69" s="288"/>
+      <c r="J69" s="288"/>
+      <c r="K69" s="288"/>
+      <c r="L69" s="288"/>
+      <c r="M69" s="289"/>
+      <c r="N69" s="294"/>
+      <c r="O69" s="294">
         <v>60000</v>
       </c>
-      <c r="P69" s="334">
+      <c r="P69" s="294">
         <v>60000</v>
       </c>
-      <c r="Q69" s="334">
+      <c r="Q69" s="294">
         <v>60000</v>
       </c>
-      <c r="R69" s="334"/>
-      <c r="S69" s="331"/>
-      <c r="T69" s="331"/>
-      <c r="U69" s="331"/>
-      <c r="V69" s="331"/>
-      <c r="W69" s="331"/>
-      <c r="X69" s="331"/>
-      <c r="Y69" s="331"/>
-      <c r="Z69" s="331"/>
-      <c r="AA69" s="331"/>
-      <c r="AB69" s="331"/>
-      <c r="AC69" s="331"/>
-      <c r="AD69" s="331"/>
-      <c r="AE69" s="331"/>
-      <c r="AF69" s="331"/>
-      <c r="AL69" s="335"/>
-    </row>
-    <row r="70" spans="1:38" s="327" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="337" t="s">
+      <c r="R69" s="294"/>
+      <c r="S69" s="291"/>
+      <c r="T69" s="291"/>
+      <c r="U69" s="291"/>
+      <c r="V69" s="291"/>
+      <c r="W69" s="291"/>
+      <c r="X69" s="291"/>
+      <c r="Y69" s="291"/>
+      <c r="Z69" s="291"/>
+      <c r="AA69" s="291"/>
+      <c r="AB69" s="291"/>
+      <c r="AC69" s="291"/>
+      <c r="AD69" s="291"/>
+      <c r="AE69" s="291"/>
+      <c r="AF69" s="291"/>
+      <c r="AL69" s="295"/>
+    </row>
+    <row r="70" spans="1:38" s="287" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="297" t="s">
         <v>347</v>
       </c>
-      <c r="F70" s="329"/>
-      <c r="G70" s="329"/>
-      <c r="H70" s="329"/>
-      <c r="I70" s="328"/>
-      <c r="J70" s="328"/>
-      <c r="K70" s="328"/>
-      <c r="L70" s="328"/>
-      <c r="M70" s="329"/>
-      <c r="N70" s="334"/>
-      <c r="O70" s="334">
+      <c r="F70" s="289"/>
+      <c r="G70" s="289"/>
+      <c r="H70" s="289"/>
+      <c r="I70" s="288"/>
+      <c r="J70" s="288"/>
+      <c r="K70" s="288"/>
+      <c r="L70" s="288"/>
+      <c r="M70" s="289"/>
+      <c r="N70" s="294"/>
+      <c r="O70" s="294">
         <v>109330</v>
       </c>
-      <c r="P70" s="334">
+      <c r="P70" s="294">
         <v>109330</v>
       </c>
-      <c r="Q70" s="334">
+      <c r="Q70" s="294">
         <v>109330</v>
       </c>
-      <c r="R70" s="334"/>
-      <c r="S70" s="331"/>
-      <c r="T70" s="331"/>
-      <c r="U70" s="331"/>
-      <c r="V70" s="331"/>
-      <c r="W70" s="331"/>
-      <c r="X70" s="331"/>
-      <c r="Y70" s="331"/>
-      <c r="Z70" s="331"/>
-      <c r="AA70" s="331"/>
-      <c r="AB70" s="331"/>
-      <c r="AC70" s="331"/>
-      <c r="AD70" s="331"/>
-      <c r="AE70" s="331"/>
-      <c r="AF70" s="331"/>
-      <c r="AL70" s="335"/>
-    </row>
-    <row r="71" spans="1:38" s="327" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="337" t="s">
+      <c r="R70" s="294"/>
+      <c r="S70" s="291"/>
+      <c r="T70" s="291"/>
+      <c r="U70" s="291"/>
+      <c r="V70" s="291"/>
+      <c r="W70" s="291"/>
+      <c r="X70" s="291"/>
+      <c r="Y70" s="291"/>
+      <c r="Z70" s="291"/>
+      <c r="AA70" s="291"/>
+      <c r="AB70" s="291"/>
+      <c r="AC70" s="291"/>
+      <c r="AD70" s="291"/>
+      <c r="AE70" s="291"/>
+      <c r="AF70" s="291"/>
+      <c r="AL70" s="295"/>
+    </row>
+    <row r="71" spans="1:38" s="287" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="297" t="s">
         <v>348</v>
       </c>
-      <c r="F71" s="329"/>
-      <c r="G71" s="329"/>
-      <c r="H71" s="329"/>
-      <c r="I71" s="328"/>
-      <c r="J71" s="328"/>
-      <c r="K71" s="328"/>
-      <c r="L71" s="328"/>
-      <c r="M71" s="329"/>
-      <c r="N71" s="334"/>
-      <c r="O71" s="334">
+      <c r="F71" s="289"/>
+      <c r="G71" s="289"/>
+      <c r="H71" s="289"/>
+      <c r="I71" s="288"/>
+      <c r="J71" s="288"/>
+      <c r="K71" s="288"/>
+      <c r="L71" s="288"/>
+      <c r="M71" s="289"/>
+      <c r="N71" s="294"/>
+      <c r="O71" s="294">
         <v>21330</v>
       </c>
-      <c r="P71" s="334">
+      <c r="P71" s="294">
         <v>21330</v>
       </c>
-      <c r="Q71" s="334">
+      <c r="Q71" s="294">
         <v>21330</v>
       </c>
-      <c r="R71" s="334"/>
-      <c r="S71" s="331"/>
-      <c r="T71" s="331"/>
-      <c r="U71" s="331"/>
-      <c r="V71" s="331"/>
-      <c r="W71" s="331"/>
-      <c r="X71" s="331"/>
-      <c r="Y71" s="331"/>
-      <c r="Z71" s="331"/>
-      <c r="AA71" s="331"/>
-      <c r="AB71" s="331"/>
-      <c r="AC71" s="331"/>
-      <c r="AD71" s="331"/>
-      <c r="AE71" s="331"/>
-      <c r="AF71" s="331"/>
-      <c r="AL71" s="335"/>
+      <c r="R71" s="294"/>
+      <c r="S71" s="291"/>
+      <c r="T71" s="291"/>
+      <c r="U71" s="291"/>
+      <c r="V71" s="291"/>
+      <c r="W71" s="291"/>
+      <c r="X71" s="291"/>
+      <c r="Y71" s="291"/>
+      <c r="Z71" s="291"/>
+      <c r="AA71" s="291"/>
+      <c r="AB71" s="291"/>
+      <c r="AC71" s="291"/>
+      <c r="AD71" s="291"/>
+      <c r="AE71" s="291"/>
+      <c r="AF71" s="291"/>
+      <c r="AL71" s="295"/>
     </row>
     <row r="72" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="145" t="s">
@@ -8174,47 +8180,47 @@
         <v>279250</v>
       </c>
       <c r="M72" s="199">
-        <f t="shared" ref="M72:W72" si="44">M61+M63</f>
+        <f t="shared" ref="M72:W72" si="45">M61+M63</f>
         <v>286950.6143673578</v>
       </c>
       <c r="N72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>298372.88477706735</v>
       </c>
       <c r="O72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>472800.99544764287</v>
       </c>
       <c r="P72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>445682.43392207247</v>
       </c>
       <c r="Q72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>446714.97613497748</v>
       </c>
       <c r="R72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>251544.37969325102</v>
       </c>
       <c r="S72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>247240.80684971521</v>
       </c>
       <c r="T72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>248958.57178194768</v>
       </c>
       <c r="U72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>250866.80125051294</v>
       </c>
       <c r="V72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>252622.47677399646</v>
       </c>
       <c r="W72" s="144">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>254572.45802602731</v>
       </c>
       <c r="X72" s="44"/>
@@ -8416,43 +8422,43 @@
         <v>7.4875799399045651E-3</v>
       </c>
       <c r="O76" s="188">
-        <f t="shared" ref="O76:V76" si="45">O75/N75-1</f>
+        <f t="shared" ref="O76:V76" si="46">O75/N75-1</f>
         <v>4.0136860113193507E-3</v>
       </c>
       <c r="P76" s="188">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>4.5874565829953085E-3</v>
       </c>
       <c r="Q76" s="188">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>5.3493378563544969E-3</v>
       </c>
       <c r="R76" s="188">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>7.6751629251576858E-3</v>
       </c>
       <c r="S76" s="188">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>8.675407388979206E-3</v>
       </c>
       <c r="T76" s="188">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>8.7089733593581631E-3</v>
       </c>
       <c r="U76" s="188">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>9.5910894990571816E-3</v>
       </c>
       <c r="V76" s="188">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>8.7404962520107876E-3</v>
       </c>
       <c r="W76" s="188">
-        <f t="shared" ref="W76" si="46">W75/V75-1</f>
+        <f t="shared" ref="W76" si="47">W75/V75-1</f>
         <v>9.6237163965073869E-3</v>
       </c>
       <c r="X76" s="188">
-        <f t="shared" ref="X76" si="47">X75/W75-1</f>
+        <f t="shared" ref="X76" si="48">X75/W75-1</f>
         <v>8.7455736250123817E-3</v>
       </c>
       <c r="Y76" s="188">
@@ -8460,7 +8466,7 @@
         <v>9.6201658414407643E-3</v>
       </c>
       <c r="Z76" s="188">
-        <f t="shared" ref="Z76" si="48">Z75/Y75-1</f>
+        <f t="shared" ref="Z76" si="49">Z75/Y75-1</f>
         <v>3.1021950970274714E-2</v>
       </c>
       <c r="AA76" s="188"/>
@@ -8510,27 +8516,27 @@
         <v>486072</v>
       </c>
       <c r="N77" s="116">
-        <f t="shared" ref="N77:S77" si="49">N84*0.74</f>
+        <f t="shared" ref="N77:S77" si="50">N84*0.74</f>
         <v>520762.48586017155</v>
       </c>
       <c r="O77" s="116">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>530153.75073570432</v>
       </c>
       <c r="P77" s="116">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>535444.10571143136</v>
       </c>
       <c r="Q77" s="116">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>535444.10571143136</v>
       </c>
       <c r="R77" s="116">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>535444.10571143136</v>
       </c>
       <c r="S77" s="116">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>535444.10571143136</v>
       </c>
       <c r="T77" s="116">
@@ -8591,35 +8597,35 @@
       <c r="B78" s="141"/>
       <c r="E78" s="141"/>
       <c r="F78" s="203">
-        <f>F44+F41+F32+F36</f>
+        <f t="shared" ref="F78:M78" si="51">F44+F41+F32+F36</f>
         <v>1440187</v>
       </c>
       <c r="G78" s="203">
-        <f>G44+G41+G32+G36</f>
+        <f t="shared" si="51"/>
         <v>1503410</v>
       </c>
       <c r="H78" s="203">
-        <f>H44+H41+H32+H36</f>
+        <f t="shared" si="51"/>
         <v>1508652</v>
       </c>
       <c r="I78" s="203">
-        <f>I44+I41+I32+I36</f>
+        <f t="shared" si="51"/>
         <v>1513957</v>
       </c>
       <c r="J78" s="203">
-        <f>J44+J41+J32+J36</f>
+        <f t="shared" si="51"/>
         <v>1521941</v>
       </c>
       <c r="K78" s="203">
-        <f>K44+K41+K32+K36</f>
+        <f t="shared" si="51"/>
         <v>1574462</v>
       </c>
       <c r="L78" s="203">
-        <f>L44+L41+L32+L36</f>
+        <f t="shared" si="51"/>
         <v>3713565.333333333</v>
       </c>
       <c r="M78" s="199">
-        <f>M44+M41+M32+M36</f>
+        <f t="shared" si="51"/>
         <v>2508714</v>
       </c>
       <c r="N78" s="142">
@@ -8631,31 +8637,31 @@
         <v>3170742.7957109897</v>
       </c>
       <c r="P78" s="142">
-        <f t="shared" ref="P78:V78" si="50">P44+P41+P32+P36+P33</f>
+        <f t="shared" ref="P78:V78" si="52">P44+P41+P32+P36+P33</f>
         <v>1799230.9611612814</v>
       </c>
       <c r="Q78" s="142">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1662989.228952572</v>
       </c>
       <c r="R78" s="142">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1659289.0673868605</v>
       </c>
       <c r="S78" s="142">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1668953.4033976633</v>
       </c>
       <c r="T78" s="142">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1693987.704448628</v>
       </c>
       <c r="U78" s="142">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1719397.5200153573</v>
       </c>
       <c r="V78" s="142">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1736591.4952155109</v>
       </c>
       <c r="AL78" s="243"/>
@@ -8673,47 +8679,47 @@
       <c r="J79" s="199"/>
       <c r="K79" s="199"/>
       <c r="L79" s="205">
-        <f>L77+L31</f>
+        <f t="shared" ref="L79:V79" si="53">L77+L31</f>
         <v>1336698</v>
       </c>
       <c r="M79" s="199">
-        <f>M77+M31</f>
+        <f t="shared" si="53"/>
         <v>1328805</v>
       </c>
       <c r="N79" s="143">
-        <f>N77+N31</f>
+        <f t="shared" si="53"/>
         <v>1373815.6728590003</v>
       </c>
       <c r="O79" s="143">
-        <f>O77+O31</f>
+        <f t="shared" si="53"/>
         <v>1393653.5067068823</v>
       </c>
       <c r="P79" s="143">
-        <f>P77+P31</f>
+        <f t="shared" si="53"/>
         <v>1409518.3603139264</v>
       </c>
       <c r="Q79" s="143">
-        <f>Q77+Q31</f>
+        <f t="shared" si="53"/>
         <v>1420222.3552427585</v>
       </c>
       <c r="R79" s="143">
-        <f>R77+R31</f>
+        <f t="shared" si="53"/>
         <v>1449154.204832383</v>
       </c>
       <c r="S79" s="143">
-        <f>S77+S31</f>
+        <f t="shared" si="53"/>
         <v>1479032.1128509077</v>
       </c>
       <c r="T79" s="143">
-        <f>T77+T31</f>
+        <f t="shared" si="53"/>
         <v>1466472.6280325653</v>
       </c>
       <c r="U79" s="143">
-        <f>U77+U31</f>
+        <f t="shared" si="53"/>
         <v>1498336.4715432189</v>
       </c>
       <c r="V79" s="143">
-        <f>V77+V31</f>
+        <f t="shared" si="53"/>
         <v>1508477.1168994233</v>
       </c>
       <c r="AL79" s="243"/>
@@ -8766,39 +8772,39 @@
         <v>835999</v>
       </c>
       <c r="N81" s="133">
-        <f t="shared" ref="N81:U81" si="51">N82+N84</f>
+        <f t="shared" ref="N81:U81" si="54">N82+N84</f>
         <v>846655.9390002318</v>
       </c>
       <c r="O81" s="133">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>859704.14460568153</v>
       </c>
       <c r="P81" s="133">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>867211.47334407107</v>
       </c>
       <c r="Q81" s="133">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>867929.66513166018</v>
       </c>
       <c r="R81" s="133">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>869012.33925145073</v>
       </c>
       <c r="S81" s="133">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>870466.73148570256</v>
       </c>
       <c r="T81" s="133">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>872014.07451017783</v>
       </c>
       <c r="U81" s="133">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>873408.51802630571</v>
       </c>
       <c r="V81" s="133">
-        <f t="shared" ref="V81" si="52">V82+V84</f>
+        <f t="shared" ref="V81" si="55">V82+V84</f>
         <v>874637.8300734181</v>
       </c>
       <c r="AL81" s="243"/>
@@ -8808,27 +8814,27 @@
         <v>231</v>
       </c>
       <c r="F82" s="205">
-        <f t="shared" ref="F82:K82" si="53">F81-F84</f>
+        <f t="shared" ref="F82:K82" si="56">F81-F84</f>
         <v>139025</v>
       </c>
       <c r="G82" s="205">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>139342</v>
       </c>
       <c r="H82" s="205">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>140228</v>
       </c>
       <c r="I82" s="205">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>141105</v>
       </c>
       <c r="J82" s="205">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>141335</v>
       </c>
       <c r="K82" s="205">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>142991</v>
       </c>
       <c r="L82" s="205">
@@ -8844,35 +8850,35 @@
         <v>142922.84999999998</v>
       </c>
       <c r="O82" s="133">
-        <f t="shared" ref="O82:V82" si="54">N82*(1+O93)</f>
+        <f t="shared" ref="O82:V82" si="57">N82*(1+O93)</f>
         <v>143280.15712499997</v>
       </c>
       <c r="P82" s="133">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>143638.35751781246</v>
       </c>
       <c r="Q82" s="133">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>144356.54930540151</v>
       </c>
       <c r="R82" s="133">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>145439.22342519203</v>
       </c>
       <c r="S82" s="133">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>146893.61565944395</v>
       </c>
       <c r="T82" s="133">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>148440.9586839191</v>
       </c>
       <c r="U82" s="133">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>149835.40220004701</v>
       </c>
       <c r="V82" s="133">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>151064.71424715937</v>
       </c>
       <c r="AL82" s="243"/>
@@ -8941,23 +8947,23 @@
         <v>723573.11582625867</v>
       </c>
       <c r="R84" s="135">
-        <f t="shared" ref="R84:V84" si="55">Q84*(1+R85)</f>
+        <f t="shared" ref="R84:V84" si="58">Q84*(1+R85)</f>
         <v>723573.11582625867</v>
       </c>
       <c r="S84" s="135">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>723573.11582625867</v>
       </c>
       <c r="T84" s="135">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>723573.11582625867</v>
       </c>
       <c r="U84" s="135">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>723573.11582625867</v>
       </c>
       <c r="V84" s="135">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>723573.11582625867</v>
       </c>
       <c r="AC84" s="45">
@@ -9033,23 +9039,23 @@
         <v>0.66058231423538405</v>
       </c>
       <c r="G86" s="210">
-        <f t="shared" ref="G86:I86" si="56">G77/G84</f>
+        <f t="shared" ref="G86:I86" si="59">G77/G84</f>
         <v>0.6749214177505789</v>
       </c>
       <c r="H86" s="210">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.68242012696430432</v>
       </c>
       <c r="I86" s="210">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>0.6730637268687778</v>
       </c>
       <c r="J86" s="210">
-        <f t="shared" ref="J86" si="57">J77/J84</f>
+        <f t="shared" ref="J86" si="60">J77/J84</f>
         <v>0.66395699382859508</v>
       </c>
       <c r="K86" s="210">
-        <f t="shared" ref="K86" si="58">K77/K84</f>
+        <f t="shared" ref="K86" si="61">K77/K84</f>
         <v>0.67846773573296415</v>
       </c>
       <c r="L86" s="211"/>
@@ -9103,35 +9109,35 @@
         <v>2031.6535672371635</v>
       </c>
       <c r="O87" s="35">
-        <f t="shared" ref="O87:V87" si="59">N87*(1+O89)</f>
+        <f t="shared" ref="O87:V87" si="62">N87*(1+O89)</f>
         <v>2057.2848967789942</v>
       </c>
       <c r="P87" s="35">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>2079.7387887743166</v>
       </c>
       <c r="Q87" s="35">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>2094.5668306580201</v>
       </c>
       <c r="R87" s="35">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>2104.8405453917289</v>
       </c>
       <c r="S87" s="35">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>2115.0083455405543</v>
       </c>
       <c r="T87" s="35">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>2122.4223664824062</v>
       </c>
       <c r="U87" s="35">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>2126.9766936324008</v>
       </c>
       <c r="V87" s="35">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>2128.6713269905381</v>
       </c>
       <c r="AL87" s="243"/>
@@ -9145,27 +9151,27 @@
       <c r="D88" s="35"/>
       <c r="F88" s="202"/>
       <c r="G88" s="202">
-        <f t="shared" ref="G88:L88" si="60">(G87/F87)-1</f>
+        <f t="shared" ref="G88:L88" si="63">(G87/F87)-1</f>
         <v>7.8113264233139468E-3</v>
       </c>
       <c r="H88" s="202">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>6.3596164356336526E-3</v>
       </c>
       <c r="I88" s="202">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>1.3823747222907468E-3</v>
       </c>
       <c r="J88" s="202">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>3.5990731154167399E-3</v>
       </c>
       <c r="K88" s="202">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>2.6527805069758159E-3</v>
       </c>
       <c r="L88" s="202">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>-1.36697697207252E-2</v>
       </c>
       <c r="M88" s="199">
@@ -9325,31 +9331,31 @@
         <v>2341.3399454812497</v>
       </c>
       <c r="P91">
-        <f t="shared" ref="P91:V91" si="61">O91*(1+P93)</f>
+        <f t="shared" ref="P91:V91" si="64">O91*(1+P93)</f>
         <v>2347.1932953449527</v>
       </c>
       <c r="Q91">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>2358.9292618216773</v>
       </c>
       <c r="R91">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>2376.6212312853399</v>
       </c>
       <c r="S91">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>2400.3874435981934</v>
       </c>
       <c r="T91">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>2425.6725640591153</v>
       </c>
       <c r="U91">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>2448.4591548302242</v>
       </c>
       <c r="V91">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>2468.5473335363272</v>
       </c>
       <c r="W91"/>
@@ -9370,11 +9376,11 @@
       <c r="I92" s="202"/>
       <c r="J92" s="202"/>
       <c r="K92" s="202">
-        <f t="shared" ref="K92" si="62">(K90/J90)-1</f>
+        <f t="shared" ref="K92" si="65">(K90/J90)-1</f>
         <v>1.0265546788835067E-2</v>
       </c>
       <c r="L92" s="202">
-        <f t="shared" ref="L92" si="63">(L90/K90)-1</f>
+        <f t="shared" ref="L92" si="66">(L90/K90)-1</f>
         <v>-1.9776620759153429E-2</v>
       </c>
       <c r="M92" s="202">
@@ -9467,83 +9473,83 @@
         <v>164</v>
       </c>
       <c r="F95" s="203">
-        <f>F81+F40-F77</f>
+        <f t="shared" ref="F95:Y95" si="67">F81+F40-F77</f>
         <v>339220</v>
       </c>
       <c r="G95" s="203">
-        <f>G81+G40-G77</f>
+        <f t="shared" si="67"/>
         <v>334185</v>
       </c>
       <c r="H95" s="203">
-        <f>H81+H40-H77</f>
+        <f t="shared" si="67"/>
         <v>335532</v>
       </c>
       <c r="I95" s="203">
-        <f>I81+I40-I77</f>
+        <f t="shared" si="67"/>
         <v>344546</v>
       </c>
       <c r="J95" s="203">
-        <f>J81+J40-J77</f>
+        <f t="shared" si="67"/>
         <v>349558</v>
       </c>
       <c r="K95" s="203">
-        <f>K81+K40-K77</f>
+        <f t="shared" si="67"/>
         <v>343658</v>
       </c>
       <c r="L95" s="203">
-        <f>L81+L40-L77</f>
+        <f t="shared" si="67"/>
         <v>577118</v>
       </c>
       <c r="M95" s="199">
-        <f>M81+M40-M77</f>
+        <f t="shared" si="67"/>
         <v>489927</v>
       </c>
       <c r="N95" s="223">
-        <f>N81+N40-N77</f>
+        <f t="shared" si="67"/>
         <v>405893.45314006024</v>
       </c>
       <c r="O95" s="223">
-        <f>O81+O40-O77</f>
+        <f t="shared" si="67"/>
         <v>389550.39386997721</v>
       </c>
       <c r="P95" s="223">
-        <f>P81+P40-P77</f>
+        <f t="shared" si="67"/>
         <v>375767.36763263971</v>
       </c>
       <c r="Q95" s="223">
-        <f>Q81+Q40-Q77</f>
+        <f t="shared" si="67"/>
         <v>376485.55942022882</v>
       </c>
       <c r="R95" s="223">
-        <f>R81+R40-R77</f>
+        <f t="shared" si="67"/>
         <v>377568.23354001937</v>
       </c>
       <c r="S95" s="223">
-        <f>S81+S40-S77</f>
+        <f t="shared" si="67"/>
         <v>379022.6257742712</v>
       </c>
       <c r="T95" s="223">
-        <f>T81+T40-T77</f>
+        <f t="shared" si="67"/>
         <v>423984.35574832192</v>
       </c>
       <c r="U95" s="223">
-        <f>U81+U40-U77</f>
+        <f t="shared" si="67"/>
         <v>425378.7992644498</v>
       </c>
       <c r="V95" s="223">
-        <f>V81+V40-V77</f>
+        <f t="shared" si="67"/>
         <v>426608.11131156218</v>
       </c>
       <c r="W95" s="223">
-        <f>W81+W40-W77</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="X95" s="223">
-        <f>X81+X40-X77</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="Y95" s="223">
-        <f>Y81+Y40-Y77</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="AL95" s="243"/>
@@ -9565,55 +9571,55 @@
         <v>156183</v>
       </c>
       <c r="M96" s="199">
-        <f t="shared" ref="M96:U96" si="64">M84-M77</f>
+        <f t="shared" ref="M96:U96" si="68">M84-M77</f>
         <v>205195</v>
       </c>
       <c r="N96" s="142">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>182970.60314006027</v>
       </c>
       <c r="O96" s="142">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>186270.23674497718</v>
       </c>
       <c r="P96" s="142">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>188129.01011482731</v>
       </c>
       <c r="Q96" s="142">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>188129.01011482731</v>
       </c>
       <c r="R96" s="142">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>188129.01011482731</v>
       </c>
       <c r="S96" s="142">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>188129.01011482731</v>
       </c>
       <c r="T96" s="142">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>231543.39706440276</v>
       </c>
       <c r="U96" s="142">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>231543.39706440276</v>
       </c>
       <c r="V96" s="142">
-        <f t="shared" ref="V96:Y96" si="65">V84-V77</f>
+        <f t="shared" ref="V96:Y96" si="69">V84-V77</f>
         <v>231543.39706440276</v>
       </c>
       <c r="W96" s="142">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="X96" s="142">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="Y96" s="142">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="AL96" s="243"/>
@@ -9629,27 +9635,27 @@
         <v>139025</v>
       </c>
       <c r="G97" s="203">
-        <f t="shared" ref="G97:V97" si="66">G95-(G84-G77)</f>
+        <f t="shared" ref="G97:V97" si="70">G95-(G84-G77)</f>
         <v>139342</v>
       </c>
       <c r="H97" s="203">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>140228</v>
       </c>
       <c r="I97" s="203">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>141105</v>
       </c>
       <c r="J97" s="203">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>141335</v>
       </c>
       <c r="K97" s="203">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>142991</v>
       </c>
       <c r="L97" s="203">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>420935</v>
       </c>
       <c r="M97" s="199">
@@ -9657,51 +9663,51 @@
         <v>284732</v>
       </c>
       <c r="N97" s="143">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>222922.84999999998</v>
       </c>
       <c r="O97" s="143">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>203280.15712500003</v>
       </c>
       <c r="P97" s="143">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>187638.3575178124</v>
       </c>
       <c r="Q97" s="143">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>188356.54930540151</v>
       </c>
       <c r="R97" s="143">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>189439.22342519206</v>
       </c>
       <c r="S97" s="143">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>190893.61565944389</v>
       </c>
       <c r="T97" s="143">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>192440.95868391916</v>
       </c>
       <c r="U97" s="143">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>193835.40220004704</v>
       </c>
       <c r="V97" s="143">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>195064.71424715943</v>
       </c>
       <c r="W97" s="143">
-        <f t="shared" ref="W97:Y97" si="67">W95-(W84-W77)</f>
+        <f t="shared" ref="W97:Y97" si="71">W95-(W84-W77)</f>
         <v>0</v>
       </c>
       <c r="X97" s="143">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="Y97" s="143">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="AL97" s="267"/>
@@ -9949,50 +9955,50 @@
     <row r="3" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="299" t="s">
+      <c r="A5" s="313" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="300"/>
-      <c r="C5" s="300"/>
-      <c r="D5" s="300"/>
-      <c r="E5" s="300"/>
-      <c r="F5" s="300"/>
-      <c r="G5" s="300"/>
-      <c r="H5" s="300"/>
-      <c r="I5" s="300"/>
-      <c r="J5" s="300"/>
-      <c r="K5" s="300"/>
-      <c r="L5" s="300"/>
-      <c r="M5" s="300"/>
-      <c r="N5" s="300"/>
-      <c r="O5" s="300"/>
-      <c r="P5" s="300"/>
-      <c r="Q5" s="300"/>
-      <c r="R5" s="300"/>
-      <c r="S5" s="300"/>
+      <c r="B5" s="314"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="314"/>
+      <c r="H5" s="314"/>
+      <c r="I5" s="314"/>
+      <c r="J5" s="314"/>
+      <c r="K5" s="314"/>
+      <c r="L5" s="314"/>
+      <c r="M5" s="314"/>
+      <c r="N5" s="314"/>
+      <c r="O5" s="314"/>
+      <c r="P5" s="314"/>
+      <c r="Q5" s="314"/>
+      <c r="R5" s="314"/>
+      <c r="S5" s="314"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="301" t="s">
+      <c r="A6" s="315" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="301"/>
-      <c r="C6" s="301"/>
-      <c r="D6" s="301"/>
-      <c r="E6" s="301"/>
-      <c r="F6" s="301"/>
-      <c r="G6" s="301"/>
-      <c r="H6" s="301"/>
-      <c r="I6" s="301"/>
-      <c r="J6" s="301"/>
-      <c r="K6" s="301"/>
-      <c r="L6" s="301"/>
-      <c r="M6" s="301"/>
-      <c r="N6" s="301"/>
-      <c r="O6" s="301"/>
-      <c r="P6" s="301"/>
-      <c r="Q6" s="301"/>
-      <c r="R6" s="301"/>
-      <c r="S6" s="301"/>
+      <c r="B6" s="315"/>
+      <c r="C6" s="315"/>
+      <c r="D6" s="315"/>
+      <c r="E6" s="315"/>
+      <c r="F6" s="315"/>
+      <c r="G6" s="315"/>
+      <c r="H6" s="315"/>
+      <c r="I6" s="315"/>
+      <c r="J6" s="315"/>
+      <c r="K6" s="315"/>
+      <c r="L6" s="315"/>
+      <c r="M6" s="315"/>
+      <c r="N6" s="315"/>
+      <c r="O6" s="315"/>
+      <c r="P6" s="315"/>
+      <c r="Q6" s="315"/>
+      <c r="R6" s="315"/>
+      <c r="S6" s="315"/>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
@@ -10033,8 +10039,8 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="131"/>
-      <c r="R8" s="302"/>
-      <c r="S8" s="303"/>
+      <c r="R8" s="316"/>
+      <c r="S8" s="317"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="130"/>
@@ -10299,10 +10305,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="300" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="286"/>
+      <c r="B1" s="300"/>
       <c r="C1" s="35"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -10310,18 +10316,18 @@
       <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="304" t="s">
+      <c r="Z1" s="318" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" s="304"/>
-      <c r="AB1" s="304"/>
-      <c r="AC1" s="285"/>
-      <c r="AD1" s="285"/>
-      <c r="AE1" s="285"/>
-      <c r="AF1" s="285"/>
+      <c r="AA1" s="318"/>
+      <c r="AB1" s="318"/>
+      <c r="AC1" s="299"/>
+      <c r="AD1" s="299"/>
+      <c r="AE1" s="299"/>
+      <c r="AF1" s="299"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A2" s="305" t="s">
+      <c r="A2" s="319" t="s">
         <v>192</v>
       </c>
       <c r="B2" s="107"/>
@@ -10330,45 +10336,45 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A3" s="305"/>
+      <c r="A3" s="319"/>
       <c r="B3" s="108"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A4" s="305"/>
+      <c r="A4" s="319"/>
       <c r="B4" s="109"/>
       <c r="C4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A5" s="305"/>
+      <c r="A5" s="319"/>
       <c r="B5" s="98"/>
       <c r="C5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C7" s="295" t="s">
+      <c r="C7" s="309" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="296"/>
-      <c r="E7" s="296"/>
-      <c r="F7" s="297"/>
-      <c r="G7" s="295" t="s">
+      <c r="D7" s="310"/>
+      <c r="E7" s="310"/>
+      <c r="F7" s="311"/>
+      <c r="G7" s="309" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="296"/>
-      <c r="I7" s="296"/>
-      <c r="J7" s="297"/>
-      <c r="K7" s="295" t="s">
+      <c r="H7" s="310"/>
+      <c r="I7" s="310"/>
+      <c r="J7" s="311"/>
+      <c r="K7" s="309" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="296"/>
-      <c r="M7" s="296"/>
-      <c r="N7" s="297"/>
+      <c r="L7" s="310"/>
+      <c r="M7" s="310"/>
+      <c r="N7" s="311"/>
     </row>
     <row r="8" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
@@ -12249,88 +12255,88 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" s="311" t="s">
+      <c r="A2" s="320" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="311"/>
-      <c r="C2" s="311"/>
-      <c r="D2" s="311"/>
-      <c r="E2" s="311"/>
-      <c r="F2" s="311"/>
-      <c r="G2" s="311"/>
-      <c r="H2" s="311"/>
-      <c r="I2" s="311"/>
-      <c r="J2" s="311"/>
+      <c r="B2" s="320"/>
+      <c r="C2" s="320"/>
+      <c r="D2" s="320"/>
+      <c r="E2" s="320"/>
+      <c r="F2" s="320"/>
+      <c r="G2" s="320"/>
+      <c r="H2" s="320"/>
+      <c r="I2" s="320"/>
+      <c r="J2" s="320"/>
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A3" s="311" t="s">
+      <c r="A3" s="320" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="311"/>
-      <c r="C3" s="311"/>
-      <c r="D3" s="311"/>
-      <c r="E3" s="311"/>
-      <c r="F3" s="311"/>
-      <c r="G3" s="311"/>
-      <c r="H3" s="311"/>
-      <c r="I3" s="311"/>
-      <c r="J3" s="311"/>
+      <c r="B3" s="320"/>
+      <c r="C3" s="320"/>
+      <c r="D3" s="320"/>
+      <c r="E3" s="320"/>
+      <c r="F3" s="320"/>
+      <c r="G3" s="320"/>
+      <c r="H3" s="320"/>
+      <c r="I3" s="320"/>
+      <c r="J3" s="320"/>
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="312"/>
-      <c r="B4" s="312"/>
-      <c r="C4" s="312"/>
-      <c r="D4" s="312"/>
-      <c r="E4" s="312"/>
-      <c r="F4" s="312"/>
-      <c r="G4" s="312"/>
-      <c r="H4" s="312"/>
-      <c r="I4" s="312"/>
-      <c r="J4" s="312"/>
-      <c r="K4" s="317" t="s">
+      <c r="A4" s="321"/>
+      <c r="B4" s="321"/>
+      <c r="C4" s="321"/>
+      <c r="D4" s="321"/>
+      <c r="E4" s="321"/>
+      <c r="F4" s="321"/>
+      <c r="G4" s="321"/>
+      <c r="H4" s="321"/>
+      <c r="I4" s="321"/>
+      <c r="J4" s="321"/>
+      <c r="K4" s="326" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="317"/>
-      <c r="M4" s="317"/>
-      <c r="N4" s="317"/>
+      <c r="L4" s="326"/>
+      <c r="M4" s="326"/>
+      <c r="N4" s="326"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
-      <c r="C5" s="313" t="s">
+      <c r="C5" s="322" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="314"/>
-      <c r="E5" s="314"/>
-      <c r="F5" s="314"/>
-      <c r="G5" s="314"/>
-      <c r="H5" s="314"/>
-      <c r="I5" s="314"/>
-      <c r="J5" s="315"/>
+      <c r="D5" s="323"/>
+      <c r="E5" s="323"/>
+      <c r="F5" s="323"/>
+      <c r="G5" s="323"/>
+      <c r="H5" s="323"/>
+      <c r="I5" s="323"/>
+      <c r="J5" s="324"/>
       <c r="K5" s="78"/>
-      <c r="L5" s="316" t="s">
+      <c r="L5" s="325" t="s">
         <v>107</v>
       </c>
-      <c r="M5" s="285"/>
-      <c r="N5" s="285"/>
+      <c r="M5" s="299"/>
+      <c r="N5" s="299"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="307">
+      <c r="C6" s="328">
         <v>2020</v>
       </c>
-      <c r="D6" s="308"/>
-      <c r="E6" s="308"/>
-      <c r="F6" s="308"/>
-      <c r="G6" s="308"/>
-      <c r="H6" s="308"/>
-      <c r="I6" s="308"/>
-      <c r="J6" s="309"/>
+      <c r="D6" s="329"/>
+      <c r="E6" s="329"/>
+      <c r="F6" s="329"/>
+      <c r="G6" s="329"/>
+      <c r="H6" s="329"/>
+      <c r="I6" s="329"/>
+      <c r="J6" s="330"/>
       <c r="K6" s="78" t="s">
         <v>135</v>
       </c>
@@ -12767,24 +12773,24 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="K22" s="285" t="s">
+      <c r="K22" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="285"/>
-      <c r="M22" s="285"/>
-      <c r="N22" s="285"/>
-      <c r="O22" s="285" t="s">
+      <c r="L22" s="299"/>
+      <c r="M22" s="299"/>
+      <c r="N22" s="299"/>
+      <c r="O22" s="299" t="s">
         <v>10</v>
       </c>
-      <c r="P22" s="285"/>
-      <c r="Q22" s="285"/>
-      <c r="R22" s="285"/>
-      <c r="S22" s="285" t="s">
+      <c r="P22" s="299"/>
+      <c r="Q22" s="299"/>
+      <c r="R22" s="299"/>
+      <c r="S22" s="299" t="s">
         <v>11</v>
       </c>
-      <c r="T22" s="285"/>
-      <c r="U22" s="285"/>
-      <c r="V22" s="285"/>
+      <c r="T22" s="299"/>
+      <c r="U22" s="299"/>
+      <c r="V22" s="299"/>
     </row>
     <row r="23" spans="3:23" x14ac:dyDescent="0.35">
       <c r="C23" s="67"/>
@@ -12801,12 +12807,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="K23" s="310" t="s">
+      <c r="K23" s="331" t="s">
         <v>108</v>
       </c>
-      <c r="L23" s="310"/>
-      <c r="M23" s="310"/>
-      <c r="N23" s="310"/>
+      <c r="L23" s="331"/>
+      <c r="M23" s="331"/>
+      <c r="N23" s="331"/>
       <c r="O23" s="35" t="s">
         <v>146</v>
       </c>
@@ -12975,7 +12981,7 @@
       <c r="S27" s="72"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.35">
-      <c r="I28" s="306" t="s">
+      <c r="I28" s="327" t="s">
         <v>259</v>
       </c>
       <c r="J28" s="82" t="s">
@@ -13026,7 +13032,7 @@
       <c r="H29">
         <v>67</v>
       </c>
-      <c r="I29" s="306"/>
+      <c r="I29" s="327"/>
       <c r="J29" s="82" t="s">
         <v>143</v>
       </c>
@@ -13075,7 +13081,7 @@
         <f>H29</f>
         <v>67</v>
       </c>
-      <c r="I30" s="306"/>
+      <c r="I30" s="327"/>
       <c r="J30" s="82" t="s">
         <v>142</v>
       </c>
@@ -13124,7 +13130,7 @@
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="I31" s="306"/>
+      <c r="I31" s="327"/>
       <c r="J31" s="35" t="s">
         <v>140</v>
       </c>
@@ -13186,7 +13192,7 @@
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="I33" s="306" t="s">
+      <c r="I33" s="327" t="s">
         <v>141</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -13234,7 +13240,7 @@
       </c>
     </row>
     <row r="34" spans="3:23" x14ac:dyDescent="0.35">
-      <c r="I34" s="306"/>
+      <c r="I34" s="327"/>
       <c r="J34" t="s">
         <v>260</v>
       </c>
@@ -13413,12 +13419,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="K4:N4"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="I28:I31"/>
@@ -13426,6 +13426,12 @@
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K23:N23"/>
     <mergeCell ref="K22:N22"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -13533,30 +13539,30 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="319" t="s">
+      <c r="E6" s="335" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="319"/>
-      <c r="G6" s="319"/>
-      <c r="H6" s="319"/>
-      <c r="I6" s="319"/>
-      <c r="J6" s="319"/>
-      <c r="K6" s="319"/>
-      <c r="L6" s="319"/>
-      <c r="M6" s="319"/>
-      <c r="N6" s="319"/>
-      <c r="O6" s="319"/>
-      <c r="P6" s="319"/>
-      <c r="Q6" s="319"/>
-      <c r="R6" s="319"/>
+      <c r="F6" s="335"/>
+      <c r="G6" s="335"/>
+      <c r="H6" s="335"/>
+      <c r="I6" s="335"/>
+      <c r="J6" s="335"/>
+      <c r="K6" s="335"/>
+      <c r="L6" s="335"/>
+      <c r="M6" s="335"/>
+      <c r="N6" s="335"/>
+      <c r="O6" s="335"/>
+      <c r="P6" s="335"/>
+      <c r="Q6" s="335"/>
+      <c r="R6" s="335"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="318" t="s">
+      <c r="A7" s="332" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="318"/>
-      <c r="C7" s="318"/>
-      <c r="D7" s="318"/>
+      <c r="B7" s="332"/>
+      <c r="C7" s="332"/>
+      <c r="D7" s="332"/>
       <c r="E7" s="36"/>
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
@@ -13574,11 +13580,11 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="36"/>
-      <c r="B8" s="318" t="s">
+      <c r="B8" s="332" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="318"/>
-      <c r="D8" s="318"/>
+      <c r="C8" s="332"/>
+      <c r="D8" s="332"/>
       <c r="E8" s="42">
         <v>1717.857</v>
       </c>
@@ -13624,11 +13630,11 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="36"/>
-      <c r="B9" s="318" t="s">
+      <c r="B9" s="332" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="318"/>
-      <c r="D9" s="318"/>
+      <c r="C9" s="332"/>
+      <c r="D9" s="332"/>
       <c r="E9" s="42">
         <v>1243.3720000000001</v>
       </c>
@@ -13674,11 +13680,11 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="36"/>
-      <c r="B10" s="318" t="s">
+      <c r="B10" s="332" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="318"/>
-      <c r="D10" s="318"/>
+      <c r="C10" s="332"/>
+      <c r="D10" s="332"/>
       <c r="E10" s="42">
         <v>230.245</v>
       </c>
@@ -13724,11 +13730,11 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="36"/>
-      <c r="B11" s="318" t="s">
+      <c r="B11" s="332" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="318"/>
-      <c r="D11" s="318"/>
+      <c r="C11" s="332"/>
+      <c r="D11" s="332"/>
       <c r="E11" s="42">
         <v>271.327</v>
       </c>
@@ -13823,10 +13829,10 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="36"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="318" t="s">
+      <c r="C13" s="332" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="318"/>
+      <c r="D13" s="332"/>
       <c r="E13" s="42">
         <v>3462.8009999999999</v>
       </c>
@@ -13977,11 +13983,11 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="36"/>
-      <c r="B19" s="318" t="s">
+      <c r="B19" s="332" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="318"/>
-      <c r="D19" s="318"/>
+      <c r="C19" s="332"/>
+      <c r="D19" s="332"/>
       <c r="E19" s="42">
         <v>1717.857</v>
       </c>
@@ -14040,11 +14046,11 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="36"/>
-      <c r="B20" s="318" t="s">
+      <c r="B20" s="332" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="318"/>
-      <c r="D20" s="318"/>
+      <c r="C20" s="332"/>
+      <c r="D20" s="332"/>
       <c r="E20" s="42">
         <v>1243.3720000000001</v>
       </c>
@@ -14104,11 +14110,11 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="36"/>
-      <c r="B21" s="318" t="s">
+      <c r="B21" s="332" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="318"/>
-      <c r="D21" s="318"/>
+      <c r="C21" s="332"/>
+      <c r="D21" s="332"/>
       <c r="E21" s="42">
         <v>230.245</v>
       </c>
@@ -14167,11 +14173,11 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="36"/>
-      <c r="B22" s="318" t="s">
+      <c r="B22" s="332" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="318"/>
-      <c r="D22" s="318"/>
+      <c r="C22" s="332"/>
+      <c r="D22" s="332"/>
       <c r="E22" s="42">
         <v>271.327</v>
       </c>
@@ -14284,21 +14290,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="320" t="s">
+      <c r="H27" s="333" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="320"/>
-      <c r="J27" s="320"/>
-      <c r="K27" s="320"/>
-      <c r="L27" s="320"/>
-      <c r="M27" s="320"/>
-      <c r="N27" s="320"/>
-      <c r="O27" s="320"/>
-      <c r="P27" s="320"/>
-      <c r="Q27" s="320"/>
-      <c r="R27" s="320"/>
-      <c r="S27" s="320"/>
-      <c r="T27" s="320"/>
+      <c r="I27" s="333"/>
+      <c r="J27" s="333"/>
+      <c r="K27" s="333"/>
+      <c r="L27" s="333"/>
+      <c r="M27" s="333"/>
+      <c r="N27" s="333"/>
+      <c r="O27" s="333"/>
+      <c r="P27" s="333"/>
+      <c r="Q27" s="333"/>
+      <c r="R27" s="333"/>
+      <c r="S27" s="333"/>
+      <c r="T27" s="333"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="24" t="s">
@@ -14614,21 +14620,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="321" t="s">
+      <c r="F37" s="334" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="321"/>
-      <c r="H37" s="321"/>
-      <c r="I37" s="321"/>
-      <c r="J37" s="321"/>
-      <c r="K37" s="321"/>
-      <c r="L37" s="321"/>
-      <c r="M37" s="321"/>
-      <c r="N37" s="321"/>
-      <c r="O37" s="321"/>
-      <c r="P37" s="321"/>
-      <c r="Q37" s="321"/>
-      <c r="R37" s="321"/>
+      <c r="G37" s="334"/>
+      <c r="H37" s="334"/>
+      <c r="I37" s="334"/>
+      <c r="J37" s="334"/>
+      <c r="K37" s="334"/>
+      <c r="L37" s="334"/>
+      <c r="M37" s="334"/>
+      <c r="N37" s="334"/>
+      <c r="O37" s="334"/>
+      <c r="P37" s="334"/>
+      <c r="Q37" s="334"/>
+      <c r="R37" s="334"/>
     </row>
     <row r="38" spans="1:18" ht="17" x14ac:dyDescent="0.35">
       <c r="A38" s="24" t="s">
@@ -14944,21 +14950,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="320" t="s">
+      <c r="F48" s="333" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="320"/>
-      <c r="H48" s="320"/>
-      <c r="I48" s="320"/>
-      <c r="J48" s="320"/>
-      <c r="K48" s="320"/>
-      <c r="L48" s="320"/>
-      <c r="M48" s="320"/>
-      <c r="N48" s="320"/>
-      <c r="O48" s="320"/>
-      <c r="P48" s="320"/>
-      <c r="Q48" s="320"/>
-      <c r="R48" s="320"/>
+      <c r="G48" s="333"/>
+      <c r="H48" s="333"/>
+      <c r="I48" s="333"/>
+      <c r="J48" s="333"/>
+      <c r="K48" s="333"/>
+      <c r="L48" s="333"/>
+      <c r="M48" s="333"/>
+      <c r="N48" s="333"/>
+      <c r="O48" s="333"/>
+      <c r="P48" s="333"/>
+      <c r="Q48" s="333"/>
+      <c r="R48" s="333"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="24" t="s">
@@ -15270,6 +15276,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -15278,12 +15290,6 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15322,50 +15328,50 @@
     <row r="3" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="299" t="s">
+      <c r="A5" s="313" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="300"/>
-      <c r="C5" s="300"/>
-      <c r="D5" s="300"/>
-      <c r="E5" s="300"/>
-      <c r="F5" s="300"/>
-      <c r="G5" s="300"/>
-      <c r="H5" s="300"/>
-      <c r="I5" s="300"/>
-      <c r="J5" s="300"/>
-      <c r="K5" s="300"/>
-      <c r="L5" s="300"/>
-      <c r="M5" s="300"/>
-      <c r="N5" s="300"/>
-      <c r="O5" s="300"/>
-      <c r="P5" s="300"/>
-      <c r="Q5" s="300"/>
-      <c r="R5" s="300"/>
-      <c r="S5" s="300"/>
+      <c r="B5" s="314"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="314"/>
+      <c r="H5" s="314"/>
+      <c r="I5" s="314"/>
+      <c r="J5" s="314"/>
+      <c r="K5" s="314"/>
+      <c r="L5" s="314"/>
+      <c r="M5" s="314"/>
+      <c r="N5" s="314"/>
+      <c r="O5" s="314"/>
+      <c r="P5" s="314"/>
+      <c r="Q5" s="314"/>
+      <c r="R5" s="314"/>
+      <c r="S5" s="314"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="301" t="s">
+      <c r="A6" s="315" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="301"/>
-      <c r="C6" s="301"/>
-      <c r="D6" s="301"/>
-      <c r="E6" s="301"/>
-      <c r="F6" s="301"/>
-      <c r="G6" s="301"/>
-      <c r="H6" s="301"/>
-      <c r="I6" s="301"/>
-      <c r="J6" s="301"/>
-      <c r="K6" s="301"/>
-      <c r="L6" s="301"/>
-      <c r="M6" s="301"/>
-      <c r="N6" s="301"/>
-      <c r="O6" s="301"/>
-      <c r="P6" s="301"/>
-      <c r="Q6" s="301"/>
-      <c r="R6" s="301"/>
-      <c r="S6" s="301"/>
+      <c r="B6" s="315"/>
+      <c r="C6" s="315"/>
+      <c r="D6" s="315"/>
+      <c r="E6" s="315"/>
+      <c r="F6" s="315"/>
+      <c r="G6" s="315"/>
+      <c r="H6" s="315"/>
+      <c r="I6" s="315"/>
+      <c r="J6" s="315"/>
+      <c r="K6" s="315"/>
+      <c r="L6" s="315"/>
+      <c r="M6" s="315"/>
+      <c r="N6" s="315"/>
+      <c r="O6" s="315"/>
+      <c r="P6" s="315"/>
+      <c r="Q6" s="315"/>
+      <c r="R6" s="315"/>
+      <c r="S6" s="315"/>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
@@ -15405,10 +15411,10 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="302" t="s">
+      <c r="R8" s="316" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="303"/>
+      <c r="S8" s="317"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
@@ -18279,10 +18285,10 @@
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
-      <c r="D75" s="322" t="s">
+      <c r="D75" s="336" t="s">
         <v>42</v>
       </c>
-      <c r="E75" s="323"/>
+      <c r="E75" s="337"/>
       <c r="F75" s="25">
         <v>-75.135000000000005</v>
       </c>
@@ -18980,23 +18986,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="304" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="291"/>
+      <c r="B1" s="305"/>
       <c r="C1" s="35"/>
       <c r="H1"/>
       <c r="I1" s="250"/>
-      <c r="J1" s="298" t="s">
+      <c r="J1" s="312" t="s">
         <v>282</v>
       </c>
-      <c r="V1" s="285"/>
-      <c r="W1" s="285"/>
-      <c r="X1" s="285"/>
-      <c r="Y1" s="285"/>
+      <c r="V1" s="299"/>
+      <c r="W1" s="299"/>
+      <c r="X1" s="299"/>
+      <c r="Y1" s="299"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" s="292" t="s">
+      <c r="A2" s="306" t="s">
         <v>192</v>
       </c>
       <c r="B2" s="126"/>
@@ -19004,68 +19010,68 @@
         <v>193</v>
       </c>
       <c r="I2" s="251"/>
-      <c r="J2" s="298"/>
+      <c r="J2" s="312"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="293"/>
+      <c r="A3" s="307"/>
       <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
       <c r="I3" s="251"/>
-      <c r="J3" s="298"/>
+      <c r="J3" s="312"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" s="293"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" s="294"/>
+      <c r="A5" s="308"/>
       <c r="B5" s="129"/>
       <c r="C5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C7" s="295" t="s">
+      <c r="C7" s="309" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="296"/>
-      <c r="E7" s="296"/>
-      <c r="F7" s="297"/>
-      <c r="G7" s="295" t="s">
+      <c r="D7" s="310"/>
+      <c r="E7" s="310"/>
+      <c r="F7" s="311"/>
+      <c r="G7" s="309" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="296"/>
-      <c r="I7" s="296"/>
-      <c r="J7" s="297"/>
-      <c r="K7" s="295" t="s">
+      <c r="H7" s="310"/>
+      <c r="I7" s="310"/>
+      <c r="J7" s="311"/>
+      <c r="K7" s="309" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="296"/>
-      <c r="M7" s="296"/>
-      <c r="N7" s="296"/>
-      <c r="O7" s="295" t="s">
+      <c r="L7" s="310"/>
+      <c r="M7" s="310"/>
+      <c r="N7" s="310"/>
+      <c r="O7" s="309" t="s">
         <v>272</v>
       </c>
-      <c r="P7" s="296"/>
-      <c r="Q7" s="296"/>
-      <c r="R7" s="296"/>
-      <c r="S7" s="295" t="s">
+      <c r="P7" s="310"/>
+      <c r="Q7" s="310"/>
+      <c r="R7" s="310"/>
+      <c r="S7" s="309" t="s">
         <v>276</v>
       </c>
-      <c r="T7" s="296"/>
-      <c r="U7" s="296"/>
-      <c r="V7" s="296"/>
-      <c r="W7" s="295" t="s">
+      <c r="T7" s="310"/>
+      <c r="U7" s="310"/>
+      <c r="V7" s="310"/>
+      <c r="W7" s="309" t="s">
         <v>277</v>
       </c>
-      <c r="X7" s="296"/>
-      <c r="Y7" s="296"/>
-      <c r="Z7" s="296"/>
+      <c r="X7" s="310"/>
+      <c r="Y7" s="310"/>
+      <c r="Z7" s="310"/>
       <c r="AA7" s="231" t="s">
         <v>278</v>
       </c>
@@ -23234,10 +23240,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304CD302-ECA7-4CE9-B89D-A357A53FDBE8}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23246,7 +23253,7 @@
     <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>257</v>
       </c>
@@ -23286,8 +23293,11 @@
       <c r="M1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="190">
         <v>44012</v>
       </c>
@@ -23328,8 +23338,12 @@
         <f t="array" ref="M2:M12">TRANSPOSE(main!L40:V40)/1000</f>
         <v>277.60000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2">
+        <f t="array" ref="N2:N16">TRANSPOSE(main!L68:Z68/1000)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="190">
         <v>44104</v>
       </c>
@@ -23379,8 +23393,11 @@
       <c r="M3">
         <v>140</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="190">
         <v>44196</v>
       </c>
@@ -23418,8 +23435,11 @@
       <c r="M4">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="190">
         <v>44286</v>
       </c>
@@ -23456,8 +23476,11 @@
       <c r="M5">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <v>190.66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="190">
         <v>44377</v>
       </c>
@@ -23494,8 +23517,11 @@
       <c r="M6">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>190.66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="190">
         <v>44469</v>
       </c>
@@ -23532,8 +23558,11 @@
       <c r="M7">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>190.66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="190">
         <v>44561</v>
       </c>
@@ -23570,8 +23599,11 @@
       <c r="M8">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="190">
         <v>44651</v>
       </c>
@@ -23608,8 +23640,11 @@
       <c r="M9">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="190">
         <v>44742</v>
       </c>
@@ -23646,8 +23681,11 @@
       <c r="M10">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="190">
         <v>44834</v>
       </c>
@@ -23684,8 +23722,11 @@
       <c r="M11">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="190">
         <v>44926</v>
       </c>
@@ -23719,8 +23760,11 @@
       <c r="M12">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="190">
         <v>45016</v>
       </c>
@@ -23748,8 +23792,11 @@
       <c r="I13">
         <v>-2.8700840526758213</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="190">
         <v>45107</v>
       </c>
@@ -23777,8 +23824,11 @@
       <c r="I14">
         <v>-3.0081206958325879</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="190">
         <v>45199</v>
       </c>
@@ -23806,8 +23856,11 @@
       <c r="I15">
         <v>-3.1545408316389967</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="190">
         <v>45291</v>
       </c>
@@ -23834,6 +23887,9 @@
       </c>
       <c r="I16">
         <v>-3.1755686603398772</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -24088,36 +24144,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="D1" s="285" t="s">
+      <c r="D1" s="299" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
-      <c r="H1" s="285" t="s">
+      <c r="E1" s="299"/>
+      <c r="F1" s="299"/>
+      <c r="G1" s="299"/>
+      <c r="H1" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="285"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="285"/>
-      <c r="L1" s="285" t="s">
+      <c r="I1" s="299"/>
+      <c r="J1" s="299"/>
+      <c r="K1" s="299"/>
+      <c r="L1" s="299" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="285"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="285"/>
-      <c r="P1" s="285" t="s">
+      <c r="M1" s="299"/>
+      <c r="N1" s="299"/>
+      <c r="O1" s="299"/>
+      <c r="P1" s="299" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="285"/>
-      <c r="R1" s="285"/>
-      <c r="S1" s="285"/>
-      <c r="T1" s="285" t="s">
+      <c r="Q1" s="299"/>
+      <c r="R1" s="299"/>
+      <c r="S1" s="299"/>
+      <c r="T1" s="299" t="s">
         <v>268</v>
       </c>
-      <c r="U1" s="285"/>
-      <c r="V1" s="285"/>
-      <c r="W1" s="285"/>
+      <c r="U1" s="299"/>
+      <c r="V1" s="299"/>
+      <c r="W1" s="299"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="D2" s="199" t="s">
@@ -24527,22 +24583,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="304" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="291"/>
+      <c r="B1" s="305"/>
       <c r="C1" s="35"/>
       <c r="I1" s="250"/>
-      <c r="J1" s="298" t="s">
+      <c r="J1" s="312" t="s">
         <v>282</v>
       </c>
-      <c r="V1" s="285"/>
-      <c r="W1" s="285"/>
-      <c r="X1" s="285"/>
-      <c r="Y1" s="285"/>
+      <c r="V1" s="299"/>
+      <c r="W1" s="299"/>
+      <c r="X1" s="299"/>
+      <c r="Y1" s="299"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" s="292" t="s">
+      <c r="A2" s="306" t="s">
         <v>192</v>
       </c>
       <c r="B2" s="126"/>
@@ -24551,20 +24607,20 @@
       </c>
       <c r="H2" s="95"/>
       <c r="I2" s="251"/>
-      <c r="J2" s="298"/>
+      <c r="J2" s="312"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="293"/>
+      <c r="A3" s="307"/>
       <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
       <c r="H3" s="95"/>
       <c r="I3" s="251"/>
-      <c r="J3" s="298"/>
+      <c r="J3" s="312"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" s="293"/>
+      <c r="A4" s="307"/>
       <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>195</v>
@@ -24574,7 +24630,7 @@
       <c r="J4" s="95"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" s="294"/>
+      <c r="A5" s="308"/>
       <c r="B5" s="129"/>
       <c r="C5" t="s">
         <v>182</v>
@@ -24589,42 +24645,42 @@
       <c r="J6" s="95"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C7" s="295" t="s">
+      <c r="C7" s="309" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="296"/>
-      <c r="E7" s="296"/>
-      <c r="F7" s="297"/>
-      <c r="G7" s="295" t="s">
+      <c r="D7" s="310"/>
+      <c r="E7" s="310"/>
+      <c r="F7" s="311"/>
+      <c r="G7" s="309" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="296"/>
-      <c r="I7" s="296"/>
-      <c r="J7" s="297"/>
-      <c r="K7" s="295" t="s">
+      <c r="H7" s="310"/>
+      <c r="I7" s="310"/>
+      <c r="J7" s="311"/>
+      <c r="K7" s="309" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="296"/>
-      <c r="M7" s="296"/>
-      <c r="N7" s="296"/>
-      <c r="O7" s="295" t="s">
+      <c r="L7" s="310"/>
+      <c r="M7" s="310"/>
+      <c r="N7" s="310"/>
+      <c r="O7" s="309" t="s">
         <v>272</v>
       </c>
-      <c r="P7" s="296"/>
-      <c r="Q7" s="296"/>
-      <c r="R7" s="296"/>
-      <c r="S7" s="295" t="s">
+      <c r="P7" s="310"/>
+      <c r="Q7" s="310"/>
+      <c r="R7" s="310"/>
+      <c r="S7" s="309" t="s">
         <v>276</v>
       </c>
-      <c r="T7" s="296"/>
-      <c r="U7" s="296"/>
-      <c r="V7" s="296"/>
-      <c r="W7" s="295" t="s">
+      <c r="T7" s="310"/>
+      <c r="U7" s="310"/>
+      <c r="V7" s="310"/>
+      <c r="W7" s="309" t="s">
         <v>277</v>
       </c>
-      <c r="X7" s="296"/>
-      <c r="Y7" s="296"/>
-      <c r="Z7" s="296"/>
+      <c r="X7" s="310"/>
+      <c r="Y7" s="310"/>
+      <c r="Z7" s="310"/>
       <c r="AA7" s="231" t="s">
         <v>278</v>
       </c>
@@ -27434,7 +27490,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29073,7 +29129,7 @@
   <dimension ref="A2:P28"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -29694,12 +29750,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29920,15 +29973,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
+    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -29953,18 +30018,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
-    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed no addons script
</commit_message>
<xml_diff>
--- a/documentation/COVID-19 Changes/September/LSFIM_KY_v6_round2.xlsx
+++ b/documentation/COVID-19 Changes/September/LSFIM_KY_v6_round2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/GitHub/Fiscal-Impact-Measure/documentation/COVID-19 Changes/September/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC038D98-3489-2D44-AEA9-51A842123149}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08109445-1EA8-C642-8B03-D8F0119526D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="460" windowWidth="33600" windowHeight="18880" activeTab="2" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
+    <workbookView xWindow="2420" yWindow="460" windowWidth="33600" windowHeight="18880" activeTab="2" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -3504,6 +3504,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="33" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3570,6 +3571,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3591,34 +3607,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="33" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4150,10 +4150,10 @@
   <dimension ref="A1:AQ115"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="G77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O33" sqref="O33"/>
+      <selection pane="bottomRight" activeCell="M105" sqref="M105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4175,10 +4175,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="315" t="s">
+      <c r="A1" s="316" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="315"/>
+      <c r="B1" s="316"/>
       <c r="C1" s="279"/>
       <c r="D1" s="279"/>
       <c r="E1" s="35"/>
@@ -4188,76 +4188,76 @@
       <c r="AC1" s="179" t="s">
         <v>249</v>
       </c>
-      <c r="AD1" s="317" t="s">
+      <c r="AD1" s="318" t="s">
         <v>247</v>
       </c>
-      <c r="AE1" s="317"/>
-      <c r="AF1" s="317"/>
+      <c r="AE1" s="318"/>
+      <c r="AF1" s="318"/>
       <c r="AG1" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="318" t="s">
+      <c r="AI1" s="319" t="s">
         <v>281</v>
       </c>
-      <c r="AJ1" s="318"/>
-      <c r="AK1" s="318"/>
-      <c r="AL1" s="318"/>
-      <c r="AM1" s="316" t="s">
+      <c r="AJ1" s="319"/>
+      <c r="AK1" s="319"/>
+      <c r="AL1" s="319"/>
+      <c r="AM1" s="317" t="s">
         <v>279</v>
       </c>
-      <c r="AN1" s="316"/>
-      <c r="AO1" s="316"/>
-      <c r="AP1" s="316"/>
+      <c r="AN1" s="317"/>
+      <c r="AO1" s="317"/>
+      <c r="AP1" s="317"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="F2" s="314" t="s">
+      <c r="F2" s="315" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="314"/>
-      <c r="H2" s="314"/>
-      <c r="I2" s="314"/>
-      <c r="J2" s="314" t="s">
+      <c r="G2" s="315"/>
+      <c r="H2" s="315"/>
+      <c r="I2" s="315"/>
+      <c r="J2" s="315" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="314"/>
-      <c r="L2" s="314"/>
-      <c r="M2" s="314"/>
-      <c r="N2" s="314" t="s">
+      <c r="K2" s="315"/>
+      <c r="L2" s="315"/>
+      <c r="M2" s="315"/>
+      <c r="N2" s="315" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="314"/>
-      <c r="P2" s="314"/>
-      <c r="Q2" s="314"/>
-      <c r="R2" s="314" t="s">
+      <c r="O2" s="315"/>
+      <c r="P2" s="315"/>
+      <c r="Q2" s="315"/>
+      <c r="R2" s="315" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="314"/>
-      <c r="T2" s="314"/>
-      <c r="U2" s="314"/>
-      <c r="V2" s="314" t="s">
+      <c r="S2" s="315"/>
+      <c r="T2" s="315"/>
+      <c r="U2" s="315"/>
+      <c r="V2" s="315" t="s">
         <v>268</v>
       </c>
-      <c r="W2" s="314"/>
-      <c r="X2" s="314"/>
-      <c r="Y2" s="314"/>
+      <c r="W2" s="315"/>
+      <c r="X2" s="315"/>
+      <c r="Y2" s="315"/>
       <c r="Z2" s="229"/>
       <c r="AA2" s="296"/>
       <c r="AB2" s="229"/>
       <c r="AC2" s="156"/>
-      <c r="AD2" s="314" t="s">
+      <c r="AD2" s="315" t="s">
         <v>102</v>
       </c>
-      <c r="AE2" s="314"/>
-      <c r="AF2" s="314"/>
+      <c r="AE2" s="315"/>
+      <c r="AF2" s="315"/>
       <c r="AG2" s="156"/>
       <c r="AH2" s="156" t="s">
         <v>21</v>
       </c>
-      <c r="AI2" s="314" t="s">
+      <c r="AI2" s="315" t="s">
         <v>102</v>
       </c>
-      <c r="AJ2" s="314"/>
-      <c r="AK2" s="314"/>
+      <c r="AJ2" s="315"/>
+      <c r="AK2" s="315"/>
       <c r="AL2" s="230"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.2">
@@ -4365,10 +4365,10 @@
       </c>
     </row>
     <row r="4" spans="1:43" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="313" t="s">
+      <c r="A4" s="314" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="313"/>
+      <c r="B4" s="314"/>
       <c r="C4" s="279"/>
       <c r="D4" s="279"/>
       <c r="F4" s="199"/>
@@ -12233,50 +12233,50 @@
     <row r="3" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="328" t="s">
+      <c r="A5" s="329" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="329"/>
-      <c r="C5" s="329"/>
-      <c r="D5" s="329"/>
-      <c r="E5" s="329"/>
-      <c r="F5" s="329"/>
-      <c r="G5" s="329"/>
-      <c r="H5" s="329"/>
-      <c r="I5" s="329"/>
-      <c r="J5" s="329"/>
-      <c r="K5" s="329"/>
-      <c r="L5" s="329"/>
-      <c r="M5" s="329"/>
-      <c r="N5" s="329"/>
-      <c r="O5" s="329"/>
-      <c r="P5" s="329"/>
-      <c r="Q5" s="329"/>
-      <c r="R5" s="329"/>
-      <c r="S5" s="329"/>
+      <c r="B5" s="330"/>
+      <c r="C5" s="330"/>
+      <c r="D5" s="330"/>
+      <c r="E5" s="330"/>
+      <c r="F5" s="330"/>
+      <c r="G5" s="330"/>
+      <c r="H5" s="330"/>
+      <c r="I5" s="330"/>
+      <c r="J5" s="330"/>
+      <c r="K5" s="330"/>
+      <c r="L5" s="330"/>
+      <c r="M5" s="330"/>
+      <c r="N5" s="330"/>
+      <c r="O5" s="330"/>
+      <c r="P5" s="330"/>
+      <c r="Q5" s="330"/>
+      <c r="R5" s="330"/>
+      <c r="S5" s="330"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="330" t="s">
+      <c r="A6" s="331" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="330"/>
-      <c r="C6" s="330"/>
-      <c r="D6" s="330"/>
-      <c r="E6" s="330"/>
-      <c r="F6" s="330"/>
-      <c r="G6" s="330"/>
-      <c r="H6" s="330"/>
-      <c r="I6" s="330"/>
-      <c r="J6" s="330"/>
-      <c r="K6" s="330"/>
-      <c r="L6" s="330"/>
-      <c r="M6" s="330"/>
-      <c r="N6" s="330"/>
-      <c r="O6" s="330"/>
-      <c r="P6" s="330"/>
-      <c r="Q6" s="330"/>
-      <c r="R6" s="330"/>
-      <c r="S6" s="330"/>
+      <c r="B6" s="331"/>
+      <c r="C6" s="331"/>
+      <c r="D6" s="331"/>
+      <c r="E6" s="331"/>
+      <c r="F6" s="331"/>
+      <c r="G6" s="331"/>
+      <c r="H6" s="331"/>
+      <c r="I6" s="331"/>
+      <c r="J6" s="331"/>
+      <c r="K6" s="331"/>
+      <c r="L6" s="331"/>
+      <c r="M6" s="331"/>
+      <c r="N6" s="331"/>
+      <c r="O6" s="331"/>
+      <c r="P6" s="331"/>
+      <c r="Q6" s="331"/>
+      <c r="R6" s="331"/>
+      <c r="S6" s="331"/>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9"/>
@@ -12317,8 +12317,8 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="131"/>
-      <c r="R8" s="331"/>
-      <c r="S8" s="332"/>
+      <c r="R8" s="332"/>
+      <c r="S8" s="333"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="130"/>
@@ -12583,10 +12583,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="315" t="s">
+      <c r="A1" s="316" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="315"/>
+      <c r="B1" s="316"/>
       <c r="C1" s="35"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -12594,18 +12594,18 @@
       <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="333" t="s">
+      <c r="Z1" s="334" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" s="333"/>
-      <c r="AB1" s="333"/>
-      <c r="AC1" s="314"/>
-      <c r="AD1" s="314"/>
-      <c r="AE1" s="314"/>
-      <c r="AF1" s="314"/>
+      <c r="AA1" s="334"/>
+      <c r="AB1" s="334"/>
+      <c r="AC1" s="315"/>
+      <c r="AD1" s="315"/>
+      <c r="AE1" s="315"/>
+      <c r="AF1" s="315"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A2" s="334" t="s">
+      <c r="A2" s="335" t="s">
         <v>192</v>
       </c>
       <c r="B2" s="107"/>
@@ -12614,45 +12614,45 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A3" s="334"/>
+      <c r="A3" s="335"/>
       <c r="B3" s="108"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="334"/>
+      <c r="A4" s="335"/>
       <c r="B4" s="109"/>
       <c r="C4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A5" s="334"/>
+      <c r="A5" s="335"/>
       <c r="B5" s="98"/>
       <c r="C5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="C7" s="324" t="s">
+      <c r="C7" s="325" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="325"/>
-      <c r="E7" s="325"/>
-      <c r="F7" s="326"/>
-      <c r="G7" s="324" t="s">
+      <c r="D7" s="326"/>
+      <c r="E7" s="326"/>
+      <c r="F7" s="327"/>
+      <c r="G7" s="325" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="325"/>
-      <c r="I7" s="325"/>
-      <c r="J7" s="326"/>
-      <c r="K7" s="324" t="s">
+      <c r="H7" s="326"/>
+      <c r="I7" s="326"/>
+      <c r="J7" s="327"/>
+      <c r="K7" s="325" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="325"/>
-      <c r="M7" s="325"/>
-      <c r="N7" s="326"/>
+      <c r="L7" s="326"/>
+      <c r="M7" s="326"/>
+      <c r="N7" s="327"/>
     </row>
     <row r="8" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
@@ -14533,88 +14533,88 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="335" t="s">
+      <c r="A2" s="341" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="335"/>
-      <c r="C2" s="335"/>
-      <c r="D2" s="335"/>
-      <c r="E2" s="335"/>
-      <c r="F2" s="335"/>
-      <c r="G2" s="335"/>
-      <c r="H2" s="335"/>
-      <c r="I2" s="335"/>
-      <c r="J2" s="335"/>
+      <c r="B2" s="341"/>
+      <c r="C2" s="341"/>
+      <c r="D2" s="341"/>
+      <c r="E2" s="341"/>
+      <c r="F2" s="341"/>
+      <c r="G2" s="341"/>
+      <c r="H2" s="341"/>
+      <c r="I2" s="341"/>
+      <c r="J2" s="341"/>
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="335" t="s">
+      <c r="A3" s="341" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="335"/>
-      <c r="C3" s="335"/>
-      <c r="D3" s="335"/>
-      <c r="E3" s="335"/>
-      <c r="F3" s="335"/>
-      <c r="G3" s="335"/>
-      <c r="H3" s="335"/>
-      <c r="I3" s="335"/>
-      <c r="J3" s="335"/>
+      <c r="B3" s="341"/>
+      <c r="C3" s="341"/>
+      <c r="D3" s="341"/>
+      <c r="E3" s="341"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="341"/>
+      <c r="H3" s="341"/>
+      <c r="I3" s="341"/>
+      <c r="J3" s="341"/>
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="336"/>
-      <c r="B4" s="336"/>
-      <c r="C4" s="336"/>
-      <c r="D4" s="336"/>
-      <c r="E4" s="336"/>
-      <c r="F4" s="336"/>
-      <c r="G4" s="336"/>
-      <c r="H4" s="336"/>
-      <c r="I4" s="336"/>
-      <c r="J4" s="336"/>
-      <c r="K4" s="341" t="s">
+      <c r="A4" s="342"/>
+      <c r="B4" s="342"/>
+      <c r="C4" s="342"/>
+      <c r="D4" s="342"/>
+      <c r="E4" s="342"/>
+      <c r="F4" s="342"/>
+      <c r="G4" s="342"/>
+      <c r="H4" s="342"/>
+      <c r="I4" s="342"/>
+      <c r="J4" s="342"/>
+      <c r="K4" s="347" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="341"/>
-      <c r="M4" s="341"/>
-      <c r="N4" s="341"/>
+      <c r="L4" s="347"/>
+      <c r="M4" s="347"/>
+      <c r="N4" s="347"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
-      <c r="C5" s="337" t="s">
+      <c r="C5" s="343" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="338"/>
-      <c r="E5" s="338"/>
-      <c r="F5" s="338"/>
-      <c r="G5" s="338"/>
-      <c r="H5" s="338"/>
-      <c r="I5" s="338"/>
-      <c r="J5" s="339"/>
+      <c r="D5" s="344"/>
+      <c r="E5" s="344"/>
+      <c r="F5" s="344"/>
+      <c r="G5" s="344"/>
+      <c r="H5" s="344"/>
+      <c r="I5" s="344"/>
+      <c r="J5" s="345"/>
       <c r="K5" s="78"/>
-      <c r="L5" s="340" t="s">
+      <c r="L5" s="346" t="s">
         <v>107</v>
       </c>
-      <c r="M5" s="314"/>
-      <c r="N5" s="314"/>
+      <c r="M5" s="315"/>
+      <c r="N5" s="315"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="343">
+      <c r="C6" s="337">
         <v>2020</v>
       </c>
-      <c r="D6" s="344"/>
-      <c r="E6" s="344"/>
-      <c r="F6" s="344"/>
-      <c r="G6" s="344"/>
-      <c r="H6" s="344"/>
-      <c r="I6" s="344"/>
-      <c r="J6" s="345"/>
+      <c r="D6" s="338"/>
+      <c r="E6" s="338"/>
+      <c r="F6" s="338"/>
+      <c r="G6" s="338"/>
+      <c r="H6" s="338"/>
+      <c r="I6" s="338"/>
+      <c r="J6" s="339"/>
       <c r="K6" s="78" t="s">
         <v>135</v>
       </c>
@@ -15051,24 +15051,24 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="K22" s="314" t="s">
+      <c r="K22" s="315" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="314"/>
-      <c r="M22" s="314"/>
-      <c r="N22" s="314"/>
-      <c r="O22" s="314" t="s">
+      <c r="L22" s="315"/>
+      <c r="M22" s="315"/>
+      <c r="N22" s="315"/>
+      <c r="O22" s="315" t="s">
         <v>10</v>
       </c>
-      <c r="P22" s="314"/>
-      <c r="Q22" s="314"/>
-      <c r="R22" s="314"/>
-      <c r="S22" s="314" t="s">
+      <c r="P22" s="315"/>
+      <c r="Q22" s="315"/>
+      <c r="R22" s="315"/>
+      <c r="S22" s="315" t="s">
         <v>11</v>
       </c>
-      <c r="T22" s="314"/>
-      <c r="U22" s="314"/>
-      <c r="V22" s="314"/>
+      <c r="T22" s="315"/>
+      <c r="U22" s="315"/>
+      <c r="V22" s="315"/>
     </row>
     <row r="23" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C23" s="67"/>
@@ -15085,12 +15085,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="K23" s="346" t="s">
+      <c r="K23" s="340" t="s">
         <v>108</v>
       </c>
-      <c r="L23" s="346"/>
-      <c r="M23" s="346"/>
-      <c r="N23" s="346"/>
+      <c r="L23" s="340"/>
+      <c r="M23" s="340"/>
+      <c r="N23" s="340"/>
       <c r="O23" s="35" t="s">
         <v>146</v>
       </c>
@@ -15259,7 +15259,7 @@
       <c r="S27" s="72"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I28" s="342" t="s">
+      <c r="I28" s="336" t="s">
         <v>259</v>
       </c>
       <c r="J28" s="82" t="s">
@@ -15310,7 +15310,7 @@
       <c r="H29">
         <v>67</v>
       </c>
-      <c r="I29" s="342"/>
+      <c r="I29" s="336"/>
       <c r="J29" s="82" t="s">
         <v>143</v>
       </c>
@@ -15359,7 +15359,7 @@
         <f>H29</f>
         <v>67</v>
       </c>
-      <c r="I30" s="342"/>
+      <c r="I30" s="336"/>
       <c r="J30" s="82" t="s">
         <v>142</v>
       </c>
@@ -15408,7 +15408,7 @@
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="I31" s="342"/>
+      <c r="I31" s="336"/>
       <c r="J31" s="35" t="s">
         <v>140</v>
       </c>
@@ -15470,7 +15470,7 @@
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="I33" s="342" t="s">
+      <c r="I33" s="336" t="s">
         <v>141</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -15518,7 +15518,7 @@
       </c>
     </row>
     <row r="34" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I34" s="342"/>
+      <c r="I34" s="336"/>
       <c r="J34" t="s">
         <v>260</v>
       </c>
@@ -15697,6 +15697,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="K4:N4"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="I28:I31"/>
@@ -15704,12 +15710,6 @@
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K23:N23"/>
     <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -15817,30 +15817,30 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="350" t="s">
+      <c r="E6" s="349" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="350"/>
-      <c r="G6" s="350"/>
-      <c r="H6" s="350"/>
-      <c r="I6" s="350"/>
-      <c r="J6" s="350"/>
-      <c r="K6" s="350"/>
-      <c r="L6" s="350"/>
-      <c r="M6" s="350"/>
-      <c r="N6" s="350"/>
-      <c r="O6" s="350"/>
-      <c r="P6" s="350"/>
-      <c r="Q6" s="350"/>
-      <c r="R6" s="350"/>
+      <c r="F6" s="349"/>
+      <c r="G6" s="349"/>
+      <c r="H6" s="349"/>
+      <c r="I6" s="349"/>
+      <c r="J6" s="349"/>
+      <c r="K6" s="349"/>
+      <c r="L6" s="349"/>
+      <c r="M6" s="349"/>
+      <c r="N6" s="349"/>
+      <c r="O6" s="349"/>
+      <c r="P6" s="349"/>
+      <c r="Q6" s="349"/>
+      <c r="R6" s="349"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="347" t="s">
+      <c r="A7" s="348" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="347"/>
-      <c r="C7" s="347"/>
-      <c r="D7" s="347"/>
+      <c r="B7" s="348"/>
+      <c r="C7" s="348"/>
+      <c r="D7" s="348"/>
       <c r="E7" s="36"/>
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
@@ -15858,11 +15858,11 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="36"/>
-      <c r="B8" s="347" t="s">
+      <c r="B8" s="348" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="347"/>
-      <c r="D8" s="347"/>
+      <c r="C8" s="348"/>
+      <c r="D8" s="348"/>
       <c r="E8" s="42">
         <v>1717.857</v>
       </c>
@@ -15908,11 +15908,11 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="36"/>
-      <c r="B9" s="347" t="s">
+      <c r="B9" s="348" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="347"/>
-      <c r="D9" s="347"/>
+      <c r="C9" s="348"/>
+      <c r="D9" s="348"/>
       <c r="E9" s="42">
         <v>1243.3720000000001</v>
       </c>
@@ -15958,11 +15958,11 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="36"/>
-      <c r="B10" s="347" t="s">
+      <c r="B10" s="348" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="347"/>
-      <c r="D10" s="347"/>
+      <c r="C10" s="348"/>
+      <c r="D10" s="348"/>
       <c r="E10" s="42">
         <v>230.245</v>
       </c>
@@ -16008,11 +16008,11 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="36"/>
-      <c r="B11" s="347" t="s">
+      <c r="B11" s="348" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="347"/>
-      <c r="D11" s="347"/>
+      <c r="C11" s="348"/>
+      <c r="D11" s="348"/>
       <c r="E11" s="42">
         <v>271.327</v>
       </c>
@@ -16107,10 +16107,10 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="36"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="347" t="s">
+      <c r="C13" s="348" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="347"/>
+      <c r="D13" s="348"/>
       <c r="E13" s="42">
         <v>3462.8009999999999</v>
       </c>
@@ -16261,11 +16261,11 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
-      <c r="B19" s="347" t="s">
+      <c r="B19" s="348" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="347"/>
-      <c r="D19" s="347"/>
+      <c r="C19" s="348"/>
+      <c r="D19" s="348"/>
       <c r="E19" s="42">
         <v>1717.857</v>
       </c>
@@ -16324,11 +16324,11 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="36"/>
-      <c r="B20" s="347" t="s">
+      <c r="B20" s="348" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="347"/>
-      <c r="D20" s="347"/>
+      <c r="C20" s="348"/>
+      <c r="D20" s="348"/>
       <c r="E20" s="42">
         <v>1243.3720000000001</v>
       </c>
@@ -16388,11 +16388,11 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="36"/>
-      <c r="B21" s="347" t="s">
+      <c r="B21" s="348" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="347"/>
-      <c r="D21" s="347"/>
+      <c r="C21" s="348"/>
+      <c r="D21" s="348"/>
       <c r="E21" s="42">
         <v>230.245</v>
       </c>
@@ -16451,11 +16451,11 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="36"/>
-      <c r="B22" s="347" t="s">
+      <c r="B22" s="348" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="347"/>
-      <c r="D22" s="347"/>
+      <c r="C22" s="348"/>
+      <c r="D22" s="348"/>
       <c r="E22" s="42">
         <v>271.327</v>
       </c>
@@ -16568,21 +16568,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="348" t="s">
+      <c r="H27" s="350" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="348"/>
-      <c r="J27" s="348"/>
-      <c r="K27" s="348"/>
-      <c r="L27" s="348"/>
-      <c r="M27" s="348"/>
-      <c r="N27" s="348"/>
-      <c r="O27" s="348"/>
-      <c r="P27" s="348"/>
-      <c r="Q27" s="348"/>
-      <c r="R27" s="348"/>
-      <c r="S27" s="348"/>
-      <c r="T27" s="348"/>
+      <c r="I27" s="350"/>
+      <c r="J27" s="350"/>
+      <c r="K27" s="350"/>
+      <c r="L27" s="350"/>
+      <c r="M27" s="350"/>
+      <c r="N27" s="350"/>
+      <c r="O27" s="350"/>
+      <c r="P27" s="350"/>
+      <c r="Q27" s="350"/>
+      <c r="R27" s="350"/>
+      <c r="S27" s="350"/>
+      <c r="T27" s="350"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
@@ -16898,21 +16898,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="349" t="s">
+      <c r="F37" s="351" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="349"/>
-      <c r="H37" s="349"/>
-      <c r="I37" s="349"/>
-      <c r="J37" s="349"/>
-      <c r="K37" s="349"/>
-      <c r="L37" s="349"/>
-      <c r="M37" s="349"/>
-      <c r="N37" s="349"/>
-      <c r="O37" s="349"/>
-      <c r="P37" s="349"/>
-      <c r="Q37" s="349"/>
-      <c r="R37" s="349"/>
+      <c r="G37" s="351"/>
+      <c r="H37" s="351"/>
+      <c r="I37" s="351"/>
+      <c r="J37" s="351"/>
+      <c r="K37" s="351"/>
+      <c r="L37" s="351"/>
+      <c r="M37" s="351"/>
+      <c r="N37" s="351"/>
+      <c r="O37" s="351"/>
+      <c r="P37" s="351"/>
+      <c r="Q37" s="351"/>
+      <c r="R37" s="351"/>
     </row>
     <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
@@ -17228,21 +17228,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="348" t="s">
+      <c r="F48" s="350" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="348"/>
-      <c r="H48" s="348"/>
-      <c r="I48" s="348"/>
-      <c r="J48" s="348"/>
-      <c r="K48" s="348"/>
-      <c r="L48" s="348"/>
-      <c r="M48" s="348"/>
-      <c r="N48" s="348"/>
-      <c r="O48" s="348"/>
-      <c r="P48" s="348"/>
-      <c r="Q48" s="348"/>
-      <c r="R48" s="348"/>
+      <c r="G48" s="350"/>
+      <c r="H48" s="350"/>
+      <c r="I48" s="350"/>
+      <c r="J48" s="350"/>
+      <c r="K48" s="350"/>
+      <c r="L48" s="350"/>
+      <c r="M48" s="350"/>
+      <c r="N48" s="350"/>
+      <c r="O48" s="350"/>
+      <c r="P48" s="350"/>
+      <c r="Q48" s="350"/>
+      <c r="R48" s="350"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
@@ -17554,12 +17554,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -17568,6 +17562,12 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17606,50 +17606,50 @@
     <row r="3" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="328" t="s">
+      <c r="A5" s="329" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="329"/>
-      <c r="C5" s="329"/>
-      <c r="D5" s="329"/>
-      <c r="E5" s="329"/>
-      <c r="F5" s="329"/>
-      <c r="G5" s="329"/>
-      <c r="H5" s="329"/>
-      <c r="I5" s="329"/>
-      <c r="J5" s="329"/>
-      <c r="K5" s="329"/>
-      <c r="L5" s="329"/>
-      <c r="M5" s="329"/>
-      <c r="N5" s="329"/>
-      <c r="O5" s="329"/>
-      <c r="P5" s="329"/>
-      <c r="Q5" s="329"/>
-      <c r="R5" s="329"/>
-      <c r="S5" s="329"/>
+      <c r="B5" s="330"/>
+      <c r="C5" s="330"/>
+      <c r="D5" s="330"/>
+      <c r="E5" s="330"/>
+      <c r="F5" s="330"/>
+      <c r="G5" s="330"/>
+      <c r="H5" s="330"/>
+      <c r="I5" s="330"/>
+      <c r="J5" s="330"/>
+      <c r="K5" s="330"/>
+      <c r="L5" s="330"/>
+      <c r="M5" s="330"/>
+      <c r="N5" s="330"/>
+      <c r="O5" s="330"/>
+      <c r="P5" s="330"/>
+      <c r="Q5" s="330"/>
+      <c r="R5" s="330"/>
+      <c r="S5" s="330"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="330" t="s">
+      <c r="A6" s="331" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="330"/>
-      <c r="C6" s="330"/>
-      <c r="D6" s="330"/>
-      <c r="E6" s="330"/>
-      <c r="F6" s="330"/>
-      <c r="G6" s="330"/>
-      <c r="H6" s="330"/>
-      <c r="I6" s="330"/>
-      <c r="J6" s="330"/>
-      <c r="K6" s="330"/>
-      <c r="L6" s="330"/>
-      <c r="M6" s="330"/>
-      <c r="N6" s="330"/>
-      <c r="O6" s="330"/>
-      <c r="P6" s="330"/>
-      <c r="Q6" s="330"/>
-      <c r="R6" s="330"/>
-      <c r="S6" s="330"/>
+      <c r="B6" s="331"/>
+      <c r="C6" s="331"/>
+      <c r="D6" s="331"/>
+      <c r="E6" s="331"/>
+      <c r="F6" s="331"/>
+      <c r="G6" s="331"/>
+      <c r="H6" s="331"/>
+      <c r="I6" s="331"/>
+      <c r="J6" s="331"/>
+      <c r="K6" s="331"/>
+      <c r="L6" s="331"/>
+      <c r="M6" s="331"/>
+      <c r="N6" s="331"/>
+      <c r="O6" s="331"/>
+      <c r="P6" s="331"/>
+      <c r="Q6" s="331"/>
+      <c r="R6" s="331"/>
+      <c r="S6" s="331"/>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9"/>
@@ -17689,10 +17689,10 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="331" t="s">
+      <c r="R8" s="332" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="332"/>
+      <c r="S8" s="333"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
@@ -20563,10 +20563,10 @@
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
-      <c r="D75" s="351" t="s">
+      <c r="D75" s="352" t="s">
         <v>42</v>
       </c>
-      <c r="E75" s="352"/>
+      <c r="E75" s="353"/>
       <c r="F75" s="25">
         <v>-75.135000000000005</v>
       </c>
@@ -21514,10 +21514,10 @@
   <dimension ref="A1:AF76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="8" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21536,23 +21536,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="320" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="320"/>
+      <c r="B1" s="321"/>
       <c r="C1" s="35"/>
       <c r="H1"/>
       <c r="I1" s="250"/>
-      <c r="J1" s="327" t="s">
+      <c r="J1" s="328" t="s">
         <v>282</v>
       </c>
-      <c r="V1" s="314"/>
-      <c r="W1" s="314"/>
-      <c r="X1" s="314"/>
-      <c r="Y1" s="314"/>
+      <c r="V1" s="315"/>
+      <c r="W1" s="315"/>
+      <c r="X1" s="315"/>
+      <c r="Y1" s="315"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="321" t="s">
+      <c r="A2" s="322" t="s">
         <v>192</v>
       </c>
       <c r="B2" s="126"/>
@@ -21560,68 +21560,68 @@
         <v>193</v>
       </c>
       <c r="I2" s="251"/>
-      <c r="J2" s="327"/>
+      <c r="J2" s="328"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="322"/>
+      <c r="A3" s="323"/>
       <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
       <c r="I3" s="251"/>
-      <c r="J3" s="327"/>
+      <c r="J3" s="328"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="322"/>
+      <c r="A4" s="323"/>
       <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="323"/>
+      <c r="A5" s="324"/>
       <c r="B5" s="129"/>
       <c r="C5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="C7" s="324" t="s">
+      <c r="C7" s="325" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="325"/>
-      <c r="E7" s="325"/>
-      <c r="F7" s="326"/>
-      <c r="G7" s="324" t="s">
+      <c r="D7" s="326"/>
+      <c r="E7" s="326"/>
+      <c r="F7" s="327"/>
+      <c r="G7" s="325" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="325"/>
-      <c r="I7" s="325"/>
-      <c r="J7" s="326"/>
-      <c r="K7" s="324" t="s">
+      <c r="H7" s="326"/>
+      <c r="I7" s="326"/>
+      <c r="J7" s="327"/>
+      <c r="K7" s="325" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="325"/>
-      <c r="M7" s="325"/>
-      <c r="N7" s="325"/>
-      <c r="O7" s="324" t="s">
+      <c r="L7" s="326"/>
+      <c r="M7" s="326"/>
+      <c r="N7" s="326"/>
+      <c r="O7" s="325" t="s">
         <v>272</v>
       </c>
-      <c r="P7" s="325"/>
-      <c r="Q7" s="325"/>
-      <c r="R7" s="325"/>
-      <c r="S7" s="324" t="s">
+      <c r="P7" s="326"/>
+      <c r="Q7" s="326"/>
+      <c r="R7" s="326"/>
+      <c r="S7" s="325" t="s">
         <v>276</v>
       </c>
-      <c r="T7" s="325"/>
-      <c r="U7" s="325"/>
-      <c r="V7" s="325"/>
-      <c r="W7" s="324" t="s">
+      <c r="T7" s="326"/>
+      <c r="U7" s="326"/>
+      <c r="V7" s="326"/>
+      <c r="W7" s="325" t="s">
         <v>277</v>
       </c>
-      <c r="X7" s="325"/>
-      <c r="Y7" s="325"/>
-      <c r="Z7" s="325"/>
+      <c r="X7" s="326"/>
+      <c r="Y7" s="326"/>
+      <c r="Z7" s="326"/>
       <c r="AA7" s="231" t="s">
         <v>278</v>
       </c>
@@ -21816,70 +21816,70 @@
         <v>370.81066666666698</v>
       </c>
       <c r="F11">
-        <v>881.93300000000011</v>
+        <v>143.73299999999989</v>
       </c>
       <c r="G11">
-        <v>891.98651810076751</v>
+        <v>119.7103015934359</v>
       </c>
       <c r="H11">
-        <v>891.27501716779318</v>
+        <v>95.692774643121879</v>
       </c>
       <c r="I11">
-        <v>892.48838718787158</v>
+        <v>71.680432077698356</v>
       </c>
       <c r="J11">
-        <v>887.49939524811271</v>
+        <v>49.757422545121358</v>
       </c>
       <c r="K11">
-        <v>912.80995474617953</v>
+        <v>63.885229528435843</v>
       </c>
       <c r="L11">
-        <v>939.90280216374003</v>
+        <v>80.170429568141572</v>
       </c>
       <c r="M11">
-        <v>965.78369379604453</v>
+        <v>96.995101270948112</v>
       </c>
       <c r="N11">
-        <v>989.88229750885569</v>
+        <v>112.932368446504</v>
       </c>
       <c r="O11">
-        <v>1011.979044291314</v>
+        <v>127.8342527553297</v>
       </c>
       <c r="P11">
-        <v>1033.576750456315</v>
+        <v>142.4876637965252</v>
       </c>
       <c r="Q11">
-        <v>1056.7428699904699</v>
+        <v>157.92199082170151</v>
       </c>
       <c r="R11">
-        <v>1079.766406491065</v>
+        <v>173.28532548469749</v>
       </c>
       <c r="S11">
-        <v>1086.988730126506</v>
+        <v>172.77585661115961</v>
       </c>
       <c r="T11">
-        <v>1095.0665519633039</v>
+        <v>172.69234191070231</v>
       </c>
       <c r="U11">
-        <v>1103.9285804846791</v>
+        <v>172.999285202235</v>
       </c>
       <c r="V11">
-        <v>1113.93127327453</v>
+        <v>173.8741673912084</v>
       </c>
       <c r="W11">
-        <v>1121.9665712579019</v>
+        <v>172.67426876663441</v>
       </c>
       <c r="X11">
-        <v>1129.859286207716</v>
+        <v>171.4033777798804</v>
       </c>
       <c r="Y11">
-        <v>1138.3223332917671</v>
+        <v>170.41645624184639</v>
       </c>
       <c r="Z11">
-        <v>1147.4270040268359</v>
+        <v>169.74900033362289</v>
       </c>
       <c r="AA11">
-        <v>1156.681516820131</v>
+        <v>168.94502379810791</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
@@ -22201,70 +22201,70 @@
         <v>3763.7893333333341</v>
       </c>
       <c r="F16">
-        <v>1915.067</v>
+        <v>2653.2669999999998</v>
       </c>
       <c r="G16">
-        <v>1653.243063736659</v>
+        <v>2317.9343666284731</v>
       </c>
       <c r="H16">
-        <v>1447.6763216952199</v>
+        <v>2053.9178721883209</v>
       </c>
       <c r="I16">
-        <v>1282.6115778747101</v>
+        <v>1841.244964503114</v>
       </c>
       <c r="J16">
-        <v>1168.218036502012</v>
+        <v>1692.806943814478</v>
       </c>
       <c r="K16">
-        <v>1196.0977521572081</v>
+        <v>1738.8476760207</v>
       </c>
       <c r="L16">
-        <v>1201.420957574891</v>
+        <v>1756.293963726893</v>
       </c>
       <c r="M16">
-        <v>1192.398092607149</v>
+        <v>1755.5540200918881</v>
       </c>
       <c r="N16">
-        <v>1163.510521947278</v>
+        <v>1729.6319796501559</v>
       </c>
       <c r="O16">
-        <v>1162.952327464749</v>
+        <v>1731.529779708525</v>
       </c>
       <c r="P16">
-        <v>1163.223418033522</v>
+        <v>1734.478848120219</v>
       </c>
       <c r="Q16">
-        <v>1164.061655925231</v>
+        <v>1738.1468780413959</v>
       </c>
       <c r="R16">
-        <v>1166.5248859901251</v>
+        <v>1743.874878588342</v>
       </c>
       <c r="S16">
-        <v>1179.2527801172971</v>
+        <v>1761.5240430940889</v>
       </c>
       <c r="T16">
-        <v>1191.4351178432501</v>
+        <v>1778.481616477271</v>
       </c>
       <c r="U16">
-        <v>1201.0737372062879</v>
+        <v>1792.214568108853</v>
       </c>
       <c r="V16">
-        <v>1209.153135236118</v>
+        <v>1803.970925515257</v>
       </c>
       <c r="W16">
-        <v>1235.6991953270949</v>
+        <v>1845.574035042185</v>
       </c>
       <c r="X16">
-        <v>1257.112926395658</v>
+        <v>1880.670991984249</v>
       </c>
       <c r="Y16">
-        <v>1273.980106203785</v>
+        <v>1910.0043752921761</v>
       </c>
       <c r="Z16">
-        <v>1285.81146007862</v>
+        <v>1932.953941083782</v>
       </c>
       <c r="AA16">
-        <v>1291.320506480959</v>
+        <v>1945.2974943481329</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
@@ -23097,63 +23097,63 @@
       </c>
       <c r="M31" s="104">
         <f>L31*(1 + M33)</f>
-        <v>196.196936733694</v>
+        <v>231.01005759196664</v>
       </c>
       <c r="N31" s="104">
         <f t="shared" ref="N31:AA31" si="22">M31*(1 + N33)</f>
-        <v>201.09251765764702</v>
+        <v>268.96732512240902</v>
       </c>
       <c r="O31" s="104">
         <f t="shared" si="22"/>
-        <v>205.5814255345841</v>
+        <v>304.45865517210234</v>
       </c>
       <c r="P31" s="104">
         <f t="shared" si="22"/>
-        <v>209.96895435420245</v>
+        <v>339.35820457397739</v>
       </c>
       <c r="Q31" s="104">
         <f t="shared" si="22"/>
-        <v>214.67510306825145</v>
+        <v>376.11763601185311</v>
       </c>
       <c r="R31" s="104">
         <f t="shared" si="22"/>
-        <v>219.35228633735218</v>
+        <v>412.70798726463727</v>
       </c>
       <c r="S31" s="104">
         <f t="shared" si="22"/>
-        <v>220.8194862729851</v>
+        <v>411.49460192584024</v>
       </c>
       <c r="T31" s="104">
         <f t="shared" si="22"/>
-        <v>222.46047887830755</v>
+        <v>411.29569769758933</v>
       </c>
       <c r="U31" s="104">
         <f t="shared" si="22"/>
-        <v>224.26078143084538</v>
+        <v>412.02673448733771</v>
       </c>
       <c r="V31" s="104">
         <f t="shared" si="22"/>
-        <v>226.2928075429692</v>
+        <v>414.11041275781412</v>
       </c>
       <c r="W31" s="104">
         <f t="shared" si="22"/>
-        <v>227.92516151643866</v>
+        <v>411.25265348198167</v>
       </c>
       <c r="X31" s="104">
         <f t="shared" si="22"/>
-        <v>229.52855004496021</v>
+        <v>408.2258140210584</v>
       </c>
       <c r="Y31" s="104">
         <f t="shared" si="22"/>
-        <v>231.24780035327461</v>
+        <v>405.87529530049824</v>
       </c>
       <c r="Z31" s="104">
         <f t="shared" si="22"/>
-        <v>233.09739516385611</v>
+        <v>404.28563741284785</v>
       </c>
       <c r="AA31" s="104">
         <f t="shared" si="22"/>
-        <v>234.97743007505923</v>
+        <v>402.37083281613849</v>
       </c>
       <c r="AB31" s="95"/>
     </row>
@@ -23171,91 +23171,91 @@
       </c>
       <c r="F32" s="104">
         <f t="shared" si="23"/>
-        <v>881.93300000000011</v>
+        <v>143.73299999999989</v>
       </c>
       <c r="G32" s="149">
         <f t="shared" si="23"/>
-        <v>891.98651810076751</v>
+        <v>119.7103015934359</v>
       </c>
       <c r="H32" s="104">
         <f t="shared" si="23"/>
-        <v>891.27501716779318</v>
+        <v>95.692774643121879</v>
       </c>
       <c r="I32" s="104">
         <f t="shared" si="23"/>
-        <v>892.48838718787158</v>
+        <v>71.680432077698356</v>
       </c>
       <c r="J32" s="104">
         <f t="shared" si="23"/>
-        <v>887.49939524811271</v>
+        <v>49.757422545121358</v>
       </c>
       <c r="K32" s="149">
         <f t="shared" si="23"/>
-        <v>912.80995474617953</v>
+        <v>63.885229528435843</v>
       </c>
       <c r="L32" s="232">
         <f t="shared" si="23"/>
-        <v>939.90280216374003</v>
+        <v>80.170429568141572</v>
       </c>
       <c r="M32" s="104">
         <f t="shared" si="23"/>
-        <v>965.78369379604453</v>
+        <v>96.995101270948112</v>
       </c>
       <c r="N32" s="104">
         <f t="shared" si="23"/>
-        <v>989.88229750885569</v>
+        <v>112.932368446504</v>
       </c>
       <c r="O32" s="149">
         <f t="shared" si="23"/>
-        <v>1011.979044291314</v>
+        <v>127.8342527553297</v>
       </c>
       <c r="P32" s="104">
         <f t="shared" si="23"/>
-        <v>1033.576750456315</v>
+        <v>142.4876637965252</v>
       </c>
       <c r="Q32" s="104">
         <f t="shared" si="23"/>
-        <v>1056.7428699904699</v>
+        <v>157.92199082170151</v>
       </c>
       <c r="R32" s="104">
         <f t="shared" si="23"/>
-        <v>1079.766406491065</v>
+        <v>173.28532548469749</v>
       </c>
       <c r="S32" s="149">
         <f t="shared" si="23"/>
-        <v>1086.988730126506</v>
+        <v>172.77585661115961</v>
       </c>
       <c r="T32" s="104">
         <f t="shared" si="23"/>
-        <v>1095.0665519633039</v>
+        <v>172.69234191070231</v>
       </c>
       <c r="U32" s="104">
         <f t="shared" si="23"/>
-        <v>1103.9285804846791</v>
+        <v>172.999285202235</v>
       </c>
       <c r="V32" s="104">
         <f t="shared" si="23"/>
-        <v>1113.93127327453</v>
+        <v>173.8741673912084</v>
       </c>
       <c r="W32" s="149">
         <f t="shared" si="23"/>
-        <v>1121.9665712579019</v>
+        <v>172.67426876663441</v>
       </c>
       <c r="X32" s="104">
         <f t="shared" si="23"/>
-        <v>1129.859286207716</v>
+        <v>171.4033777798804</v>
       </c>
       <c r="Y32" s="104">
         <f t="shared" si="23"/>
-        <v>1138.3223332917671</v>
+        <v>170.41645624184639</v>
       </c>
       <c r="Z32" s="104">
         <f t="shared" si="23"/>
-        <v>1147.4270040268359</v>
+        <v>169.74900033362289</v>
       </c>
       <c r="AA32" s="149">
         <f t="shared" si="23"/>
-        <v>1156.681516820131</v>
+        <v>168.94502379810791</v>
       </c>
       <c r="AB32" s="95"/>
     </row>
@@ -23274,63 +23274,63 @@
       <c r="L33" s="239"/>
       <c r="M33" s="239">
         <f t="shared" ref="M33" si="24">(M32/L32)-1</f>
-        <v>2.7535710684896797E-2</v>
+        <v>0.20986131412089115</v>
       </c>
       <c r="N33" s="239">
         <f t="shared" ref="N33" si="25">(N32/M32)-1</f>
-        <v>2.4952382057819689E-2</v>
+        <v>0.16431002150342011</v>
       </c>
       <c r="O33" s="256">
         <f t="shared" ref="O33" si="26">(O32/N32)-1</f>
-        <v>2.232260021021415E-2</v>
+        <v>0.13195405811297323</v>
       </c>
       <c r="P33" s="239">
         <f t="shared" ref="P33" si="27">(P32/O32)-1</f>
-        <v>2.1342048816955339E-2</v>
+        <v>0.11462820586311562</v>
       </c>
       <c r="Q33" s="239">
         <f t="shared" ref="Q33" si="28">(Q32/P32)-1</f>
-        <v>2.2413545509733179E-2</v>
+        <v>0.10832044412782849</v>
       </c>
       <c r="R33" s="239">
         <f t="shared" ref="R33" si="29">(R32/Q32)-1</f>
-        <v>2.1787264579133492E-2</v>
+        <v>9.7284327426834682E-2</v>
       </c>
       <c r="S33" s="256">
         <f t="shared" ref="S33" si="30">(S32/R32)-1</f>
-        <v>6.6887834183613215E-3</v>
+        <v>-2.940057804161067E-3</v>
       </c>
       <c r="T33" s="239">
         <f t="shared" ref="T33" si="31">(T32/S32)-1</f>
-        <v>7.4313758854316347E-3</v>
+        <v>-4.8337020053246249E-4</v>
       </c>
       <c r="U33" s="239">
         <f t="shared" ref="U33" si="32">(U32/T32)-1</f>
-        <v>8.0926848742541857E-3</v>
+        <v>1.7773995542396115E-3</v>
       </c>
       <c r="V33" s="239">
         <f t="shared" ref="V33" si="33">(V32/U32)-1</f>
-        <v>9.0609963059922194E-3</v>
+        <v>5.0571433746138261E-3</v>
       </c>
       <c r="W33" s="256">
         <f t="shared" ref="W33" si="34">(W32/V32)-1</f>
-        <v>7.2134593723642837E-3</v>
+        <v>-6.9009597145864854E-3</v>
       </c>
       <c r="X33" s="239">
         <f t="shared" ref="X33" si="35">(X32/W32)-1</f>
-        <v>7.0347148943707971E-3</v>
+        <v>-7.3600484648445041E-3</v>
       </c>
       <c r="Y33" s="239">
         <f t="shared" ref="Y33" si="36">(Y32/X32)-1</f>
-        <v>7.4903549383187329E-3</v>
+        <v>-5.7578885014823999E-3</v>
       </c>
       <c r="Z33" s="239">
         <f t="shared" ref="Z33" si="37">(Z32/Y32)-1</f>
-        <v>7.9983239094854053E-3</v>
+        <v>-3.9166165225046345E-3</v>
       </c>
       <c r="AA33" s="256">
         <f t="shared" ref="AA33" si="38">(AA32/Z32)-1</f>
-        <v>8.0654479638502252E-3</v>
+        <v>-4.736266687490609E-3</v>
       </c>
       <c r="AB33" s="253"/>
     </row>
@@ -23342,91 +23342,91 @@
       <c r="E34" s="225"/>
       <c r="F34" s="225">
         <f t="shared" ref="F34" si="39">F31-F32</f>
-        <v>-597.15600000000018</v>
+        <v>141.0440000000001</v>
       </c>
       <c r="G34" s="150">
         <f t="shared" ref="G34" si="40">G31-G32</f>
-        <v>-669.01923060076751</v>
+        <v>103.25698590656407</v>
       </c>
       <c r="H34" s="225">
         <f t="shared" ref="H34" si="41">H31-H32</f>
-        <v>-687.95031144904317</v>
+        <v>107.63193107562813</v>
       </c>
       <c r="I34" s="225">
         <f t="shared" ref="I34" si="42">I31-I32</f>
-        <v>-704.80536970482467</v>
+        <v>116.0025854053485</v>
       </c>
       <c r="J34" s="225">
         <f t="shared" ref="J34" si="43">J31-J32</f>
-        <v>-699.09796267765057</v>
+        <v>138.64401002534075</v>
       </c>
       <c r="K34" s="150">
         <f t="shared" ref="K34:N34" si="44">K31-K32</f>
-        <v>-723.32551143143894</v>
+        <v>125.59921378630472</v>
       </c>
       <c r="L34" s="249">
         <f t="shared" si="44"/>
-        <v>-748.96351441585216</v>
+        <v>110.76885817974633</v>
       </c>
       <c r="M34" s="225">
         <f t="shared" si="44"/>
-        <v>-769.58675706235056</v>
+        <v>134.01495632101853</v>
       </c>
       <c r="N34" s="225">
         <f t="shared" si="44"/>
-        <v>-788.78977985120866</v>
+        <v>156.03495667590502</v>
       </c>
       <c r="O34" s="150">
         <f t="shared" ref="O34:AA34" si="45">O31-O32</f>
-        <v>-806.39761875672991</v>
+        <v>176.62440241677263</v>
       </c>
       <c r="P34" s="150">
         <f t="shared" si="45"/>
-        <v>-823.60779610211262</v>
+        <v>196.87054077745219</v>
       </c>
       <c r="Q34" s="150">
         <f t="shared" si="45"/>
-        <v>-842.06776692221842</v>
+        <v>218.19564519015159</v>
       </c>
       <c r="R34" s="150">
         <f t="shared" si="45"/>
-        <v>-860.41412015371282</v>
+        <v>239.42266177993977</v>
       </c>
       <c r="S34" s="150">
         <f t="shared" si="45"/>
-        <v>-866.16924385352081</v>
+        <v>238.71874531468063</v>
       </c>
       <c r="T34" s="150">
         <f t="shared" si="45"/>
-        <v>-872.60607308499641</v>
+        <v>238.60335578688702</v>
       </c>
       <c r="U34" s="150">
         <f t="shared" si="45"/>
-        <v>-879.66779905383373</v>
+        <v>239.0274492851027</v>
       </c>
       <c r="V34" s="150">
         <f t="shared" si="45"/>
-        <v>-887.63846573156081</v>
+        <v>240.23624536660571</v>
       </c>
       <c r="W34" s="150">
         <f t="shared" si="45"/>
-        <v>-894.04140974146321</v>
+        <v>238.57838471534725</v>
       </c>
       <c r="X34" s="150">
         <f t="shared" si="45"/>
-        <v>-900.33073616275578</v>
+        <v>236.822436241178</v>
       </c>
       <c r="Y34" s="150">
         <f t="shared" si="45"/>
-        <v>-907.07453293849244</v>
+        <v>235.45883905865185</v>
       </c>
       <c r="Z34" s="150">
         <f t="shared" si="45"/>
-        <v>-914.32960886297974</v>
+        <v>234.53663707922496</v>
       </c>
       <c r="AA34" s="150">
         <f t="shared" si="45"/>
-        <v>-921.70408674507178</v>
+        <v>233.42580901803058</v>
       </c>
       <c r="AB34" s="254"/>
     </row>
@@ -24504,67 +24504,67 @@
       </c>
       <c r="L57" s="104">
         <f>K57*(1+L59)</f>
-        <v>1671.9798691013036</v>
+        <v>1681.2727898882304</v>
       </c>
       <c r="M57" s="104">
         <f t="shared" ref="M57:AA57" si="75">L57*(1+M59)</f>
-        <v>1659.4230308902108</v>
+        <v>1680.5644533994202</v>
       </c>
       <c r="N57" s="104">
         <f t="shared" si="75"/>
-        <v>1619.2211047409951</v>
+        <v>1655.7496888137784</v>
       </c>
       <c r="O57" s="104">
         <f t="shared" si="75"/>
-        <v>1618.4442829851005</v>
+        <v>1657.566423178687</v>
       </c>
       <c r="P57" s="104">
         <f t="shared" si="75"/>
-        <v>1618.8215512280372</v>
+        <v>1660.3895203244397</v>
       </c>
       <c r="Q57" s="104">
         <f t="shared" si="75"/>
-        <v>1619.9881006140947</v>
+        <v>1663.9008680978411</v>
       </c>
       <c r="R57" s="104">
         <f t="shared" si="75"/>
-        <v>1623.4161006464742</v>
+        <v>1669.3841935883013</v>
       </c>
       <c r="S57" s="104">
         <f t="shared" si="75"/>
-        <v>1641.1291117459646</v>
+        <v>1686.2794632075206</v>
       </c>
       <c r="T57" s="104">
         <f t="shared" si="75"/>
-        <v>1658.0828891109786</v>
+        <v>1702.5126834431453</v>
       </c>
       <c r="U57" s="104">
         <f t="shared" si="75"/>
-        <v>1671.496653403437</v>
+        <v>1715.659023623029</v>
       </c>
       <c r="V57" s="104">
         <f t="shared" si="75"/>
-        <v>1682.7404982649418</v>
+        <v>1726.9132010123569</v>
       </c>
       <c r="W57" s="104">
         <f t="shared" si="75"/>
-        <v>1719.6838175871369</v>
+        <v>1766.739208199637</v>
       </c>
       <c r="X57" s="104">
         <f t="shared" si="75"/>
-        <v>1749.4846355629252</v>
+        <v>1800.3369771000982</v>
       </c>
       <c r="Y57" s="104">
         <f t="shared" si="75"/>
-        <v>1772.9581607331754</v>
+        <v>1828.4173669491454</v>
       </c>
       <c r="Z57" s="104">
         <f t="shared" si="75"/>
-        <v>1789.4234848797325</v>
+        <v>1850.3866279624326</v>
       </c>
       <c r="AA57" s="104">
         <f t="shared" si="75"/>
-        <v>1797.0902519896126</v>
+        <v>1862.2029187784933</v>
       </c>
       <c r="AB57" s="95"/>
     </row>
@@ -24582,91 +24582,91 @@
       </c>
       <c r="F58" s="104">
         <f t="shared" si="76"/>
-        <v>1915.067</v>
+        <v>2653.2669999999998</v>
       </c>
       <c r="G58" s="149">
         <f t="shared" si="76"/>
-        <v>1653.243063736659</v>
+        <v>2317.9343666284731</v>
       </c>
       <c r="H58" s="104">
         <f t="shared" si="76"/>
-        <v>1447.6763216952199</v>
+        <v>2053.9178721883209</v>
       </c>
       <c r="I58" s="104">
         <f t="shared" si="76"/>
-        <v>1282.6115778747101</v>
+        <v>1841.244964503114</v>
       </c>
       <c r="J58" s="104">
         <f t="shared" si="76"/>
-        <v>1168.218036502012</v>
+        <v>1692.806943814478</v>
       </c>
       <c r="K58" s="274">
         <f t="shared" si="76"/>
-        <v>1196.0977521572081</v>
+        <v>1738.8476760207</v>
       </c>
       <c r="L58" s="104">
         <f t="shared" si="76"/>
-        <v>1201.420957574891</v>
+        <v>1756.293963726893</v>
       </c>
       <c r="M58" s="104">
         <f t="shared" si="76"/>
-        <v>1192.398092607149</v>
+        <v>1755.5540200918881</v>
       </c>
       <c r="N58" s="104">
         <f t="shared" si="76"/>
-        <v>1163.510521947278</v>
+        <v>1729.6319796501559</v>
       </c>
       <c r="O58" s="149">
         <f t="shared" si="76"/>
-        <v>1162.952327464749</v>
+        <v>1731.529779708525</v>
       </c>
       <c r="P58" s="104">
         <f t="shared" si="76"/>
-        <v>1163.223418033522</v>
+        <v>1734.478848120219</v>
       </c>
       <c r="Q58" s="104">
         <f t="shared" si="76"/>
-        <v>1164.061655925231</v>
+        <v>1738.1468780413959</v>
       </c>
       <c r="R58" s="104">
         <f t="shared" si="76"/>
-        <v>1166.5248859901251</v>
+        <v>1743.874878588342</v>
       </c>
       <c r="S58" s="149">
         <f t="shared" si="76"/>
-        <v>1179.2527801172971</v>
+        <v>1761.5240430940889</v>
       </c>
       <c r="T58" s="104">
         <f t="shared" si="76"/>
-        <v>1191.4351178432501</v>
+        <v>1778.481616477271</v>
       </c>
       <c r="U58" s="104">
         <f t="shared" si="76"/>
-        <v>1201.0737372062879</v>
+        <v>1792.214568108853</v>
       </c>
       <c r="V58" s="104">
         <f t="shared" si="76"/>
-        <v>1209.153135236118</v>
+        <v>1803.970925515257</v>
       </c>
       <c r="W58" s="149">
         <f t="shared" si="76"/>
-        <v>1235.6991953270949</v>
+        <v>1845.574035042185</v>
       </c>
       <c r="X58" s="104">
         <f t="shared" si="76"/>
-        <v>1257.112926395658</v>
+        <v>1880.670991984249</v>
       </c>
       <c r="Y58" s="104">
         <f t="shared" si="76"/>
-        <v>1273.980106203785</v>
+        <v>1910.0043752921761</v>
       </c>
       <c r="Z58" s="104">
         <f t="shared" si="76"/>
-        <v>1285.81146007862</v>
+        <v>1932.953941083782</v>
       </c>
       <c r="AA58" s="149">
         <f t="shared" si="76"/>
-        <v>1291.320506480959</v>
+        <v>1945.2974943481329</v>
       </c>
       <c r="AB58" s="95"/>
     </row>
@@ -24684,67 +24684,67 @@
       <c r="K59" s="256"/>
       <c r="L59" s="239">
         <f t="shared" ref="L59" si="77">(L58/K58)-1</f>
-        <v>4.4504769013087309E-3</v>
+        <v>1.0033246699399534E-2</v>
       </c>
       <c r="M59" s="239">
         <f t="shared" ref="M59" si="78">(M58/L58)-1</f>
-        <v>-7.5101611228381993E-3</v>
+        <v>-4.2130967268982911E-4</v>
       </c>
       <c r="N59" s="239">
         <f t="shared" ref="N59" si="79">(N58/M58)-1</f>
-        <v>-2.4226448229809794E-2</v>
+        <v>-1.4765732153531497E-2</v>
       </c>
       <c r="O59" s="256">
         <f t="shared" ref="O59" si="80">(O58/N58)-1</f>
-        <v>-4.7975026611257743E-4</v>
+        <v>1.0972276650162982E-3</v>
       </c>
       <c r="P59" s="239">
         <f t="shared" ref="P59" si="81">(P58/O58)-1</f>
-        <v>2.331054871045346E-4</v>
+        <v>1.7031577777371076E-3</v>
       </c>
       <c r="Q59" s="239">
         <f t="shared" ref="Q59" si="82">(Q58/P58)-1</f>
-        <v>7.2061641703036194E-4</v>
+        <v>2.114773509721557E-3</v>
       </c>
       <c r="R59" s="239">
         <f t="shared" ref="R59" si="83">(R58/Q58)-1</f>
-        <v>2.116064945835161E-3</v>
+        <v>3.2954640481248632E-3</v>
       </c>
       <c r="S59" s="256">
         <f t="shared" ref="S59" si="84">(S58/R58)-1</f>
-        <v>1.0910949504835399E-2</v>
+        <v>1.0120659872131288E-2</v>
       </c>
       <c r="T59" s="239">
         <f t="shared" ref="T59" si="85">(T58/S58)-1</f>
-        <v>1.0330556714686079E-2</v>
+        <v>9.626648838352736E-3</v>
       </c>
       <c r="U59" s="239">
         <f t="shared" ref="U59" si="86">(U58/T58)-1</f>
-        <v>8.0899238394833706E-3</v>
+        <v>7.7217281890062939E-3</v>
       </c>
       <c r="V59" s="239">
         <f t="shared" ref="V59" si="87">(V58/U58)-1</f>
-        <v>6.7268126673245554E-3</v>
+        <v>6.5596818682316371E-3</v>
       </c>
       <c r="W59" s="256">
         <f t="shared" ref="W59" si="88">(W58/V58)-1</f>
-        <v>2.1954258164159635E-2</v>
+        <v>2.3061962329046448E-2</v>
       </c>
       <c r="X59" s="239">
         <f t="shared" ref="X59" si="89">(X58/W58)-1</f>
-        <v>1.7329242545063517E-2</v>
+        <v>1.9016824183518466E-2</v>
       </c>
       <c r="Y59" s="239">
         <f t="shared" ref="Y59" si="90">(Y58/X58)-1</f>
-        <v>1.3417394296062035E-2</v>
+        <v>1.5597296620701417E-2</v>
       </c>
       <c r="Z59" s="239">
         <f t="shared" ref="Z59" si="91">(Z58/Y58)-1</f>
-        <v>9.2869219991904561E-3</v>
+        <v>1.20154519479021E-2</v>
       </c>
       <c r="AA59" s="256">
         <f t="shared" ref="AA59" si="92">(AA58/Z58)-1</f>
-        <v>4.2844900464662494E-3</v>
+        <v>6.3858496583886204E-3</v>
       </c>
       <c r="AB59" s="253"/>
     </row>
@@ -24756,91 +24756,91 @@
       <c r="E60" s="225"/>
       <c r="F60" s="225">
         <f t="shared" ref="F60" si="93">F57-F58</f>
-        <v>593.9340000000002</v>
+        <v>-144.26599999999962</v>
       </c>
       <c r="G60" s="150">
         <f t="shared" ref="G60" si="94">G57-G58</f>
-        <v>313.63927041675925</v>
+        <v>-351.05203247505483</v>
       </c>
       <c r="H60" s="225">
         <f t="shared" ref="H60" si="95">H57-H58</f>
-        <v>1641.5491851595202</v>
+        <v>1035.3076346664193</v>
       </c>
       <c r="I60" s="225">
         <f t="shared" ref="I60" si="96">I57-I58</f>
-        <v>573.89997409674311</v>
+        <v>15.266587468339139</v>
       </c>
       <c r="J60" s="225">
         <f t="shared" ref="J60" si="97">J57-J58</f>
-        <v>500.04967882965548</v>
+        <v>-24.539228482810586</v>
       </c>
       <c r="K60" s="275">
         <f t="shared" ref="K60" si="98">K57-K58</f>
-        <v>468.47397890443426</v>
+        <v>-74.275944959057597</v>
       </c>
       <c r="L60" s="225">
         <f t="shared" ref="L60:AA60" si="99">L57-L58</f>
-        <v>470.55891152641266</v>
+        <v>-75.021173838662662</v>
       </c>
       <c r="M60" s="225">
         <f t="shared" si="99"/>
-        <v>467.02493828306183</v>
+        <v>-74.989566692467861</v>
       </c>
       <c r="N60" s="225">
         <f t="shared" si="99"/>
-        <v>455.71058279371709</v>
+        <v>-73.882290836377479</v>
       </c>
       <c r="O60" s="150">
         <f t="shared" si="99"/>
-        <v>455.49195552035144</v>
+        <v>-73.963356529837938</v>
       </c>
       <c r="P60" s="225">
         <f t="shared" si="99"/>
-        <v>455.59813319451519</v>
+        <v>-74.089327795779354</v>
       </c>
       <c r="Q60" s="225">
         <f t="shared" si="99"/>
-        <v>455.92644468886374</v>
+        <v>-74.246009943554782</v>
       </c>
       <c r="R60" s="225">
         <f t="shared" si="99"/>
-        <v>456.89121465634912</v>
+        <v>-74.490685000040685</v>
       </c>
       <c r="S60" s="150">
         <f t="shared" si="99"/>
-        <v>461.87633162866746</v>
+        <v>-75.244579886568317</v>
       </c>
       <c r="T60" s="225">
         <f t="shared" si="99"/>
-        <v>466.64777126772856</v>
+        <v>-75.968933034125712</v>
       </c>
       <c r="U60" s="225">
         <f t="shared" si="99"/>
-        <v>470.42291619714911</v>
+        <v>-76.55554448582393</v>
       </c>
       <c r="V60" s="225">
         <f t="shared" si="99"/>
-        <v>473.5873630288238</v>
+        <v>-77.057724502900101</v>
       </c>
       <c r="W60" s="150">
         <f t="shared" si="99"/>
-        <v>483.98462226004199</v>
+        <v>-78.834826842547955</v>
       </c>
       <c r="X60" s="225">
         <f t="shared" si="99"/>
-        <v>492.37170916726723</v>
+        <v>-80.334014884150747</v>
       </c>
       <c r="Y60" s="225">
         <f t="shared" si="99"/>
-        <v>498.97805452939042</v>
+        <v>-81.587008343030675</v>
       </c>
       <c r="Z60" s="225">
         <f t="shared" si="99"/>
-        <v>503.61202480111251</v>
+        <v>-82.567313121349343</v>
       </c>
       <c r="AA60" s="150">
         <f t="shared" si="99"/>
-        <v>505.76974550865361</v>
+        <v>-83.094575569639574</v>
       </c>
       <c r="AB60" s="254"/>
     </row>
@@ -25790,8 +25790,8 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M24" sqref="M23:M24"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25913,7 +25913,7 @@
       </c>
       <c r="C3">
         <f t="array" ref="C3:C24">TRANSPOSE('add-ons calculations'!F34:AA34)</f>
-        <v>-597.15600000000018</v>
+        <v>141.0440000000001</v>
       </c>
       <c r="D3">
         <f t="array" ref="D3:D24">TRANSPOSE('add-ons calculations'!F40:AA40)</f>
@@ -25929,7 +25929,7 @@
       </c>
       <c r="G3">
         <f t="array" ref="G3:G24">TRANSPOSE('add-ons calculations'!F60:AA60)</f>
-        <v>593.9340000000002</v>
+        <v>-144.26599999999962</v>
       </c>
       <c r="H3">
         <f t="array" ref="H3:H24">TRANSPOSE('add-ons calculations'!F67:AA67)</f>
@@ -25971,7 +25971,7 @@
         <v>-20.937831399481894</v>
       </c>
       <c r="C4">
-        <v>-669.01923060076751</v>
+        <v>103.25698590656407</v>
       </c>
       <c r="D4">
         <v>-1.0953270393285948</v>
@@ -25983,7 +25983,7 @@
         <v>33.585746620749433</v>
       </c>
       <c r="G4">
-        <v>313.63927041675925</v>
+        <v>-351.05203247505483</v>
       </c>
       <c r="H4">
         <v>-833.94013103694624</v>
@@ -26019,7 +26019,7 @@
         <v>-26.641254195579705</v>
       </c>
       <c r="C5">
-        <v>-687.95031144904317</v>
+        <v>107.63193107562813</v>
       </c>
       <c r="D5">
         <v>-1.1134929435183949</v>
@@ -26031,7 +26031,7 @@
         <v>47.561193892373922</v>
       </c>
       <c r="G5">
-        <v>1641.5491851595202</v>
+        <v>1035.3076346664193</v>
       </c>
       <c r="H5">
         <v>-643.57844188676734</v>
@@ -26054,7 +26054,7 @@
       <c r="O5">
         <v>71.400000000000006</v>
       </c>
-      <c r="P5" s="353">
+      <c r="P5" s="313">
         <f>664000/1000</f>
         <v>664</v>
       </c>
@@ -26067,7 +26067,7 @@
         <v>-34.183111242533812</v>
       </c>
       <c r="C6">
-        <v>-704.80536970482467</v>
+        <v>116.0025854053485</v>
       </c>
       <c r="D6">
         <v>-1.1311990867463919</v>
@@ -26079,7 +26079,7 @@
         <v>57.608534007630169</v>
       </c>
       <c r="G6">
-        <v>573.89997409674311</v>
+        <v>15.266587468339139</v>
       </c>
       <c r="H6">
         <v>-647.99123064723142</v>
@@ -26114,7 +26114,7 @@
         <v>-41.724968289487691</v>
       </c>
       <c r="C7">
-        <v>-699.09796267765057</v>
+        <v>138.64401002534075</v>
       </c>
       <c r="D7">
         <v>-1.150124131134362</v>
@@ -26126,7 +26126,7 @@
         <v>62.552903706427287</v>
       </c>
       <c r="G7">
-        <v>500.04967882965548</v>
+        <v>-24.539228482810586</v>
       </c>
       <c r="H7">
         <v>-652.75653890924525</v>
@@ -26161,7 +26161,7 @@
         <v>-39.457568432331414</v>
       </c>
       <c r="C8">
-        <v>-723.32551143143894</v>
+        <v>125.59921378630472</v>
       </c>
       <c r="D8">
         <v>-1.1627996340230311</v>
@@ -26173,7 +26173,7 @@
         <v>64.144221767586032</v>
       </c>
       <c r="G8">
-        <v>468.47397890443426</v>
+        <v>-74.275944959057597</v>
       </c>
       <c r="H8">
         <v>-1112.559918312772</v>
@@ -26208,7 +26208,7 @@
         <v>5.749168324439097</v>
       </c>
       <c r="C9">
-        <v>-748.96351441585216</v>
+        <v>110.76885817974633</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -26220,7 +26220,7 @@
         <v>65.735539828744777</v>
       </c>
       <c r="G9">
-        <v>470.55891152641266</v>
+        <v>-75.021173838662662</v>
       </c>
       <c r="H9">
         <v>-1163.3117757737041</v>
@@ -26255,7 +26255,7 @@
         <v>8.0165681815954883</v>
       </c>
       <c r="C10">
-        <v>-769.58675706235056</v>
+        <v>134.01495632101853</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -26267,7 +26267,7 @@
         <v>67.326857889903522</v>
       </c>
       <c r="G10">
-        <v>467.02493828306183</v>
+        <v>-74.989566692467861</v>
       </c>
       <c r="H10">
         <v>-1168.3939307885266</v>
@@ -26302,7 +26302,7 @@
         <v>7.9343178535486345</v>
       </c>
       <c r="C11">
-        <v>-788.78977985120866</v>
+        <v>156.03495667590502</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -26314,7 +26314,7 @@
         <v>68.918175951062267</v>
       </c>
       <c r="G11">
-        <v>455.71058279371709</v>
+        <v>-73.882290836377479</v>
       </c>
       <c r="H11">
         <v>-1173.5410146130612</v>
@@ -26349,7 +26349,7 @@
         <v>7.8528747680539652</v>
       </c>
       <c r="C12">
-        <v>-806.39761875672991</v>
+        <v>176.62440241677263</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -26361,7 +26361,7 @@
         <v>69.113046846045563</v>
       </c>
       <c r="G12">
-        <v>455.49195552035144</v>
+        <v>-73.963356529837938</v>
       </c>
       <c r="H12">
         <v>-1178.7530272473091</v>
@@ -26396,7 +26396,7 @@
         <v>7.771431682559296</v>
       </c>
       <c r="C13">
-        <v>-823.60779610211262</v>
+        <v>196.87054077745219</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -26408,7 +26408,7 @@
         <v>69.307917741028632</v>
       </c>
       <c r="G13">
-        <v>455.59813319451519</v>
+        <v>-74.089327795779354</v>
       </c>
       <c r="H13">
         <v>-1184.0417739294007</v>
@@ -26443,7 +26443,7 @@
         <v>7.6899885970646267</v>
       </c>
       <c r="C14">
-        <v>-842.06776692221842</v>
+        <v>218.19564519015159</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -26455,7 +26455,7 @@
         <v>69.502788636011701</v>
       </c>
       <c r="G14">
-        <v>455.92644468886374</v>
+        <v>-74.246009943554782</v>
       </c>
       <c r="H14">
         <v>-1189.3541310877511</v>
@@ -26490,7 +26490,7 @@
         <v>7.6085455115699858</v>
       </c>
       <c r="C15">
-        <v>-860.41412015371282</v>
+        <v>239.42266177993977</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -26502,7 +26502,7 @@
         <v>69.697659530994997</v>
       </c>
       <c r="G15">
-        <v>456.89121465634912</v>
+        <v>-74.490685000040685</v>
       </c>
       <c r="H15">
         <v>-1194.7432222939442</v>
@@ -26537,7 +26537,7 @@
         <v>7.694282358640038</v>
       </c>
       <c r="C16">
-        <v>-866.16924385352081</v>
+        <v>238.71874531468063</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -26549,7 +26549,7 @@
         <v>70.228421056227035</v>
       </c>
       <c r="G16">
-        <v>461.87633162866746</v>
+        <v>-75.244579886568317</v>
       </c>
       <c r="H16">
         <v>-1200.2090475479797</v>
@@ -26584,7 +26584,7 @@
         <v>7.7800192057100617</v>
       </c>
       <c r="C17">
-        <v>-872.60607308499641</v>
+        <v>238.60335578688702</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -26596,7 +26596,7 @@
         <v>70.759182581458845</v>
       </c>
       <c r="G17">
-        <v>466.64777126772856</v>
+        <v>-75.968933034125712</v>
       </c>
       <c r="H17">
         <v>-1205.733898992665</v>
@@ -26631,7 +26631,7 @@
         <v>7.8657560527801138</v>
       </c>
       <c r="C18">
-        <v>-879.66779905383373</v>
+        <v>239.0274492851027</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -26643,7 +26643,7 @@
         <v>71.289944106690882</v>
       </c>
       <c r="G18">
-        <v>470.42291619714911</v>
+        <v>-76.55554448582393</v>
       </c>
       <c r="H18">
         <v>-1211.2705556754795</v>
@@ -26678,7 +26678,7 @@
         <v>7.9514928998501375</v>
       </c>
       <c r="C19">
-        <v>-887.63846573156081</v>
+        <v>240.23624536660571</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -26690,7 +26690,7 @@
         <v>71.82070563192292</v>
       </c>
       <c r="G19">
-        <v>473.5873630288238</v>
+        <v>-77.057724502900101</v>
       </c>
       <c r="H19">
         <v>-1216.8367254536176</v>
@@ -26725,7 +26725,7 @@
         <v>8.0601016192330803</v>
       </c>
       <c r="C20">
-        <v>-894.04140974146321</v>
+        <v>238.57838471534725</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -26737,7 +26737,7 @@
         <v>73.535966403592056</v>
       </c>
       <c r="G20">
-        <v>483.98462226004199</v>
+        <v>-78.834826842547955</v>
       </c>
       <c r="H20">
         <v>-1222.4324083270799</v>
@@ -26772,7 +26772,7 @@
         <v>8.1687103386159947</v>
       </c>
       <c r="C21">
-        <v>-900.33073616275578</v>
+        <v>236.822436241178</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -26784,7 +26784,7 @@
         <v>75.251227175261192</v>
       </c>
       <c r="G21">
-        <v>492.37170916726723</v>
+        <v>-80.334014884150747</v>
       </c>
       <c r="H21">
         <v>-1228.0398964386723</v>
@@ -26819,7 +26819,7 @@
         <v>8.2773190579989091</v>
       </c>
       <c r="C22">
-        <v>-907.07453293849244</v>
+        <v>235.45883905865185</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -26831,7 +26831,7 @@
         <v>76.966487946930556</v>
       </c>
       <c r="G22">
-        <v>498.97805452939042</v>
+        <v>-81.587008343030675</v>
       </c>
       <c r="H22">
         <v>-1233.6178714549401</v>
@@ -26866,7 +26866,7 @@
         <v>8.3859277773818519</v>
       </c>
       <c r="C23">
-        <v>-914.32960886297974</v>
+        <v>234.53663707922496</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -26878,7 +26878,7 @@
         <v>78.68174871859992</v>
       </c>
       <c r="G23">
-        <v>503.61202480111251</v>
+        <v>-82.567313121349343</v>
       </c>
       <c r="H23">
         <v>-1239.2017490902733</v>
@@ -26913,7 +26913,7 @@
         <v>8.4989455787047632</v>
       </c>
       <c r="C24">
-        <v>-921.70408674507178</v>
+        <v>233.42580901803058</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -26925,7 +26925,7 @@
         <v>79.962880996821241</v>
       </c>
       <c r="G24">
-        <v>505.76974550865361</v>
+        <v>-83.094575569639574</v>
       </c>
       <c r="H24">
         <v>-1244.7856267256061</v>
@@ -26961,7 +26961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C37CCB5-9AFD-AA42-ADF6-76E6C38F7458}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -26972,36 +26972,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="D1" s="314" t="s">
+      <c r="D1" s="315" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="314" t="s">
+      <c r="E1" s="315"/>
+      <c r="F1" s="315"/>
+      <c r="G1" s="315"/>
+      <c r="H1" s="315" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="314"/>
-      <c r="J1" s="314"/>
-      <c r="K1" s="314"/>
-      <c r="L1" s="314" t="s">
+      <c r="I1" s="315"/>
+      <c r="J1" s="315"/>
+      <c r="K1" s="315"/>
+      <c r="L1" s="315" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="314"/>
-      <c r="N1" s="314"/>
-      <c r="O1" s="314"/>
-      <c r="P1" s="314" t="s">
+      <c r="M1" s="315"/>
+      <c r="N1" s="315"/>
+      <c r="O1" s="315"/>
+      <c r="P1" s="315" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="314"/>
-      <c r="R1" s="314"/>
-      <c r="S1" s="314"/>
-      <c r="T1" s="314" t="s">
+      <c r="Q1" s="315"/>
+      <c r="R1" s="315"/>
+      <c r="S1" s="315"/>
+      <c r="T1" s="315" t="s">
         <v>268</v>
       </c>
-      <c r="U1" s="314"/>
-      <c r="V1" s="314"/>
-      <c r="W1" s="314"/>
+      <c r="U1" s="315"/>
+      <c r="V1" s="315"/>
+      <c r="W1" s="315"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="D2" s="199" t="s">
@@ -27411,22 +27411,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="320" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="320"/>
+      <c r="B1" s="321"/>
       <c r="C1" s="35"/>
       <c r="I1" s="250"/>
-      <c r="J1" s="327" t="s">
+      <c r="J1" s="328" t="s">
         <v>282</v>
       </c>
-      <c r="V1" s="314"/>
-      <c r="W1" s="314"/>
-      <c r="X1" s="314"/>
-      <c r="Y1" s="314"/>
+      <c r="V1" s="315"/>
+      <c r="W1" s="315"/>
+      <c r="X1" s="315"/>
+      <c r="Y1" s="315"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="321" t="s">
+      <c r="A2" s="322" t="s">
         <v>192</v>
       </c>
       <c r="B2" s="126"/>
@@ -27435,20 +27435,20 @@
       </c>
       <c r="H2" s="95"/>
       <c r="I2" s="251"/>
-      <c r="J2" s="327"/>
+      <c r="J2" s="328"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="322"/>
+      <c r="A3" s="323"/>
       <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
       <c r="H3" s="95"/>
       <c r="I3" s="251"/>
-      <c r="J3" s="327"/>
+      <c r="J3" s="328"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="322"/>
+      <c r="A4" s="323"/>
       <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>195</v>
@@ -27458,7 +27458,7 @@
       <c r="J4" s="95"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="323"/>
+      <c r="A5" s="324"/>
       <c r="B5" s="129"/>
       <c r="C5" t="s">
         <v>182</v>
@@ -27473,42 +27473,42 @@
       <c r="J6" s="95"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="C7" s="324" t="s">
+      <c r="C7" s="325" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="325"/>
-      <c r="E7" s="325"/>
-      <c r="F7" s="326"/>
-      <c r="G7" s="324" t="s">
+      <c r="D7" s="326"/>
+      <c r="E7" s="326"/>
+      <c r="F7" s="327"/>
+      <c r="G7" s="325" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="325"/>
-      <c r="I7" s="325"/>
-      <c r="J7" s="326"/>
-      <c r="K7" s="324" t="s">
+      <c r="H7" s="326"/>
+      <c r="I7" s="326"/>
+      <c r="J7" s="327"/>
+      <c r="K7" s="325" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="325"/>
-      <c r="M7" s="325"/>
-      <c r="N7" s="325"/>
-      <c r="O7" s="324" t="s">
+      <c r="L7" s="326"/>
+      <c r="M7" s="326"/>
+      <c r="N7" s="326"/>
+      <c r="O7" s="325" t="s">
         <v>272</v>
       </c>
-      <c r="P7" s="325"/>
-      <c r="Q7" s="325"/>
-      <c r="R7" s="325"/>
-      <c r="S7" s="324" t="s">
+      <c r="P7" s="326"/>
+      <c r="Q7" s="326"/>
+      <c r="R7" s="326"/>
+      <c r="S7" s="325" t="s">
         <v>276</v>
       </c>
-      <c r="T7" s="325"/>
-      <c r="U7" s="325"/>
-      <c r="V7" s="325"/>
-      <c r="W7" s="324" t="s">
+      <c r="T7" s="326"/>
+      <c r="U7" s="326"/>
+      <c r="V7" s="326"/>
+      <c r="W7" s="325" t="s">
         <v>277</v>
       </c>
-      <c r="X7" s="325"/>
-      <c r="Y7" s="325"/>
-      <c r="Z7" s="325"/>
+      <c r="X7" s="326"/>
+      <c r="Y7" s="326"/>
+      <c r="Z7" s="326"/>
       <c r="AA7" s="231" t="s">
         <v>278</v>
       </c>
@@ -31949,9 +31949,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -32172,27 +32175,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
-    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -32217,9 +32208,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
+    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added info the chnages file
</commit_message>
<xml_diff>
--- a/documentation/COVID-19 Changes/September/LSFIM_KY_v6_round2.xlsx
+++ b/documentation/COVID-19 Changes/September/LSFIM_KY_v6_round2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyilla\Documents\Git\Fiscal-Impact-Measure\documentation\COVID-19 Changes\September\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29472AD-BB99-499B-9090-BDDA871E27AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB8D0E3-F3E5-483A-ABAE-DE6D45E8FCCC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -2193,7 +2193,7 @@
     <numFmt numFmtId="172" formatCode="0.0000"/>
     <numFmt numFmtId="173" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2424,12 +2424,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="19">
@@ -3526,6 +3520,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="27" fillId="16" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="25" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="27" fillId="17" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3592,6 +3596,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3613,43 +3632,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="27" fillId="16" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="25" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="27" fillId="17" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4184,10 +4178,10 @@
   <dimension ref="A1:AS115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="L94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="J35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q31" sqref="Q31"/>
+      <selection pane="bottomRight" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4211,10 +4205,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="317" t="s">
+      <c r="A1" s="325" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="317"/>
+      <c r="B1" s="325"/>
       <c r="C1" s="279"/>
       <c r="D1" s="279"/>
       <c r="E1" s="35"/>
@@ -4230,78 +4224,78 @@
       <c r="AE1" s="179" t="s">
         <v>249</v>
       </c>
-      <c r="AF1" s="319" t="s">
+      <c r="AF1" s="327" t="s">
         <v>247</v>
       </c>
-      <c r="AG1" s="319"/>
-      <c r="AH1" s="319"/>
+      <c r="AG1" s="327"/>
+      <c r="AH1" s="327"/>
       <c r="AI1" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" s="320" t="s">
+      <c r="AK1" s="328" t="s">
         <v>281</v>
       </c>
-      <c r="AL1" s="320"/>
-      <c r="AM1" s="320"/>
-      <c r="AN1" s="320"/>
-      <c r="AO1" s="318" t="s">
+      <c r="AL1" s="328"/>
+      <c r="AM1" s="328"/>
+      <c r="AN1" s="328"/>
+      <c r="AO1" s="326" t="s">
         <v>279</v>
       </c>
-      <c r="AP1" s="318"/>
-      <c r="AQ1" s="318"/>
-      <c r="AR1" s="318"/>
+      <c r="AP1" s="326"/>
+      <c r="AQ1" s="326"/>
+      <c r="AR1" s="326"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="F2" s="316" t="s">
+      <c r="F2" s="324" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="316"/>
-      <c r="H2" s="316"/>
-      <c r="I2" s="316"/>
-      <c r="J2" s="316" t="s">
+      <c r="G2" s="324"/>
+      <c r="H2" s="324"/>
+      <c r="I2" s="324"/>
+      <c r="J2" s="324" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="316"/>
-      <c r="L2" s="316"/>
-      <c r="M2" s="316"/>
+      <c r="K2" s="324"/>
+      <c r="L2" s="324"/>
+      <c r="M2" s="324"/>
       <c r="N2" s="314"/>
       <c r="O2" s="314"/>
-      <c r="P2" s="316" t="s">
+      <c r="P2" s="324" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="316"/>
-      <c r="R2" s="316"/>
-      <c r="S2" s="316"/>
-      <c r="T2" s="316" t="s">
+      <c r="Q2" s="324"/>
+      <c r="R2" s="324"/>
+      <c r="S2" s="324"/>
+      <c r="T2" s="324" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="316"/>
-      <c r="V2" s="316"/>
-      <c r="W2" s="316"/>
-      <c r="X2" s="316" t="s">
+      <c r="U2" s="324"/>
+      <c r="V2" s="324"/>
+      <c r="W2" s="324"/>
+      <c r="X2" s="324" t="s">
         <v>268</v>
       </c>
-      <c r="Y2" s="316"/>
-      <c r="Z2" s="316"/>
-      <c r="AA2" s="316"/>
+      <c r="Y2" s="324"/>
+      <c r="Z2" s="324"/>
+      <c r="AA2" s="324"/>
       <c r="AB2" s="229"/>
       <c r="AC2" s="296"/>
       <c r="AD2" s="229"/>
       <c r="AE2" s="156"/>
-      <c r="AF2" s="316" t="s">
+      <c r="AF2" s="324" t="s">
         <v>102</v>
       </c>
-      <c r="AG2" s="316"/>
-      <c r="AH2" s="316"/>
+      <c r="AG2" s="324"/>
+      <c r="AH2" s="324"/>
       <c r="AI2" s="156"/>
       <c r="AJ2" s="156" t="s">
         <v>21</v>
       </c>
-      <c r="AK2" s="316" t="s">
+      <c r="AK2" s="324" t="s">
         <v>102</v>
       </c>
-      <c r="AL2" s="316"/>
-      <c r="AM2" s="316"/>
+      <c r="AL2" s="324"/>
+      <c r="AM2" s="324"/>
       <c r="AN2" s="230"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.35">
@@ -4329,8 +4323,8 @@
       <c r="M3" s="199" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="355"/>
-      <c r="O3" s="355"/>
+      <c r="N3" s="315"/>
+      <c r="O3" s="315"/>
       <c r="P3" t="s">
         <v>5</v>
       </c>
@@ -4411,10 +4405,10 @@
       </c>
     </row>
     <row r="4" spans="1:45" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="315" t="s">
+      <c r="A4" s="323" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="315"/>
+      <c r="B4" s="323"/>
       <c r="C4" s="279"/>
       <c r="D4" s="279"/>
       <c r="F4" s="199"/>
@@ -4425,8 +4419,8 @@
       <c r="K4" s="199"/>
       <c r="L4" s="199"/>
       <c r="M4" s="199"/>
-      <c r="N4" s="355"/>
-      <c r="O4" s="355"/>
+      <c r="N4" s="315"/>
+      <c r="O4" s="315"/>
       <c r="AE4" s="192"/>
       <c r="AF4" s="180"/>
       <c r="AG4" s="192"/>
@@ -4473,10 +4467,10 @@
         <f>VLOOKUP(C5,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>21170.3</v>
       </c>
-      <c r="N5" s="355">
+      <c r="N5" s="315">
         <v>21157.1</v>
       </c>
-      <c r="O5" s="355">
+      <c r="O5" s="315">
         <f>N5-M5</f>
         <v>-13.200000000000728</v>
       </c>
@@ -4562,11 +4556,11 @@
         <f t="shared" si="0"/>
         <v>8.4538501339644911E-2</v>
       </c>
-      <c r="N6" s="356">
+      <c r="N6" s="316">
         <v>8.3862275295720767E-2</v>
       </c>
-      <c r="O6" s="355">
-        <f t="shared" ref="O6:O69" si="1">N6-M6</f>
+      <c r="O6" s="315">
+        <f t="shared" ref="O6:O68" si="1">N6-M6</f>
         <v>-6.7622604392414409E-4</v>
       </c>
       <c r="P6" s="198">
@@ -4657,10 +4651,10 @@
         <f>VLOOKUP(C7,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>18596.5</v>
       </c>
-      <c r="N7" s="355">
+      <c r="N7" s="315">
         <v>18583.5</v>
       </c>
-      <c r="O7" s="355">
+      <c r="O7" s="315">
         <f t="shared" si="1"/>
         <v>-13</v>
       </c>
@@ -4725,8 +4719,8 @@
       <c r="K8" s="217"/>
       <c r="L8" s="217"/>
       <c r="M8" s="199"/>
-      <c r="N8" s="355"/>
-      <c r="O8" s="355"/>
+      <c r="N8" s="315"/>
+      <c r="O8" s="315"/>
       <c r="P8" s="216"/>
       <c r="Q8" s="216"/>
       <c r="R8" s="216"/>
@@ -4756,8 +4750,8 @@
       <c r="K9" s="199"/>
       <c r="L9" s="199"/>
       <c r="M9" s="199"/>
-      <c r="N9" s="355"/>
-      <c r="O9" s="355"/>
+      <c r="N9" s="315"/>
+      <c r="O9" s="315"/>
       <c r="AE9" s="192"/>
       <c r="AF9" s="180"/>
       <c r="AG9" s="192"/>
@@ -4781,8 +4775,8 @@
       <c r="K10" s="199"/>
       <c r="L10" s="199"/>
       <c r="M10" s="199"/>
-      <c r="N10" s="355"/>
-      <c r="O10" s="355"/>
+      <c r="N10" s="315"/>
+      <c r="O10" s="315"/>
       <c r="AF10" s="146"/>
       <c r="AK10" s="146"/>
     </row>
@@ -4822,10 +4816,10 @@
         <f t="shared" si="2"/>
         <v>3262.3</v>
       </c>
-      <c r="N11" s="355">
+      <c r="N11" s="315">
         <v>3261.5</v>
       </c>
-      <c r="O11" s="355">
+      <c r="O11" s="315">
         <f t="shared" si="1"/>
         <v>-0.8000000000001819</v>
       </c>
@@ -4905,10 +4899,10 @@
         <f>VLOOKUP(C12,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>1687.4</v>
       </c>
-      <c r="N12" s="355">
+      <c r="N12" s="315">
         <v>1687.2</v>
       </c>
-      <c r="O12" s="355">
+      <c r="O12" s="315">
         <f t="shared" si="1"/>
         <v>-0.20000000000004547</v>
       </c>
@@ -5005,8 +4999,8 @@
       <c r="K13" s="201"/>
       <c r="L13" s="201"/>
       <c r="M13" s="199"/>
-      <c r="N13" s="355"/>
-      <c r="O13" s="355"/>
+      <c r="N13" s="315"/>
+      <c r="O13" s="315"/>
       <c r="P13" s="176">
         <v>0.06</v>
       </c>
@@ -5087,10 +5081,10 @@
         <f>VLOOKUP(C14,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>144.69999999999999</v>
       </c>
-      <c r="N14" s="355">
+      <c r="N14" s="315">
         <v>144.69999999999999</v>
       </c>
-      <c r="O14" s="355">
+      <c r="O14" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5183,8 +5177,8 @@
       <c r="K15" s="201"/>
       <c r="L15" s="201"/>
       <c r="M15" s="199"/>
-      <c r="N15" s="355"/>
-      <c r="O15" s="355"/>
+      <c r="N15" s="315"/>
+      <c r="O15" s="315"/>
       <c r="P15" s="176">
         <v>0.04</v>
       </c>
@@ -5265,10 +5259,10 @@
         <f>VLOOKUP(C16,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>1430.2</v>
       </c>
-      <c r="N16" s="355">
+      <c r="N16" s="315">
         <v>1429.6</v>
       </c>
-      <c r="O16" s="355">
+      <c r="O16" s="315">
         <f t="shared" si="1"/>
         <v>-0.60000000000013642</v>
       </c>
@@ -5365,8 +5359,8 @@
       <c r="K17" s="201"/>
       <c r="L17" s="201"/>
       <c r="M17" s="199"/>
-      <c r="N17" s="355"/>
-      <c r="O17" s="355"/>
+      <c r="N17" s="315"/>
+      <c r="O17" s="315"/>
       <c r="P17" s="176">
         <v>1.2999999999999999E-2</v>
       </c>
@@ -5447,10 +5441,10 @@
         <f>VLOOKUP(C18,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>207</v>
       </c>
-      <c r="N18" s="355">
+      <c r="N18" s="315">
         <v>205.3</v>
       </c>
-      <c r="O18" s="355">
+      <c r="O18" s="315">
         <f t="shared" si="1"/>
         <v>-1.6999999999999886</v>
       </c>
@@ -5546,8 +5540,8 @@
       <c r="K19" s="201"/>
       <c r="L19" s="201"/>
       <c r="M19" s="199"/>
-      <c r="N19" s="355"/>
-      <c r="O19" s="355"/>
+      <c r="N19" s="315"/>
+      <c r="O19" s="315"/>
       <c r="P19" s="176">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -5604,8 +5598,8 @@
       <c r="K20" s="201"/>
       <c r="L20" s="201"/>
       <c r="M20" s="199"/>
-      <c r="N20" s="355"/>
-      <c r="O20" s="355"/>
+      <c r="N20" s="315"/>
+      <c r="O20" s="315"/>
       <c r="P20" s="176"/>
       <c r="Q20" s="176"/>
       <c r="R20" s="176"/>
@@ -5646,8 +5640,8 @@
       <c r="K21" s="201"/>
       <c r="L21" s="201"/>
       <c r="M21" s="199"/>
-      <c r="N21" s="355"/>
-      <c r="O21" s="355"/>
+      <c r="N21" s="315"/>
+      <c r="O21" s="315"/>
       <c r="P21" s="176"/>
       <c r="Q21" s="176"/>
       <c r="R21" s="176"/>
@@ -5710,10 +5704,10 @@
         <f t="shared" si="13"/>
         <v>1871.3489999999999</v>
       </c>
-      <c r="N22" s="355">
+      <c r="N22" s="315">
         <v>1836.9459999999999</v>
       </c>
-      <c r="O22" s="355">
+      <c r="O22" s="315">
         <f t="shared" si="1"/>
         <v>-34.40300000000002</v>
       </c>
@@ -5787,10 +5781,10 @@
         <f>VLOOKUP(C23,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>506.6</v>
       </c>
-      <c r="N23" s="355">
+      <c r="N23" s="315">
         <v>499.4</v>
       </c>
-      <c r="O23" s="355">
+      <c r="O23" s="315">
         <f t="shared" si="1"/>
         <v>-7.2000000000000455</v>
       </c>
@@ -5864,10 +5858,10 @@
         <f>VLOOKUP(C24,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>1344.5</v>
       </c>
-      <c r="N24" s="355">
+      <c r="N24" s="315">
         <v>1317.3</v>
       </c>
-      <c r="O24" s="355">
+      <c r="O24" s="315">
         <f t="shared" si="1"/>
         <v>-27.200000000000045</v>
       </c>
@@ -5941,10 +5935,10 @@
         <f>VLOOKUP(C25,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>20.248999999999999</v>
       </c>
-      <c r="N25" s="355">
+      <c r="N25" s="315">
         <v>20.245999999999999</v>
       </c>
-      <c r="O25" s="355">
+      <c r="O25" s="315">
         <f t="shared" si="1"/>
         <v>-3.0000000000001137E-3</v>
       </c>
@@ -6018,10 +6012,10 @@
         <f>VLOOKUP(C26,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>90.2</v>
       </c>
-      <c r="N26" s="355">
+      <c r="N26" s="315">
         <v>79.099999999999994</v>
       </c>
-      <c r="O26" s="355">
+      <c r="O26" s="315">
         <f t="shared" si="1"/>
         <v>-11.100000000000009</v>
       </c>
@@ -6095,8 +6089,8 @@
         <v>0.31603498542274056</v>
       </c>
       <c r="M27" s="199"/>
-      <c r="N27" s="355"/>
-      <c r="O27" s="355"/>
+      <c r="N27" s="315"/>
+      <c r="O27" s="315"/>
       <c r="P27" s="195"/>
       <c r="Q27" s="195"/>
       <c r="R27" s="195"/>
@@ -6120,8 +6114,8 @@
       <c r="K28" s="201"/>
       <c r="L28" s="201"/>
       <c r="M28" s="199"/>
-      <c r="N28" s="355"/>
-      <c r="O28" s="355"/>
+      <c r="N28" s="315"/>
+      <c r="O28" s="315"/>
       <c r="P28" s="176"/>
       <c r="Q28" s="176"/>
       <c r="R28" s="176"/>
@@ -6166,8 +6160,8 @@
       <c r="K29" s="199"/>
       <c r="L29" s="203"/>
       <c r="M29" s="199"/>
-      <c r="N29" s="355"/>
-      <c r="O29" s="355"/>
+      <c r="N29" s="315"/>
+      <c r="O29" s="315"/>
       <c r="P29" s="88"/>
       <c r="Q29" s="88"/>
       <c r="R29" s="88"/>
@@ -6218,10 +6212,10 @@
         <f>VLOOKUP(C30,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>3494888</v>
       </c>
-      <c r="N30" s="355">
+      <c r="N30" s="315">
         <v>3488125</v>
       </c>
-      <c r="O30" s="355">
+      <c r="O30" s="315">
         <f t="shared" si="1"/>
         <v>-6763</v>
       </c>
@@ -6327,10 +6321,10 @@
         <f>VLOOKUP(C31,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>842733</v>
       </c>
-      <c r="N31" s="355">
+      <c r="N31" s="315">
         <v>842733</v>
       </c>
-      <c r="O31" s="355">
+      <c r="O31" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6452,10 +6446,10 @@
         <f>VLOOKUP(C32,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>15600</v>
       </c>
-      <c r="N32" s="355">
+      <c r="N32" s="315">
         <v>15600</v>
       </c>
-      <c r="O32" s="355">
+      <c r="O32" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6514,8 +6508,8 @@
       <c r="K33" s="286"/>
       <c r="L33" s="286"/>
       <c r="M33" s="287"/>
-      <c r="N33" s="357"/>
-      <c r="O33" s="355"/>
+      <c r="N33" s="317"/>
+      <c r="O33" s="315"/>
       <c r="P33" s="288"/>
       <c r="Q33" s="288">
         <f>'Stimulus Round 2'!C4*4</f>
@@ -6549,8 +6543,8 @@
       <c r="K34" s="286"/>
       <c r="L34" s="286"/>
       <c r="M34" s="287"/>
-      <c r="N34" s="357"/>
-      <c r="O34" s="355"/>
+      <c r="N34" s="317"/>
+      <c r="O34" s="315"/>
       <c r="P34" s="288"/>
       <c r="Q34" s="288">
         <f>'Stimulus Round 2'!$C$15*4/2</f>
@@ -6587,8 +6581,8 @@
       <c r="K35" s="286"/>
       <c r="L35" s="286"/>
       <c r="M35" s="287"/>
-      <c r="N35" s="357"/>
-      <c r="O35" s="355"/>
+      <c r="N35" s="317"/>
+      <c r="O35" s="315"/>
       <c r="P35" s="288"/>
       <c r="Q35" s="288">
         <f>'Stimulus Round 2'!$C$19*4/4</f>
@@ -6648,10 +6642,10 @@
         <f>M37+M40</f>
         <v>881354</v>
       </c>
-      <c r="N36" s="355">
+      <c r="N36" s="315">
         <v>874878</v>
       </c>
-      <c r="O36" s="355">
+      <c r="O36" s="315">
         <f t="shared" si="1"/>
         <v>-6476</v>
       </c>
@@ -6750,10 +6744,10 @@
         <f>VLOOKUP(C37,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>775154</v>
       </c>
-      <c r="N37" s="355">
+      <c r="N37" s="315">
         <v>768678</v>
       </c>
-      <c r="O37" s="355">
+      <c r="O37" s="315">
         <f t="shared" si="1"/>
         <v>-6476</v>
       </c>
@@ -6800,10 +6794,10 @@
         <f>M39+M40</f>
         <v>738200</v>
       </c>
-      <c r="N38" s="355">
+      <c r="N38" s="315">
         <v>738200</v>
       </c>
-      <c r="O38" s="355">
+      <c r="O38" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6870,10 +6864,10 @@
         <f>1000*'figuring out UI'!N17</f>
         <v>632000</v>
       </c>
-      <c r="N39" s="355">
+      <c r="N39" s="315">
         <v>632000</v>
       </c>
-      <c r="O39" s="355">
+      <c r="O39" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6950,10 +6944,10 @@
       <c r="M40" s="199">
         <v>106200</v>
       </c>
-      <c r="N40" s="355">
+      <c r="N40" s="315">
         <v>106200</v>
       </c>
-      <c r="O40" s="355">
+      <c r="O40" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6998,8 +6992,8 @@
       <c r="K41" s="286"/>
       <c r="L41" s="286"/>
       <c r="M41" s="287"/>
-      <c r="N41" s="357"/>
-      <c r="O41" s="355"/>
+      <c r="N41" s="317"/>
+      <c r="O41" s="315"/>
       <c r="P41" s="288"/>
       <c r="Q41" s="288">
         <f>'Stimulus Round 2'!$C$3*4</f>
@@ -7051,10 +7045,10 @@
         <f>1000*'figuring out UI'!N18</f>
         <v>140000</v>
       </c>
-      <c r="N42" s="355">
+      <c r="N42" s="315">
         <v>140000</v>
       </c>
-      <c r="O42" s="355">
+      <c r="O42" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7142,10 +7136,10 @@
         <f>SUM(M44:M45)</f>
         <v>85400</v>
       </c>
-      <c r="N43" s="355">
+      <c r="N43" s="315">
         <v>85400</v>
       </c>
-      <c r="O43" s="355">
+      <c r="O43" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7226,10 +7220,10 @@
         <f>VLOOKUP(C44,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>27000</v>
       </c>
-      <c r="N44" s="355">
+      <c r="N44" s="315">
         <v>27000</v>
       </c>
-      <c r="O44" s="355">
+      <c r="O44" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7293,10 +7287,10 @@
         <f>VLOOKUP(C45,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>58400</v>
       </c>
-      <c r="N45" s="355">
+      <c r="N45" s="315">
         <v>58400</v>
       </c>
-      <c r="O45" s="355">
+      <c r="O45" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7372,10 +7366,10 @@
         <f>M30-M32-M36-M31-M43</f>
         <v>1669801</v>
       </c>
-      <c r="N46" s="358">
+      <c r="N46" s="318">
         <v>1669514</v>
       </c>
-      <c r="O46" s="355">
+      <c r="O46" s="315">
         <f t="shared" si="1"/>
         <v>-287</v>
       </c>
@@ -7493,8 +7487,8 @@
         <v>2.938781628264131E-2</v>
       </c>
       <c r="M47" s="199"/>
-      <c r="N47" s="355"/>
-      <c r="O47" s="355">
+      <c r="N47" s="315"/>
+      <c r="O47" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7536,8 +7530,8 @@
       <c r="K48" s="202"/>
       <c r="L48" s="202"/>
       <c r="M48" s="199"/>
-      <c r="N48" s="355"/>
-      <c r="O48" s="355">
+      <c r="N48" s="315"/>
+      <c r="O48" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7597,8 +7591,8 @@
       <c r="K49" s="199"/>
       <c r="L49" s="199"/>
       <c r="M49" s="199"/>
-      <c r="N49" s="355"/>
-      <c r="O49" s="355"/>
+      <c r="N49" s="315"/>
+      <c r="O49" s="315"/>
       <c r="P49" s="3"/>
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
@@ -7662,10 +7656,10 @@
         <f>VLOOKUP(C50,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>1213480</v>
       </c>
-      <c r="N50" s="358">
+      <c r="N50" s="318">
         <v>1213308</v>
       </c>
-      <c r="O50" s="355">
+      <c r="O50" s="315">
         <f t="shared" si="1"/>
         <v>-172</v>
       </c>
@@ -7750,7 +7744,7 @@
       <c r="N51" s="116">
         <v>1093900</v>
       </c>
-      <c r="O51" s="355">
+      <c r="O51" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7815,7 +7809,7 @@
       <c r="K52" s="204"/>
       <c r="L52" s="204"/>
       <c r="M52" s="204"/>
-      <c r="O52" s="355"/>
+      <c r="O52" s="315"/>
       <c r="P52" s="116"/>
       <c r="Q52" s="116"/>
       <c r="R52" s="116"/>
@@ -7859,10 +7853,10 @@
         <f>VLOOKUP(C53,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>865600</v>
       </c>
-      <c r="N53" s="358">
+      <c r="N53" s="318">
         <v>865600</v>
       </c>
-      <c r="O53" s="355">
+      <c r="O53" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7935,7 +7929,7 @@
         <f>SUM(N55:N57)</f>
         <v>228300</v>
       </c>
-      <c r="O54" s="362">
+      <c r="O54" s="322">
         <f>N56-M56</f>
         <v>0</v>
       </c>
@@ -8004,10 +7998,10 @@
         <f>VLOOKUP(C55,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>15000</v>
       </c>
-      <c r="N55" s="355">
+      <c r="N55" s="315">
         <v>15000</v>
       </c>
-      <c r="O55" s="362">
+      <c r="O55" s="322">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8057,7 +8051,7 @@
         <f>VLOOKUP(C56,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>73300</v>
       </c>
-      <c r="N56" s="359">
+      <c r="N56" s="319">
         <v>73300</v>
       </c>
       <c r="P56" s="264"/>
@@ -8106,10 +8100,10 @@
         <f>VLOOKUP(C57,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>140000</v>
       </c>
-      <c r="N57" s="359">
+      <c r="N57" s="319">
         <v>140000</v>
       </c>
-      <c r="O57" s="362">
+      <c r="O57" s="322">
         <f>N57-M57</f>
         <v>0</v>
       </c>
@@ -8149,8 +8143,8 @@
       <c r="K58" s="263"/>
       <c r="L58" s="263"/>
       <c r="M58" s="199"/>
-      <c r="N58" s="355"/>
-      <c r="O58" s="355"/>
+      <c r="N58" s="315"/>
+      <c r="O58" s="315"/>
       <c r="P58" s="264"/>
       <c r="Q58" s="264"/>
       <c r="R58" s="264"/>
@@ -8185,8 +8179,8 @@
       <c r="K59" s="286"/>
       <c r="L59" s="286"/>
       <c r="M59" s="287"/>
-      <c r="N59" s="357"/>
-      <c r="O59" s="355"/>
+      <c r="N59" s="317"/>
+      <c r="O59" s="315"/>
       <c r="P59" s="292"/>
       <c r="Q59" s="292">
         <f>'Stimulus Round 2'!$C$2*4/3</f>
@@ -8230,8 +8224,8 @@
       <c r="K60" s="286"/>
       <c r="L60" s="286"/>
       <c r="M60" s="287"/>
-      <c r="N60" s="357"/>
-      <c r="O60" s="355"/>
+      <c r="N60" s="317"/>
+      <c r="O60" s="315"/>
       <c r="P60" s="292"/>
       <c r="Q60" s="292">
         <f>'Stimulus Round 2'!$C$12*4/3</f>
@@ -8275,8 +8269,8 @@
       <c r="K61" s="286"/>
       <c r="L61" s="286"/>
       <c r="M61" s="287"/>
-      <c r="N61" s="357"/>
-      <c r="O61" s="355"/>
+      <c r="N61" s="317"/>
+      <c r="O61" s="315"/>
       <c r="P61" s="292"/>
       <c r="Q61" s="292">
         <f>'Stimulus Round 2'!$C$18*4/4</f>
@@ -8323,8 +8317,8 @@
       <c r="K62" s="286"/>
       <c r="L62" s="286"/>
       <c r="M62" s="287"/>
-      <c r="N62" s="357"/>
-      <c r="O62" s="355"/>
+      <c r="N62" s="317"/>
+      <c r="O62" s="315"/>
       <c r="P62" s="292"/>
       <c r="Q62" s="292">
         <f>'Stimulus Round 2'!$C$20*4/8</f>
@@ -8381,8 +8375,8 @@
       <c r="K63" s="204"/>
       <c r="L63" s="204"/>
       <c r="M63" s="199"/>
-      <c r="N63" s="355"/>
-      <c r="O63" s="355"/>
+      <c r="N63" s="315"/>
+      <c r="O63" s="315"/>
       <c r="P63" s="116"/>
       <c r="Q63" s="116"/>
       <c r="R63" s="116"/>
@@ -8441,10 +8435,10 @@
         <f>VLOOKUP(C64,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>728172</v>
       </c>
-      <c r="N64" s="355">
+      <c r="N64" s="315">
         <v>728172</v>
       </c>
-      <c r="O64" s="355">
+      <c r="O64" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8523,10 +8517,10 @@
         <f t="shared" si="34"/>
         <v>242100</v>
       </c>
-      <c r="N65" s="355">
+      <c r="N65" s="315">
         <v>242100</v>
       </c>
-      <c r="O65" s="355">
+      <c r="O65" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8570,10 +8564,10 @@
         <f>L66*(1+M82)</f>
         <v>189980.38194444444</v>
       </c>
-      <c r="N66" s="360">
+      <c r="N66" s="320">
         <v>189950.61436735778</v>
       </c>
-      <c r="O66" s="355">
+      <c r="O66" s="315">
         <f t="shared" si="1"/>
         <v>-29.767577086662641</v>
       </c>
@@ -8658,10 +8652,10 @@
       <c r="M67" s="199">
         <v>38500</v>
       </c>
-      <c r="N67" s="355">
+      <c r="N67" s="315">
         <v>38500</v>
       </c>
-      <c r="O67" s="355">
+      <c r="O67" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8705,10 +8699,10 @@
         <f>SUM(M70:M72)</f>
         <v>97000</v>
       </c>
-      <c r="N68" s="355">
+      <c r="N68" s="315">
         <v>97000</v>
       </c>
-      <c r="O68" s="355">
+      <c r="O68" s="315">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -8785,8 +8779,8 @@
       <c r="K69" s="204"/>
       <c r="L69" s="208"/>
       <c r="M69" s="199"/>
-      <c r="N69" s="355"/>
-      <c r="O69" s="355"/>
+      <c r="N69" s="315"/>
+      <c r="O69" s="315"/>
       <c r="P69" s="116"/>
       <c r="Q69" s="116"/>
       <c r="R69" s="116"/>
@@ -8825,10 +8819,10 @@
       <c r="M70" s="199">
         <v>45000</v>
       </c>
-      <c r="N70" s="355">
+      <c r="N70" s="315">
         <v>45000</v>
       </c>
-      <c r="O70" s="355">
+      <c r="O70" s="315">
         <f t="shared" ref="O70:O107" si="43">N70-M70</f>
         <v>0</v>
       </c>
@@ -8890,10 +8884,10 @@
       <c r="M71" s="199">
         <v>27000</v>
       </c>
-      <c r="N71" s="355">
+      <c r="N71" s="315">
         <v>27000</v>
       </c>
-      <c r="O71" s="355">
+      <c r="O71" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -8945,10 +8939,10 @@
       <c r="M72" s="199">
         <v>25000</v>
       </c>
-      <c r="N72" s="355">
+      <c r="N72" s="315">
         <v>25000</v>
       </c>
-      <c r="O72" s="355">
+      <c r="O72" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -8996,8 +8990,8 @@
       <c r="K73" s="204"/>
       <c r="L73" s="204"/>
       <c r="M73" s="199"/>
-      <c r="N73" s="355"/>
-      <c r="O73" s="355"/>
+      <c r="N73" s="315"/>
+      <c r="O73" s="315"/>
       <c r="P73" s="116"/>
       <c r="Q73" s="116">
         <f>SUM(Q74:Q77)</f>
@@ -9068,8 +9062,8 @@
       <c r="K74" s="286"/>
       <c r="L74" s="286"/>
       <c r="M74" s="287"/>
-      <c r="N74" s="357"/>
-      <c r="O74" s="355"/>
+      <c r="N74" s="317"/>
+      <c r="O74" s="315"/>
       <c r="P74" s="292"/>
       <c r="Q74" s="292">
         <f>'Stimulus Round 2'!$C$13*4/12</f>
@@ -9140,8 +9134,8 @@
       <c r="K75" s="286"/>
       <c r="L75" s="286"/>
       <c r="M75" s="287"/>
-      <c r="N75" s="357"/>
-      <c r="O75" s="355"/>
+      <c r="N75" s="317"/>
+      <c r="O75" s="315"/>
       <c r="P75" s="292"/>
       <c r="Q75" s="292">
         <f>'Stimulus Round 2'!$C$5*4/12</f>
@@ -9212,8 +9206,8 @@
       <c r="K76" s="286"/>
       <c r="L76" s="286"/>
       <c r="M76" s="287"/>
-      <c r="N76" s="357"/>
-      <c r="O76" s="355"/>
+      <c r="N76" s="317"/>
+      <c r="O76" s="315"/>
       <c r="P76" s="292"/>
       <c r="Q76" s="292">
         <f>'Stimulus Round 2'!$C$10*4/12</f>
@@ -9284,8 +9278,8 @@
       <c r="K77" s="286"/>
       <c r="L77" s="286"/>
       <c r="M77" s="287"/>
-      <c r="N77" s="357"/>
-      <c r="O77" s="355"/>
+      <c r="N77" s="317"/>
+      <c r="O77" s="315"/>
       <c r="P77" s="292"/>
       <c r="Q77" s="292">
         <f>'Stimulus Round 2'!$C$16*4/12</f>
@@ -9367,10 +9361,10 @@
         <f t="shared" ref="M78:AB78" si="45">M66+M68</f>
         <v>286980.38194444444</v>
       </c>
-      <c r="N78" s="355">
+      <c r="N78" s="315">
         <v>286950.6143673578</v>
       </c>
-      <c r="O78" s="355">
+      <c r="O78" s="315">
         <f t="shared" si="43"/>
         <v>-29.767577086633537</v>
       </c>
@@ -9444,8 +9438,8 @@
       <c r="K79" s="199"/>
       <c r="L79" s="205"/>
       <c r="M79" s="199"/>
-      <c r="N79" s="355"/>
-      <c r="O79" s="355"/>
+      <c r="N79" s="315"/>
+      <c r="O79" s="315"/>
       <c r="P79" s="135"/>
       <c r="Q79" s="135"/>
       <c r="R79" s="135"/>
@@ -9504,10 +9498,10 @@
         <f>VLOOKUP(C80,'Haver NA'!$A$1:$I$34,9,0)/1000</f>
         <v>1335.133</v>
       </c>
-      <c r="N80" s="355">
+      <c r="N80" s="315">
         <v>1335.3219999999999</v>
       </c>
-      <c r="O80" s="355">
+      <c r="O80" s="315">
         <f t="shared" si="43"/>
         <v>0.18899999999985084</v>
       </c>
@@ -9565,10 +9559,10 @@
         <f>VLOOKUP(C81,'Haver NA'!$A$1:$I$34,9,0)/1000</f>
         <v>1487.0350000000001</v>
       </c>
-      <c r="N81" s="355">
+      <c r="N81" s="315">
         <v>1486.8019999999999</v>
       </c>
-      <c r="O81" s="355">
+      <c r="O81" s="315">
         <f t="shared" si="43"/>
         <v>-0.23300000000017462</v>
       </c>
@@ -9637,10 +9631,10 @@
         <f>M81/L81-1</f>
         <v>-1.1805555555555514E-2</v>
       </c>
-      <c r="N82" s="356">
+      <c r="N82" s="316">
         <v>-1.1960393407761893E-2</v>
       </c>
-      <c r="O82" s="355">
+      <c r="O82" s="315">
         <f t="shared" si="43"/>
         <v>-1.548378522063798E-4</v>
       </c>
@@ -9719,8 +9713,8 @@
       <c r="K83" s="209"/>
       <c r="L83" s="209"/>
       <c r="M83" s="202"/>
-      <c r="N83" s="356"/>
-      <c r="O83" s="355"/>
+      <c r="N83" s="316"/>
+      <c r="O83" s="315"/>
       <c r="P83" s="188"/>
       <c r="Q83" s="102">
         <f>SUM(Q84:Q86)</f>
@@ -9769,8 +9763,8 @@
       <c r="K84" s="301"/>
       <c r="L84" s="301"/>
       <c r="M84" s="302"/>
-      <c r="N84" s="361"/>
-      <c r="O84" s="355"/>
+      <c r="N84" s="321"/>
+      <c r="O84" s="315"/>
       <c r="P84" s="303"/>
       <c r="Q84" s="292">
         <f>('Stimulus Round 2'!$C7*0.7*4)/2</f>
@@ -9819,8 +9813,8 @@
       <c r="K85" s="301"/>
       <c r="L85" s="301"/>
       <c r="M85" s="302"/>
-      <c r="N85" s="361"/>
-      <c r="O85" s="355"/>
+      <c r="N85" s="321"/>
+      <c r="O85" s="315"/>
       <c r="P85" s="303"/>
       <c r="Q85" s="292">
         <f>('Stimulus Round 2'!$C8*0.7*4)/2</f>
@@ -9869,8 +9863,8 @@
       <c r="K86" s="301"/>
       <c r="L86" s="301"/>
       <c r="M86" s="302"/>
-      <c r="N86" s="361"/>
-      <c r="O86" s="355"/>
+      <c r="N86" s="321"/>
+      <c r="O86" s="315"/>
       <c r="P86" s="303"/>
       <c r="Q86" s="292">
         <f>('Stimulus Round 2'!$C9*0.7*4)/2</f>
@@ -9943,10 +9937,10 @@
         <f>VLOOKUP(C87,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>486072</v>
       </c>
-      <c r="N87" s="355">
+      <c r="N87" s="315">
         <v>486072</v>
       </c>
-      <c r="O87" s="355"/>
+      <c r="O87" s="315"/>
       <c r="P87" s="116">
         <f t="shared" ref="P87:U87" si="51">P94*0.74</f>
         <v>515064.18485195568</v>
@@ -10061,10 +10055,10 @@
         <f t="shared" si="52"/>
         <v>2509001</v>
       </c>
-      <c r="N88" s="355">
+      <c r="N88" s="315">
         <v>2508714</v>
       </c>
-      <c r="O88" s="355">
+      <c r="O88" s="315">
         <f t="shared" si="43"/>
         <v>-287</v>
       </c>
@@ -10142,10 +10136,10 @@
         <f t="shared" si="54"/>
         <v>1328805</v>
       </c>
-      <c r="N89" s="355">
+      <c r="N89" s="315">
         <v>1328805</v>
       </c>
-      <c r="O89" s="355">
+      <c r="O89" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -10212,8 +10206,8 @@
       <c r="K90" s="199"/>
       <c r="L90" s="199"/>
       <c r="M90" s="199"/>
-      <c r="N90" s="355"/>
-      <c r="O90" s="355"/>
+      <c r="N90" s="315"/>
+      <c r="O90" s="315"/>
       <c r="AO90" s="243"/>
     </row>
     <row r="91" spans="1:41" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -10252,10 +10246,10 @@
         <f>VLOOKUP(C91,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>828480</v>
       </c>
-      <c r="N91" s="355">
+      <c r="N91" s="315">
         <v>835999</v>
       </c>
-      <c r="O91" s="355">
+      <c r="O91" s="315">
         <f t="shared" si="43"/>
         <v>7519</v>
       </c>
@@ -10333,10 +10327,10 @@
         <f>M91-M94</f>
         <v>144777</v>
       </c>
-      <c r="N92" s="355">
+      <c r="N92" s="315">
         <v>144732</v>
       </c>
-      <c r="O92" s="355">
+      <c r="O92" s="315">
         <f t="shared" si="43"/>
         <v>-45</v>
       </c>
@@ -10387,8 +10381,8 @@
       <c r="K93" s="199"/>
       <c r="L93" s="199"/>
       <c r="M93" s="199"/>
-      <c r="N93" s="355"/>
-      <c r="O93" s="355">
+      <c r="N93" s="315"/>
+      <c r="O93" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -10430,10 +10424,10 @@
         <f>VLOOKUP(C94,'Haver NA'!$A$1:$I$34,9,0)</f>
         <v>683703</v>
       </c>
-      <c r="N94" s="355">
+      <c r="N94" s="315">
         <v>691267</v>
       </c>
-      <c r="O94" s="355">
+      <c r="O94" s="315">
         <f t="shared" si="43"/>
         <v>7564</v>
       </c>
@@ -10513,8 +10507,8 @@
       <c r="K95" s="202"/>
       <c r="L95" s="202"/>
       <c r="M95" s="199"/>
-      <c r="N95" s="355"/>
-      <c r="O95" s="355">
+      <c r="N95" s="315"/>
+      <c r="O95" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -10572,8 +10566,8 @@
       </c>
       <c r="L96" s="211"/>
       <c r="M96" s="199"/>
-      <c r="N96" s="355"/>
-      <c r="O96" s="355">
+      <c r="N96" s="315"/>
+      <c r="O96" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -10621,10 +10615,10 @@
         <f>VLOOKUP(C97,'Haver NA'!$A$1:$I$34,9,0)/1000</f>
         <v>1993.0509999999999</v>
       </c>
-      <c r="N97" s="355">
+      <c r="N97" s="315">
         <v>1992.6769999999999</v>
       </c>
-      <c r="O97" s="355">
+      <c r="O97" s="315">
         <f t="shared" si="43"/>
         <v>-0.37400000000002365</v>
       </c>
@@ -10702,10 +10696,10 @@
         <f>(M97/L97)-1</f>
         <v>-9.9592668024439668E-3</v>
       </c>
-      <c r="N98" s="355">
+      <c r="N98" s="315">
         <v>-1.0145049923004357E-2</v>
       </c>
-      <c r="O98" s="355">
+      <c r="O98" s="315">
         <f t="shared" si="43"/>
         <v>-1.8578312056038992E-4</v>
       </c>
@@ -10740,8 +10734,8 @@
       <c r="K99" s="202"/>
       <c r="L99" s="202"/>
       <c r="M99" s="199"/>
-      <c r="N99" s="355"/>
-      <c r="O99" s="355">
+      <c r="N99" s="315"/>
+      <c r="O99" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -10811,10 +10805,10 @@
         <f>VLOOKUP(C100,'Haver NA'!$A$1:$I$34,9,0)/1000</f>
         <v>2329.605</v>
       </c>
-      <c r="N100" s="355">
+      <c r="N100" s="315">
         <v>2329.6770000000001</v>
       </c>
-      <c r="O100" s="355">
+      <c r="O100" s="315">
         <f t="shared" si="43"/>
         <v>7.2000000000116415E-2</v>
       </c>
@@ -10865,8 +10859,8 @@
       <c r="K101" s="199"/>
       <c r="L101" s="199"/>
       <c r="M101" s="199"/>
-      <c r="N101" s="355"/>
-      <c r="O101" s="355">
+      <c r="N101" s="315"/>
+      <c r="O101" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -10935,10 +10929,10 @@
         <f>(((M100/L100))^4)-1</f>
         <v>-8.3608921686818549E-3</v>
       </c>
-      <c r="N102" s="356">
+      <c r="N102" s="316">
         <v>-8.2382940014741335E-3</v>
       </c>
-      <c r="O102" s="355">
+      <c r="O102" s="315">
         <f t="shared" si="43"/>
         <v>1.2259816720772143E-4</v>
       </c>
@@ -10968,8 +10962,8 @@
       <c r="K103" s="202"/>
       <c r="L103" s="202"/>
       <c r="M103" s="199"/>
-      <c r="N103" s="355"/>
-      <c r="O103" s="355">
+      <c r="N103" s="315"/>
+      <c r="O103" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -11017,8 +11011,8 @@
       <c r="K104" s="202"/>
       <c r="L104" s="202"/>
       <c r="M104" s="199"/>
-      <c r="N104" s="355"/>
-      <c r="O104" s="355">
+      <c r="N104" s="315"/>
+      <c r="O104" s="315">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -11069,10 +11063,10 @@
         <f t="shared" si="66"/>
         <v>482408</v>
       </c>
-      <c r="N105" s="355">
+      <c r="N105" s="315">
         <v>489927</v>
       </c>
-      <c r="O105" s="355">
+      <c r="O105" s="315">
         <f t="shared" si="43"/>
         <v>7519</v>
       </c>
@@ -11146,10 +11140,10 @@
         <f t="shared" si="67"/>
         <v>197631</v>
       </c>
-      <c r="N106" s="355">
+      <c r="N106" s="315">
         <v>205195</v>
       </c>
-      <c r="O106" s="355">
+      <c r="O106" s="315">
         <f t="shared" si="43"/>
         <v>7564</v>
       </c>
@@ -11241,10 +11235,10 @@
         <f t="shared" si="68"/>
         <v>284777</v>
       </c>
-      <c r="N107" s="355">
+      <c r="N107" s="315">
         <v>284732</v>
       </c>
-      <c r="O107" s="355">
+      <c r="O107" s="315">
         <f t="shared" si="43"/>
         <v>-45</v>
       </c>
@@ -11306,8 +11300,14 @@
       <c r="I108" s="220"/>
       <c r="J108" s="220"/>
       <c r="K108" s="220"/>
-      <c r="L108" s="220"/>
-      <c r="M108" s="135"/>
+      <c r="L108" s="135">
+        <f>L107-L42</f>
+        <v>143335</v>
+      </c>
+      <c r="M108" s="135">
+        <f>M107-M42</f>
+        <v>144777</v>
+      </c>
       <c r="N108" s="135"/>
       <c r="O108" s="135"/>
       <c r="P108" s="94"/>
@@ -12813,50 +12813,50 @@
     <row r="3" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="330" t="s">
+      <c r="A5" s="338" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="331"/>
-      <c r="C5" s="331"/>
-      <c r="D5" s="331"/>
-      <c r="E5" s="331"/>
-      <c r="F5" s="331"/>
-      <c r="G5" s="331"/>
-      <c r="H5" s="331"/>
-      <c r="I5" s="331"/>
-      <c r="J5" s="331"/>
-      <c r="K5" s="331"/>
-      <c r="L5" s="331"/>
-      <c r="M5" s="331"/>
-      <c r="N5" s="331"/>
-      <c r="O5" s="331"/>
-      <c r="P5" s="331"/>
-      <c r="Q5" s="331"/>
-      <c r="R5" s="331"/>
-      <c r="S5" s="331"/>
+      <c r="B5" s="339"/>
+      <c r="C5" s="339"/>
+      <c r="D5" s="339"/>
+      <c r="E5" s="339"/>
+      <c r="F5" s="339"/>
+      <c r="G5" s="339"/>
+      <c r="H5" s="339"/>
+      <c r="I5" s="339"/>
+      <c r="J5" s="339"/>
+      <c r="K5" s="339"/>
+      <c r="L5" s="339"/>
+      <c r="M5" s="339"/>
+      <c r="N5" s="339"/>
+      <c r="O5" s="339"/>
+      <c r="P5" s="339"/>
+      <c r="Q5" s="339"/>
+      <c r="R5" s="339"/>
+      <c r="S5" s="339"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="332" t="s">
+      <c r="A6" s="340" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="332"/>
-      <c r="C6" s="332"/>
-      <c r="D6" s="332"/>
-      <c r="E6" s="332"/>
-      <c r="F6" s="332"/>
-      <c r="G6" s="332"/>
-      <c r="H6" s="332"/>
-      <c r="I6" s="332"/>
-      <c r="J6" s="332"/>
-      <c r="K6" s="332"/>
-      <c r="L6" s="332"/>
-      <c r="M6" s="332"/>
-      <c r="N6" s="332"/>
-      <c r="O6" s="332"/>
-      <c r="P6" s="332"/>
-      <c r="Q6" s="332"/>
-      <c r="R6" s="332"/>
-      <c r="S6" s="332"/>
+      <c r="B6" s="340"/>
+      <c r="C6" s="340"/>
+      <c r="D6" s="340"/>
+      <c r="E6" s="340"/>
+      <c r="F6" s="340"/>
+      <c r="G6" s="340"/>
+      <c r="H6" s="340"/>
+      <c r="I6" s="340"/>
+      <c r="J6" s="340"/>
+      <c r="K6" s="340"/>
+      <c r="L6" s="340"/>
+      <c r="M6" s="340"/>
+      <c r="N6" s="340"/>
+      <c r="O6" s="340"/>
+      <c r="P6" s="340"/>
+      <c r="Q6" s="340"/>
+      <c r="R6" s="340"/>
+      <c r="S6" s="340"/>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
@@ -12897,8 +12897,8 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="131"/>
-      <c r="R8" s="333"/>
-      <c r="S8" s="334"/>
+      <c r="R8" s="341"/>
+      <c r="S8" s="342"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="130"/>
@@ -13163,10 +13163,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="317" t="s">
+      <c r="A1" s="325" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="317"/>
+      <c r="B1" s="325"/>
       <c r="C1" s="35"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -13174,18 +13174,18 @@
       <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="335" t="s">
+      <c r="Z1" s="343" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" s="335"/>
-      <c r="AB1" s="335"/>
-      <c r="AC1" s="316"/>
-      <c r="AD1" s="316"/>
-      <c r="AE1" s="316"/>
-      <c r="AF1" s="316"/>
+      <c r="AA1" s="343"/>
+      <c r="AB1" s="343"/>
+      <c r="AC1" s="324"/>
+      <c r="AD1" s="324"/>
+      <c r="AE1" s="324"/>
+      <c r="AF1" s="324"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A2" s="336" t="s">
+      <c r="A2" s="344" t="s">
         <v>192</v>
       </c>
       <c r="B2" s="107"/>
@@ -13194,45 +13194,45 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A3" s="336"/>
+      <c r="A3" s="344"/>
       <c r="B3" s="108"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A4" s="336"/>
+      <c r="A4" s="344"/>
       <c r="B4" s="109"/>
       <c r="C4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A5" s="336"/>
+      <c r="A5" s="344"/>
       <c r="B5" s="98"/>
       <c r="C5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C7" s="326" t="s">
+      <c r="C7" s="334" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="327"/>
-      <c r="E7" s="327"/>
-      <c r="F7" s="328"/>
-      <c r="G7" s="326" t="s">
+      <c r="D7" s="335"/>
+      <c r="E7" s="335"/>
+      <c r="F7" s="336"/>
+      <c r="G7" s="334" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="327"/>
-      <c r="I7" s="327"/>
-      <c r="J7" s="328"/>
-      <c r="K7" s="326" t="s">
+      <c r="H7" s="335"/>
+      <c r="I7" s="335"/>
+      <c r="J7" s="336"/>
+      <c r="K7" s="334" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="327"/>
-      <c r="M7" s="327"/>
-      <c r="N7" s="328"/>
+      <c r="L7" s="335"/>
+      <c r="M7" s="335"/>
+      <c r="N7" s="336"/>
     </row>
     <row r="8" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
@@ -15096,8 +15096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DF29D8-3B4C-4287-8349-C362C52DEB32}">
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView topLeftCell="C14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView topLeftCell="H12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15113,88 +15113,88 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" s="337" t="s">
+      <c r="A2" s="350" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="337"/>
-      <c r="C2" s="337"/>
-      <c r="D2" s="337"/>
-      <c r="E2" s="337"/>
-      <c r="F2" s="337"/>
-      <c r="G2" s="337"/>
-      <c r="H2" s="337"/>
-      <c r="I2" s="337"/>
-      <c r="J2" s="337"/>
+      <c r="B2" s="350"/>
+      <c r="C2" s="350"/>
+      <c r="D2" s="350"/>
+      <c r="E2" s="350"/>
+      <c r="F2" s="350"/>
+      <c r="G2" s="350"/>
+      <c r="H2" s="350"/>
+      <c r="I2" s="350"/>
+      <c r="J2" s="350"/>
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A3" s="337" t="s">
+      <c r="A3" s="350" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="337"/>
-      <c r="C3" s="337"/>
-      <c r="D3" s="337"/>
-      <c r="E3" s="337"/>
-      <c r="F3" s="337"/>
-      <c r="G3" s="337"/>
-      <c r="H3" s="337"/>
-      <c r="I3" s="337"/>
-      <c r="J3" s="337"/>
+      <c r="B3" s="350"/>
+      <c r="C3" s="350"/>
+      <c r="D3" s="350"/>
+      <c r="E3" s="350"/>
+      <c r="F3" s="350"/>
+      <c r="G3" s="350"/>
+      <c r="H3" s="350"/>
+      <c r="I3" s="350"/>
+      <c r="J3" s="350"/>
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="338"/>
-      <c r="B4" s="338"/>
-      <c r="C4" s="338"/>
-      <c r="D4" s="338"/>
-      <c r="E4" s="338"/>
-      <c r="F4" s="338"/>
-      <c r="G4" s="338"/>
-      <c r="H4" s="338"/>
-      <c r="I4" s="338"/>
-      <c r="J4" s="338"/>
-      <c r="K4" s="343" t="s">
+      <c r="A4" s="351"/>
+      <c r="B4" s="351"/>
+      <c r="C4" s="351"/>
+      <c r="D4" s="351"/>
+      <c r="E4" s="351"/>
+      <c r="F4" s="351"/>
+      <c r="G4" s="351"/>
+      <c r="H4" s="351"/>
+      <c r="I4" s="351"/>
+      <c r="J4" s="351"/>
+      <c r="K4" s="356" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="343"/>
-      <c r="M4" s="343"/>
-      <c r="N4" s="343"/>
+      <c r="L4" s="356"/>
+      <c r="M4" s="356"/>
+      <c r="N4" s="356"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
-      <c r="C5" s="339" t="s">
+      <c r="C5" s="352" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="340"/>
-      <c r="E5" s="340"/>
-      <c r="F5" s="340"/>
-      <c r="G5" s="340"/>
-      <c r="H5" s="340"/>
-      <c r="I5" s="340"/>
-      <c r="J5" s="341"/>
+      <c r="D5" s="353"/>
+      <c r="E5" s="353"/>
+      <c r="F5" s="353"/>
+      <c r="G5" s="353"/>
+      <c r="H5" s="353"/>
+      <c r="I5" s="353"/>
+      <c r="J5" s="354"/>
       <c r="K5" s="78"/>
-      <c r="L5" s="342" t="s">
+      <c r="L5" s="355" t="s">
         <v>107</v>
       </c>
-      <c r="M5" s="316"/>
-      <c r="N5" s="316"/>
+      <c r="M5" s="324"/>
+      <c r="N5" s="324"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="345">
+      <c r="C6" s="346">
         <v>2020</v>
       </c>
-      <c r="D6" s="346"/>
-      <c r="E6" s="346"/>
-      <c r="F6" s="346"/>
-      <c r="G6" s="346"/>
-      <c r="H6" s="346"/>
-      <c r="I6" s="346"/>
-      <c r="J6" s="347"/>
+      <c r="D6" s="347"/>
+      <c r="E6" s="347"/>
+      <c r="F6" s="347"/>
+      <c r="G6" s="347"/>
+      <c r="H6" s="347"/>
+      <c r="I6" s="347"/>
+      <c r="J6" s="348"/>
       <c r="K6" s="78" t="s">
         <v>135</v>
       </c>
@@ -15631,24 +15631,24 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="K22" s="316" t="s">
+      <c r="K22" s="324" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="316"/>
-      <c r="M22" s="316"/>
-      <c r="N22" s="316"/>
-      <c r="O22" s="316" t="s">
+      <c r="L22" s="324"/>
+      <c r="M22" s="324"/>
+      <c r="N22" s="324"/>
+      <c r="O22" s="324" t="s">
         <v>10</v>
       </c>
-      <c r="P22" s="316"/>
-      <c r="Q22" s="316"/>
-      <c r="R22" s="316"/>
-      <c r="S22" s="316" t="s">
+      <c r="P22" s="324"/>
+      <c r="Q22" s="324"/>
+      <c r="R22" s="324"/>
+      <c r="S22" s="324" t="s">
         <v>11</v>
       </c>
-      <c r="T22" s="316"/>
-      <c r="U22" s="316"/>
-      <c r="V22" s="316"/>
+      <c r="T22" s="324"/>
+      <c r="U22" s="324"/>
+      <c r="V22" s="324"/>
     </row>
     <row r="23" spans="3:23" x14ac:dyDescent="0.35">
       <c r="C23" s="67"/>
@@ -15665,12 +15665,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="K23" s="348" t="s">
+      <c r="K23" s="349" t="s">
         <v>108</v>
       </c>
-      <c r="L23" s="348"/>
-      <c r="M23" s="348"/>
-      <c r="N23" s="348"/>
+      <c r="L23" s="349"/>
+      <c r="M23" s="349"/>
+      <c r="N23" s="349"/>
       <c r="O23" s="35" t="s">
         <v>146</v>
       </c>
@@ -15839,7 +15839,7 @@
       <c r="S27" s="72"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.35">
-      <c r="I28" s="344" t="s">
+      <c r="I28" s="345" t="s">
         <v>259</v>
       </c>
       <c r="J28" s="82" t="s">
@@ -15890,7 +15890,7 @@
       <c r="H29">
         <v>67</v>
       </c>
-      <c r="I29" s="344"/>
+      <c r="I29" s="345"/>
       <c r="J29" s="82" t="s">
         <v>143</v>
       </c>
@@ -15939,7 +15939,7 @@
         <f>H29</f>
         <v>67</v>
       </c>
-      <c r="I30" s="344"/>
+      <c r="I30" s="345"/>
       <c r="J30" s="82" t="s">
         <v>142</v>
       </c>
@@ -15988,7 +15988,7 @@
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="I31" s="344"/>
+      <c r="I31" s="345"/>
       <c r="J31" s="35" t="s">
         <v>140</v>
       </c>
@@ -16050,7 +16050,7 @@
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="I33" s="344" t="s">
+      <c r="I33" s="345" t="s">
         <v>141</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -16098,7 +16098,7 @@
       </c>
     </row>
     <row r="34" spans="3:23" x14ac:dyDescent="0.35">
-      <c r="I34" s="344"/>
+      <c r="I34" s="345"/>
       <c r="J34" t="s">
         <v>260</v>
       </c>
@@ -16277,6 +16277,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="K4:N4"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="I28:I31"/>
@@ -16284,12 +16290,6 @@
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K23:N23"/>
     <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -16397,30 +16397,30 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="352" t="s">
+      <c r="E6" s="358" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="352"/>
-      <c r="G6" s="352"/>
-      <c r="H6" s="352"/>
-      <c r="I6" s="352"/>
-      <c r="J6" s="352"/>
-      <c r="K6" s="352"/>
-      <c r="L6" s="352"/>
-      <c r="M6" s="352"/>
-      <c r="N6" s="352"/>
-      <c r="O6" s="352"/>
-      <c r="P6" s="352"/>
-      <c r="Q6" s="352"/>
-      <c r="R6" s="352"/>
+      <c r="F6" s="358"/>
+      <c r="G6" s="358"/>
+      <c r="H6" s="358"/>
+      <c r="I6" s="358"/>
+      <c r="J6" s="358"/>
+      <c r="K6" s="358"/>
+      <c r="L6" s="358"/>
+      <c r="M6" s="358"/>
+      <c r="N6" s="358"/>
+      <c r="O6" s="358"/>
+      <c r="P6" s="358"/>
+      <c r="Q6" s="358"/>
+      <c r="R6" s="358"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="349" t="s">
+      <c r="A7" s="357" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="349"/>
-      <c r="C7" s="349"/>
-      <c r="D7" s="349"/>
+      <c r="B7" s="357"/>
+      <c r="C7" s="357"/>
+      <c r="D7" s="357"/>
       <c r="E7" s="36"/>
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
@@ -16438,11 +16438,11 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="36"/>
-      <c r="B8" s="349" t="s">
+      <c r="B8" s="357" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="349"/>
-      <c r="D8" s="349"/>
+      <c r="C8" s="357"/>
+      <c r="D8" s="357"/>
       <c r="E8" s="42">
         <v>1717.857</v>
       </c>
@@ -16488,11 +16488,11 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="36"/>
-      <c r="B9" s="349" t="s">
+      <c r="B9" s="357" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="349"/>
-      <c r="D9" s="349"/>
+      <c r="C9" s="357"/>
+      <c r="D9" s="357"/>
       <c r="E9" s="42">
         <v>1243.3720000000001</v>
       </c>
@@ -16538,11 +16538,11 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="36"/>
-      <c r="B10" s="349" t="s">
+      <c r="B10" s="357" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="349"/>
-      <c r="D10" s="349"/>
+      <c r="C10" s="357"/>
+      <c r="D10" s="357"/>
       <c r="E10" s="42">
         <v>230.245</v>
       </c>
@@ -16588,11 +16588,11 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="36"/>
-      <c r="B11" s="349" t="s">
+      <c r="B11" s="357" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="349"/>
-      <c r="D11" s="349"/>
+      <c r="C11" s="357"/>
+      <c r="D11" s="357"/>
       <c r="E11" s="42">
         <v>271.327</v>
       </c>
@@ -16687,10 +16687,10 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="36"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="349" t="s">
+      <c r="C13" s="357" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="349"/>
+      <c r="D13" s="357"/>
       <c r="E13" s="42">
         <v>3462.8009999999999</v>
       </c>
@@ -16841,11 +16841,11 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="36"/>
-      <c r="B19" s="349" t="s">
+      <c r="B19" s="357" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="349"/>
-      <c r="D19" s="349"/>
+      <c r="C19" s="357"/>
+      <c r="D19" s="357"/>
       <c r="E19" s="42">
         <v>1717.857</v>
       </c>
@@ -16904,11 +16904,11 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="36"/>
-      <c r="B20" s="349" t="s">
+      <c r="B20" s="357" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="349"/>
-      <c r="D20" s="349"/>
+      <c r="C20" s="357"/>
+      <c r="D20" s="357"/>
       <c r="E20" s="42">
         <v>1243.3720000000001</v>
       </c>
@@ -16968,11 +16968,11 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="36"/>
-      <c r="B21" s="349" t="s">
+      <c r="B21" s="357" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="349"/>
-      <c r="D21" s="349"/>
+      <c r="C21" s="357"/>
+      <c r="D21" s="357"/>
       <c r="E21" s="42">
         <v>230.245</v>
       </c>
@@ -17031,11 +17031,11 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="36"/>
-      <c r="B22" s="349" t="s">
+      <c r="B22" s="357" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="349"/>
-      <c r="D22" s="349"/>
+      <c r="C22" s="357"/>
+      <c r="D22" s="357"/>
       <c r="E22" s="42">
         <v>271.327</v>
       </c>
@@ -17148,21 +17148,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="350" t="s">
+      <c r="H27" s="359" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="350"/>
-      <c r="J27" s="350"/>
-      <c r="K27" s="350"/>
-      <c r="L27" s="350"/>
-      <c r="M27" s="350"/>
-      <c r="N27" s="350"/>
-      <c r="O27" s="350"/>
-      <c r="P27" s="350"/>
-      <c r="Q27" s="350"/>
-      <c r="R27" s="350"/>
-      <c r="S27" s="350"/>
-      <c r="T27" s="350"/>
+      <c r="I27" s="359"/>
+      <c r="J27" s="359"/>
+      <c r="K27" s="359"/>
+      <c r="L27" s="359"/>
+      <c r="M27" s="359"/>
+      <c r="N27" s="359"/>
+      <c r="O27" s="359"/>
+      <c r="P27" s="359"/>
+      <c r="Q27" s="359"/>
+      <c r="R27" s="359"/>
+      <c r="S27" s="359"/>
+      <c r="T27" s="359"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="24" t="s">
@@ -17478,21 +17478,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="351" t="s">
+      <c r="F37" s="360" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="351"/>
-      <c r="H37" s="351"/>
-      <c r="I37" s="351"/>
-      <c r="J37" s="351"/>
-      <c r="K37" s="351"/>
-      <c r="L37" s="351"/>
-      <c r="M37" s="351"/>
-      <c r="N37" s="351"/>
-      <c r="O37" s="351"/>
-      <c r="P37" s="351"/>
-      <c r="Q37" s="351"/>
-      <c r="R37" s="351"/>
+      <c r="G37" s="360"/>
+      <c r="H37" s="360"/>
+      <c r="I37" s="360"/>
+      <c r="J37" s="360"/>
+      <c r="K37" s="360"/>
+      <c r="L37" s="360"/>
+      <c r="M37" s="360"/>
+      <c r="N37" s="360"/>
+      <c r="O37" s="360"/>
+      <c r="P37" s="360"/>
+      <c r="Q37" s="360"/>
+      <c r="R37" s="360"/>
     </row>
     <row r="38" spans="1:18" ht="17" x14ac:dyDescent="0.35">
       <c r="A38" s="24" t="s">
@@ -17808,21 +17808,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="350" t="s">
+      <c r="F48" s="359" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="350"/>
-      <c r="H48" s="350"/>
-      <c r="I48" s="350"/>
-      <c r="J48" s="350"/>
-      <c r="K48" s="350"/>
-      <c r="L48" s="350"/>
-      <c r="M48" s="350"/>
-      <c r="N48" s="350"/>
-      <c r="O48" s="350"/>
-      <c r="P48" s="350"/>
-      <c r="Q48" s="350"/>
-      <c r="R48" s="350"/>
+      <c r="G48" s="359"/>
+      <c r="H48" s="359"/>
+      <c r="I48" s="359"/>
+      <c r="J48" s="359"/>
+      <c r="K48" s="359"/>
+      <c r="L48" s="359"/>
+      <c r="M48" s="359"/>
+      <c r="N48" s="359"/>
+      <c r="O48" s="359"/>
+      <c r="P48" s="359"/>
+      <c r="Q48" s="359"/>
+      <c r="R48" s="359"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="24" t="s">
@@ -18134,12 +18134,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -18148,6 +18142,12 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18186,50 +18186,50 @@
     <row r="3" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="330" t="s">
+      <c r="A5" s="338" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="331"/>
-      <c r="C5" s="331"/>
-      <c r="D5" s="331"/>
-      <c r="E5" s="331"/>
-      <c r="F5" s="331"/>
-      <c r="G5" s="331"/>
-      <c r="H5" s="331"/>
-      <c r="I5" s="331"/>
-      <c r="J5" s="331"/>
-      <c r="K5" s="331"/>
-      <c r="L5" s="331"/>
-      <c r="M5" s="331"/>
-      <c r="N5" s="331"/>
-      <c r="O5" s="331"/>
-      <c r="P5" s="331"/>
-      <c r="Q5" s="331"/>
-      <c r="R5" s="331"/>
-      <c r="S5" s="331"/>
+      <c r="B5" s="339"/>
+      <c r="C5" s="339"/>
+      <c r="D5" s="339"/>
+      <c r="E5" s="339"/>
+      <c r="F5" s="339"/>
+      <c r="G5" s="339"/>
+      <c r="H5" s="339"/>
+      <c r="I5" s="339"/>
+      <c r="J5" s="339"/>
+      <c r="K5" s="339"/>
+      <c r="L5" s="339"/>
+      <c r="M5" s="339"/>
+      <c r="N5" s="339"/>
+      <c r="O5" s="339"/>
+      <c r="P5" s="339"/>
+      <c r="Q5" s="339"/>
+      <c r="R5" s="339"/>
+      <c r="S5" s="339"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="332" t="s">
+      <c r="A6" s="340" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="332"/>
-      <c r="C6" s="332"/>
-      <c r="D6" s="332"/>
-      <c r="E6" s="332"/>
-      <c r="F6" s="332"/>
-      <c r="G6" s="332"/>
-      <c r="H6" s="332"/>
-      <c r="I6" s="332"/>
-      <c r="J6" s="332"/>
-      <c r="K6" s="332"/>
-      <c r="L6" s="332"/>
-      <c r="M6" s="332"/>
-      <c r="N6" s="332"/>
-      <c r="O6" s="332"/>
-      <c r="P6" s="332"/>
-      <c r="Q6" s="332"/>
-      <c r="R6" s="332"/>
-      <c r="S6" s="332"/>
+      <c r="B6" s="340"/>
+      <c r="C6" s="340"/>
+      <c r="D6" s="340"/>
+      <c r="E6" s="340"/>
+      <c r="F6" s="340"/>
+      <c r="G6" s="340"/>
+      <c r="H6" s="340"/>
+      <c r="I6" s="340"/>
+      <c r="J6" s="340"/>
+      <c r="K6" s="340"/>
+      <c r="L6" s="340"/>
+      <c r="M6" s="340"/>
+      <c r="N6" s="340"/>
+      <c r="O6" s="340"/>
+      <c r="P6" s="340"/>
+      <c r="Q6" s="340"/>
+      <c r="R6" s="340"/>
+      <c r="S6" s="340"/>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
@@ -18269,10 +18269,10 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="333" t="s">
+      <c r="R8" s="341" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="334"/>
+      <c r="S8" s="342"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
@@ -21143,10 +21143,10 @@
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
-      <c r="D75" s="353" t="s">
+      <c r="D75" s="361" t="s">
         <v>42</v>
       </c>
-      <c r="E75" s="354"/>
+      <c r="E75" s="362"/>
       <c r="F75" s="25">
         <v>-75.135000000000005</v>
       </c>
@@ -22097,7 +22097,7 @@
       <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22116,23 +22116,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="321" t="s">
+      <c r="A1" s="329" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="322"/>
+      <c r="B1" s="330"/>
       <c r="C1" s="35"/>
       <c r="H1"/>
       <c r="I1" s="250"/>
-      <c r="J1" s="329" t="s">
+      <c r="J1" s="337" t="s">
         <v>282</v>
       </c>
-      <c r="V1" s="316"/>
-      <c r="W1" s="316"/>
-      <c r="X1" s="316"/>
-      <c r="Y1" s="316"/>
+      <c r="V1" s="324"/>
+      <c r="W1" s="324"/>
+      <c r="X1" s="324"/>
+      <c r="Y1" s="324"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" s="323" t="s">
+      <c r="A2" s="331" t="s">
         <v>192</v>
       </c>
       <c r="B2" s="126"/>
@@ -22140,68 +22140,68 @@
         <v>193</v>
       </c>
       <c r="I2" s="251"/>
-      <c r="J2" s="329"/>
+      <c r="J2" s="337"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="324"/>
+      <c r="A3" s="332"/>
       <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
       <c r="I3" s="251"/>
-      <c r="J3" s="329"/>
+      <c r="J3" s="337"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" s="324"/>
+      <c r="A4" s="332"/>
       <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" s="325"/>
+      <c r="A5" s="333"/>
       <c r="B5" s="129"/>
       <c r="C5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C7" s="326" t="s">
+      <c r="C7" s="334" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="327"/>
-      <c r="E7" s="327"/>
-      <c r="F7" s="328"/>
-      <c r="G7" s="326" t="s">
+      <c r="D7" s="335"/>
+      <c r="E7" s="335"/>
+      <c r="F7" s="336"/>
+      <c r="G7" s="334" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="327"/>
-      <c r="I7" s="327"/>
-      <c r="J7" s="328"/>
-      <c r="K7" s="326" t="s">
+      <c r="H7" s="335"/>
+      <c r="I7" s="335"/>
+      <c r="J7" s="336"/>
+      <c r="K7" s="334" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="327"/>
-      <c r="M7" s="327"/>
-      <c r="N7" s="327"/>
-      <c r="O7" s="326" t="s">
+      <c r="L7" s="335"/>
+      <c r="M7" s="335"/>
+      <c r="N7" s="335"/>
+      <c r="O7" s="334" t="s">
         <v>272</v>
       </c>
-      <c r="P7" s="327"/>
-      <c r="Q7" s="327"/>
-      <c r="R7" s="327"/>
-      <c r="S7" s="326" t="s">
+      <c r="P7" s="335"/>
+      <c r="Q7" s="335"/>
+      <c r="R7" s="335"/>
+      <c r="S7" s="334" t="s">
         <v>276</v>
       </c>
-      <c r="T7" s="327"/>
-      <c r="U7" s="327"/>
-      <c r="V7" s="327"/>
-      <c r="W7" s="326" t="s">
+      <c r="T7" s="335"/>
+      <c r="U7" s="335"/>
+      <c r="V7" s="335"/>
+      <c r="W7" s="334" t="s">
         <v>277</v>
       </c>
-      <c r="X7" s="327"/>
-      <c r="Y7" s="327"/>
-      <c r="Z7" s="327"/>
+      <c r="X7" s="335"/>
+      <c r="Y7" s="335"/>
+      <c r="Z7" s="335"/>
       <c r="AA7" s="231" t="s">
         <v>278</v>
       </c>
@@ -27552,36 +27552,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="D1" s="316" t="s">
+      <c r="D1" s="324" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="316"/>
-      <c r="F1" s="316"/>
-      <c r="G1" s="316"/>
-      <c r="H1" s="316" t="s">
+      <c r="E1" s="324"/>
+      <c r="F1" s="324"/>
+      <c r="G1" s="324"/>
+      <c r="H1" s="324" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="316"/>
-      <c r="J1" s="316"/>
-      <c r="K1" s="316"/>
-      <c r="L1" s="316" t="s">
+      <c r="I1" s="324"/>
+      <c r="J1" s="324"/>
+      <c r="K1" s="324"/>
+      <c r="L1" s="324" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="316"/>
-      <c r="N1" s="316"/>
-      <c r="O1" s="316"/>
-      <c r="P1" s="316" t="s">
+      <c r="M1" s="324"/>
+      <c r="N1" s="324"/>
+      <c r="O1" s="324"/>
+      <c r="P1" s="324" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="316"/>
-      <c r="R1" s="316"/>
-      <c r="S1" s="316"/>
-      <c r="T1" s="316" t="s">
+      <c r="Q1" s="324"/>
+      <c r="R1" s="324"/>
+      <c r="S1" s="324"/>
+      <c r="T1" s="324" t="s">
         <v>268</v>
       </c>
-      <c r="U1" s="316"/>
-      <c r="V1" s="316"/>
-      <c r="W1" s="316"/>
+      <c r="U1" s="324"/>
+      <c r="V1" s="324"/>
+      <c r="W1" s="324"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="D2" s="199" t="s">
@@ -27991,22 +27991,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="321" t="s">
+      <c r="A1" s="329" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="322"/>
+      <c r="B1" s="330"/>
       <c r="C1" s="35"/>
       <c r="I1" s="250"/>
-      <c r="J1" s="329" t="s">
+      <c r="J1" s="337" t="s">
         <v>282</v>
       </c>
-      <c r="V1" s="316"/>
-      <c r="W1" s="316"/>
-      <c r="X1" s="316"/>
-      <c r="Y1" s="316"/>
+      <c r="V1" s="324"/>
+      <c r="W1" s="324"/>
+      <c r="X1" s="324"/>
+      <c r="Y1" s="324"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" s="323" t="s">
+      <c r="A2" s="331" t="s">
         <v>192</v>
       </c>
       <c r="B2" s="126"/>
@@ -28015,20 +28015,20 @@
       </c>
       <c r="H2" s="95"/>
       <c r="I2" s="251"/>
-      <c r="J2" s="329"/>
+      <c r="J2" s="337"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="324"/>
+      <c r="A3" s="332"/>
       <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
       <c r="H3" s="95"/>
       <c r="I3" s="251"/>
-      <c r="J3" s="329"/>
+      <c r="J3" s="337"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" s="324"/>
+      <c r="A4" s="332"/>
       <c r="B4" s="128"/>
       <c r="C4" t="s">
         <v>195</v>
@@ -28038,7 +28038,7 @@
       <c r="J4" s="95"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" s="325"/>
+      <c r="A5" s="333"/>
       <c r="B5" s="129"/>
       <c r="C5" t="s">
         <v>182</v>
@@ -28053,42 +28053,42 @@
       <c r="J6" s="95"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C7" s="326" t="s">
+      <c r="C7" s="334" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="327"/>
-      <c r="E7" s="327"/>
-      <c r="F7" s="328"/>
-      <c r="G7" s="326" t="s">
+      <c r="D7" s="335"/>
+      <c r="E7" s="335"/>
+      <c r="F7" s="336"/>
+      <c r="G7" s="334" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="327"/>
-      <c r="I7" s="327"/>
-      <c r="J7" s="328"/>
-      <c r="K7" s="326" t="s">
+      <c r="H7" s="335"/>
+      <c r="I7" s="335"/>
+      <c r="J7" s="336"/>
+      <c r="K7" s="334" t="s">
         <v>177</v>
       </c>
-      <c r="L7" s="327"/>
-      <c r="M7" s="327"/>
-      <c r="N7" s="327"/>
-      <c r="O7" s="326" t="s">
+      <c r="L7" s="335"/>
+      <c r="M7" s="335"/>
+      <c r="N7" s="335"/>
+      <c r="O7" s="334" t="s">
         <v>272</v>
       </c>
-      <c r="P7" s="327"/>
-      <c r="Q7" s="327"/>
-      <c r="R7" s="327"/>
-      <c r="S7" s="326" t="s">
+      <c r="P7" s="335"/>
+      <c r="Q7" s="335"/>
+      <c r="R7" s="335"/>
+      <c r="S7" s="334" t="s">
         <v>276</v>
       </c>
-      <c r="T7" s="327"/>
-      <c r="U7" s="327"/>
-      <c r="V7" s="327"/>
-      <c r="W7" s="326" t="s">
+      <c r="T7" s="335"/>
+      <c r="U7" s="335"/>
+      <c r="V7" s="335"/>
+      <c r="W7" s="334" t="s">
         <v>277</v>
       </c>
-      <c r="X7" s="327"/>
-      <c r="Y7" s="327"/>
-      <c r="Z7" s="327"/>
+      <c r="X7" s="335"/>
+      <c r="Y7" s="335"/>
+      <c r="Z7" s="335"/>
       <c r="AA7" s="231" t="s">
         <v>278</v>
       </c>
@@ -32535,6 +32535,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA9F3DB0CD4D844B918872BCED9B9CF9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61f75d9b13a46a58fd2456a565edcb9c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cac5d118-ba7b-4807-b700-df6f95cfff50" xmlns:ns3="66951ee6-cd93-49c7-9437-e871b2a117d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86870d415110e2c98f3a885b29630d1" ns2:_="" ns3:_="">
     <xsd:import namespace="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
@@ -32751,15 +32760,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
   <ds:schemaRefs>
@@ -32778,6 +32778,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B484070-5C48-4F32-AF92-870650EA512F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32794,12 +32802,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update projections script to read in round 2 ui override
</commit_message>
<xml_diff>
--- a/documentation/COVID-19 Changes/September/LSFIM_KY_v6_round2.xlsx
+++ b/documentation/COVID-19 Changes/September/LSFIM_KY_v6_round2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/GitHub/Fiscal-Impact-Measure/documentation/COVID-19 Changes/September/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F2BA2D-1D2D-6944-A22F-4F0B4225059D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AEAA82-3902-2C48-A90E-0C594C3A2116}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18900" activeTab="2" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" activeTab="3" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -3553,6 +3553,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3574,29 +3589,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -14531,68 +14531,68 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="336" t="s">
+      <c r="A2" s="341" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="336"/>
-      <c r="C2" s="336"/>
-      <c r="D2" s="336"/>
-      <c r="E2" s="336"/>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="336"/>
-      <c r="I2" s="336"/>
-      <c r="J2" s="336"/>
+      <c r="B2" s="341"/>
+      <c r="C2" s="341"/>
+      <c r="D2" s="341"/>
+      <c r="E2" s="341"/>
+      <c r="F2" s="341"/>
+      <c r="G2" s="341"/>
+      <c r="H2" s="341"/>
+      <c r="I2" s="341"/>
+      <c r="J2" s="341"/>
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="336" t="s">
+      <c r="A3" s="341" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="336"/>
-      <c r="C3" s="336"/>
-      <c r="D3" s="336"/>
-      <c r="E3" s="336"/>
-      <c r="F3" s="336"/>
-      <c r="G3" s="336"/>
-      <c r="H3" s="336"/>
-      <c r="I3" s="336"/>
-      <c r="J3" s="336"/>
+      <c r="B3" s="341"/>
+      <c r="C3" s="341"/>
+      <c r="D3" s="341"/>
+      <c r="E3" s="341"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="341"/>
+      <c r="H3" s="341"/>
+      <c r="I3" s="341"/>
+      <c r="J3" s="341"/>
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="337"/>
-      <c r="B4" s="337"/>
-      <c r="C4" s="337"/>
-      <c r="D4" s="337"/>
-      <c r="E4" s="337"/>
-      <c r="F4" s="337"/>
-      <c r="G4" s="337"/>
-      <c r="H4" s="337"/>
-      <c r="I4" s="337"/>
-      <c r="J4" s="337"/>
-      <c r="K4" s="342" t="s">
+      <c r="A4" s="342"/>
+      <c r="B4" s="342"/>
+      <c r="C4" s="342"/>
+      <c r="D4" s="342"/>
+      <c r="E4" s="342"/>
+      <c r="F4" s="342"/>
+      <c r="G4" s="342"/>
+      <c r="H4" s="342"/>
+      <c r="I4" s="342"/>
+      <c r="J4" s="342"/>
+      <c r="K4" s="347" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="342"/>
-      <c r="M4" s="342"/>
-      <c r="N4" s="342"/>
+      <c r="L4" s="347"/>
+      <c r="M4" s="347"/>
+      <c r="N4" s="347"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
-      <c r="C5" s="338" t="s">
+      <c r="C5" s="343" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="339"/>
-      <c r="E5" s="339"/>
-      <c r="F5" s="339"/>
-      <c r="G5" s="339"/>
-      <c r="H5" s="339"/>
-      <c r="I5" s="339"/>
-      <c r="J5" s="340"/>
+      <c r="D5" s="344"/>
+      <c r="E5" s="344"/>
+      <c r="F5" s="344"/>
+      <c r="G5" s="344"/>
+      <c r="H5" s="344"/>
+      <c r="I5" s="344"/>
+      <c r="J5" s="345"/>
       <c r="K5" s="78"/>
-      <c r="L5" s="341" t="s">
+      <c r="L5" s="346" t="s">
         <v>107</v>
       </c>
       <c r="M5" s="315"/>
@@ -14603,16 +14603,16 @@
         <v>109</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="344">
+      <c r="C6" s="337">
         <v>2020</v>
       </c>
-      <c r="D6" s="345"/>
-      <c r="E6" s="345"/>
-      <c r="F6" s="345"/>
-      <c r="G6" s="345"/>
-      <c r="H6" s="345"/>
-      <c r="I6" s="345"/>
-      <c r="J6" s="346"/>
+      <c r="D6" s="338"/>
+      <c r="E6" s="338"/>
+      <c r="F6" s="338"/>
+      <c r="G6" s="338"/>
+      <c r="H6" s="338"/>
+      <c r="I6" s="338"/>
+      <c r="J6" s="339"/>
       <c r="K6" s="78" t="s">
         <v>135</v>
       </c>
@@ -15084,12 +15084,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="K23" s="347" t="s">
+      <c r="K23" s="340" t="s">
         <v>108</v>
       </c>
-      <c r="L23" s="347"/>
-      <c r="M23" s="347"/>
-      <c r="N23" s="347"/>
+      <c r="L23" s="340"/>
+      <c r="M23" s="340"/>
+      <c r="N23" s="340"/>
       <c r="O23" s="35" t="s">
         <v>146</v>
       </c>
@@ -15258,7 +15258,7 @@
       <c r="S27" s="72"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I28" s="343" t="s">
+      <c r="I28" s="336" t="s">
         <v>259</v>
       </c>
       <c r="J28" s="82" t="s">
@@ -15308,7 +15308,7 @@
       <c r="H29">
         <v>67</v>
       </c>
-      <c r="I29" s="343"/>
+      <c r="I29" s="336"/>
       <c r="J29" s="82" t="s">
         <v>143</v>
       </c>
@@ -15356,7 +15356,7 @@
         <f>H29</f>
         <v>67</v>
       </c>
-      <c r="I30" s="343"/>
+      <c r="I30" s="336"/>
       <c r="J30" s="82" t="s">
         <v>142</v>
       </c>
@@ -15404,7 +15404,7 @@
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="I31" s="343"/>
+      <c r="I31" s="336"/>
       <c r="J31" s="35" t="s">
         <v>140</v>
       </c>
@@ -15466,7 +15466,7 @@
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="I33" s="343" t="s">
+      <c r="I33" s="336" t="s">
         <v>141</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -15514,7 +15514,7 @@
       </c>
     </row>
     <row r="34" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I34" s="343"/>
+      <c r="I34" s="336"/>
       <c r="J34" t="s">
         <v>260</v>
       </c>
@@ -15682,6 +15682,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="K4:N4"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="I28:I31"/>
@@ -15689,12 +15695,6 @@
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K23:N23"/>
     <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15801,22 +15801,22 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="351" t="s">
+      <c r="E6" s="349" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="351"/>
-      <c r="G6" s="351"/>
-      <c r="H6" s="351"/>
-      <c r="I6" s="351"/>
-      <c r="J6" s="351"/>
-      <c r="K6" s="351"/>
-      <c r="L6" s="351"/>
-      <c r="M6" s="351"/>
-      <c r="N6" s="351"/>
-      <c r="O6" s="351"/>
-      <c r="P6" s="351"/>
-      <c r="Q6" s="351"/>
-      <c r="R6" s="351"/>
+      <c r="F6" s="349"/>
+      <c r="G6" s="349"/>
+      <c r="H6" s="349"/>
+      <c r="I6" s="349"/>
+      <c r="J6" s="349"/>
+      <c r="K6" s="349"/>
+      <c r="L6" s="349"/>
+      <c r="M6" s="349"/>
+      <c r="N6" s="349"/>
+      <c r="O6" s="349"/>
+      <c r="P6" s="349"/>
+      <c r="Q6" s="349"/>
+      <c r="R6" s="349"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="348" t="s">
@@ -16552,21 +16552,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="349" t="s">
+      <c r="H27" s="350" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="349"/>
-      <c r="J27" s="349"/>
-      <c r="K27" s="349"/>
-      <c r="L27" s="349"/>
-      <c r="M27" s="349"/>
-      <c r="N27" s="349"/>
-      <c r="O27" s="349"/>
-      <c r="P27" s="349"/>
-      <c r="Q27" s="349"/>
-      <c r="R27" s="349"/>
-      <c r="S27" s="349"/>
-      <c r="T27" s="349"/>
+      <c r="I27" s="350"/>
+      <c r="J27" s="350"/>
+      <c r="K27" s="350"/>
+      <c r="L27" s="350"/>
+      <c r="M27" s="350"/>
+      <c r="N27" s="350"/>
+      <c r="O27" s="350"/>
+      <c r="P27" s="350"/>
+      <c r="Q27" s="350"/>
+      <c r="R27" s="350"/>
+      <c r="S27" s="350"/>
+      <c r="T27" s="350"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
@@ -16882,21 +16882,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="350" t="s">
+      <c r="F37" s="351" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="350"/>
-      <c r="H37" s="350"/>
-      <c r="I37" s="350"/>
-      <c r="J37" s="350"/>
-      <c r="K37" s="350"/>
-      <c r="L37" s="350"/>
-      <c r="M37" s="350"/>
-      <c r="N37" s="350"/>
-      <c r="O37" s="350"/>
-      <c r="P37" s="350"/>
-      <c r="Q37" s="350"/>
-      <c r="R37" s="350"/>
+      <c r="G37" s="351"/>
+      <c r="H37" s="351"/>
+      <c r="I37" s="351"/>
+      <c r="J37" s="351"/>
+      <c r="K37" s="351"/>
+      <c r="L37" s="351"/>
+      <c r="M37" s="351"/>
+      <c r="N37" s="351"/>
+      <c r="O37" s="351"/>
+      <c r="P37" s="351"/>
+      <c r="Q37" s="351"/>
+      <c r="R37" s="351"/>
     </row>
     <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
@@ -17212,21 +17212,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="349" t="s">
+      <c r="F48" s="350" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="349"/>
-      <c r="H48" s="349"/>
-      <c r="I48" s="349"/>
-      <c r="J48" s="349"/>
-      <c r="K48" s="349"/>
-      <c r="L48" s="349"/>
-      <c r="M48" s="349"/>
-      <c r="N48" s="349"/>
-      <c r="O48" s="349"/>
-      <c r="P48" s="349"/>
-      <c r="Q48" s="349"/>
-      <c r="R48" s="349"/>
+      <c r="G48" s="350"/>
+      <c r="H48" s="350"/>
+      <c r="I48" s="350"/>
+      <c r="J48" s="350"/>
+      <c r="K48" s="350"/>
+      <c r="L48" s="350"/>
+      <c r="M48" s="350"/>
+      <c r="N48" s="350"/>
+      <c r="O48" s="350"/>
+      <c r="P48" s="350"/>
+      <c r="Q48" s="350"/>
+      <c r="R48" s="350"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
@@ -17538,12 +17538,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -17552,6 +17546,12 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21497,7 +21497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F6A688-71E8-4308-9AE6-7C668128D989}">
   <dimension ref="A1:AF76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="8" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
@@ -25773,9 +25773,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304CD302-ECA7-4CE9-B89D-A357A53FDBE8}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31933,18 +31933,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -32165,14 +32165,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -32185,6 +32177,14 @@
     <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>